<commit_message>
Updates: add a few new columns and merged NHDMetadata into Sites
* Added SiteNativeURL to the sites table
* Added DataMappingURL to the organization table
* Added WaterAllcationNativeURL int othe AllocationAmounts table
* updated Longitude and Latitude to include _y and _x to be more intitive and map it to how the states report it as UTM_x or UTM_y

* Merged the NHDMetadata into the sites table: makes it easier to load and query data. NHDMetadtaa is site specific and sharing it among sites has some potential value but I think the cost is higher for now.
</commit_message>
<xml_diff>
--- a/Design_docs/SampleInputData/WKT_UpperColorado.xlsx
+++ b/Design_docs/SampleInputData/WKT_UpperColorado.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adel\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adel\Documents\GitHub\WaDE2.0\Design_docs\SampleInputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34DE7D0B-C017-4BD6-BD95-17F0A08BCA0B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CFC9F2B-3CC0-43F6-9B73-84BBB15DD2E1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{BF748AA9-CDE3-41BC-9A88-E7304A5A9EC1}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{BF748AA9-CDE3-41BC-9A88-E7304A5A9EC1}"/>
   </bookViews>
   <sheets>
     <sheet name="HUC" sheetId="1" r:id="rId1"/>
     <sheet name="County" sheetId="2" r:id="rId2"/>
-    <sheet name="Custom" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId3"/>
+    <sheet name="Custom" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2588" uniqueCount="1063">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2171" uniqueCount="1148">
   <si>
     <t>wkt_geom</t>
   </si>
@@ -3222,6 +3223,261 @@
   </si>
   <si>
     <t>Wyoming</t>
+  </si>
+  <si>
+    <t>GEOID</t>
+  </si>
+  <si>
+    <t>NAME</t>
+  </si>
+  <si>
+    <t>State_RU</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((-114.05048499999999478 38.49995499999999993, -114.05015385887999457 38.57297445830089799, -112.51539400000000057 38.57284500000000094, -112.51842100000000357 38.56770199999999704, -112.51580300000000534 38.53061699999999945, -112.52253899999999476 38.52134399999999914, -112.51433900000000676 38.50253000000000014, -112.51882200000000012 38.50002899999999784, -112.51010700000000497 38.48877499999999685, -112.51914200000000221 38.47870899999999494, -112.51340700000000083 38.47583199999999692, -112.50991999999999393 38.46773499999999757, -112.50114200000000153 38.46536100000000147, -112.4933809999999994 38.45162499999999994, -112.47922900000000368 38.44804899999999748, -112.45301100000000361 38.42923199999999895, -112.44443300000000363 38.40604799999999841, -112.4336449999999985 38.40198099999999926, -112.4209419999999966 38.41121899999999556, -112.41678699999999935 38.41956899999999564, -112.40303400000000522 38.41560099999999522, -112.39765599999999779 38.40487600000000157, -112.40386300000000119 38.40045299999999884, -112.40379500000000235 38.39475699999999847, -112.39807000000000414 38.38654100000000113, -112.39158899999999619 38.38069199999999626, -112.37435999999999581 38.37727299999999531, -112.36263700000000654 38.35681399999999996, -112.34348500000000115 38.34726699999999511, -112.33544200000000046 38.33303799999999484, -112.34082100000000537 38.3255229999999969, -112.33874099999999885 38.31240000000000379, -112.34847600000000511 38.30514199999999647, -112.34708899999999687 38.29100000000000392, -112.35069799999999418 38.28179799999999489, -112.38083299999999554 38.25061699999999831, -112.37115299999999252 38.23451000000000022, -112.35720499999999333 38.22505100000000056, -112.36493000000000109 38.21512099999999634, -112.39505400000000179 38.20598400000000083, -112.41052700000000186 38.1885690000000011, -112.42274100000000203 38.18319899999999478, -112.42245400000000188 38.17082399999999609, -112.43491000000000213 38.16359399999999624, -112.43289699999999698 38.15404799999999597, -112.44421400000000233 38.15000099999999605, -112.47867999999999711 38.1474189999999993, -114.04990337565800473 38.14876302667059349, -114.05048499999999478 38.49995499999999993)))</t>
+  </si>
+  <si>
+    <t>46-49001</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((-114.04255299999999806 41.21092300000000108, -114.04172300000000462 41.99371999999999616, -113.89326099999999542 41.98805699999999774, -112.70937499999999432 42.00030900000000145, -112.19297600000000159 42.00116699999999526, -112.16472371106800665 41.99669656113780292, -112.15384099999999989 41.98501199999999756, -112.15087699999999415 41.97056399999999599, -112.13417900000000316 41.95898100000000142, -112.12192400000000703 41.92817099999999897, -112.11486700000000383 41.91946499999999531, -112.10515399999999886 41.91086299999999909, -112.08549399999999707 41.90331099999999509, -112.06369700000000478 41.8750609999999952, -112.06398199999999576 41.86795199999999539, -112.0528630000000021 41.86623099999999909, -112.04615400000000136 41.84203600000000023, -112.02835500000000479 41.81973099999999732, -112.02971800000000258 41.80850000000000222, -112.01818799999999499 41.80456799999999618, -112.00862599999999247 41.79463700000000159, -112.01457299999999861 41.78065999999999747, -112.02637099999999748 41.77641200000000055, -112.03278000000000247 41.76794299999999538, -112.03386899999999571 41.74965299999999502, -112.04397500000000321 41.73525399999999763, -112.04274200000000405 41.71070799999999679, -112.05031700000000683 41.70603599999999744, -112.05186199999999985 41.70016299999999632, -112.04507200000000466 41.68684999999999974, -112.03090399999999249 41.68183899999999653, -112.02751700000000312 41.67175900000000155, -112.01587399999999661 41.65827499999999617, -112.01319700000000523 41.63606999999999658, -112.00463799999999992 41.62962399999999974, -112.00770699999999636 41.62352200000000124, -112.00368600000000185 41.60953399999999647, -112.00772100000000364 41.59976999999999947, -111.99410699999999963 41.56612499999999955, -111.99660599999999988 41.5575720000000004, -111.98183299999999463 41.53410199999999719, -111.97255300000000489 41.54356899999999797, -111.96195500000000322 41.54360099999999534, -111.94608900000000062 41.55302899999999511, -111.93672399999999811 41.55070899999999767, -111.928323000000006 41.53793699999999944, -111.91635200000000339 41.53840599999999483, -111.91190000000000282 41.51851800000000026, -111.90581699999999898 41.51497299999999768, -111.90911699999999485 41.50709699999999458, -111.90516900000000078 41.49684999999999491, -111.88415600000000438 41.49602300000000099, -111.87331399999999348 41.48574299999999937, -111.87778199999999629 41.4822810000000004, -111.87833700000000192 41.47422799999999654, -111.89622099999999705 41.46951999999999572, -111.90638699999999517 41.4720659999999981, -111.91680099999999243 41.46445800000000048, -111.9165880000000044 41.46037499999999909, -111.90010900000000049 41.45369099999999918, -111.89745700000000284 41.44541999999999859, -111.88156399999999735 41.4411879999999968, -111.88367999999999824 41.42791299999999666, -111.89301199999999881 41.41809500000000099, -111.90107299999999668 41.41948199999999503, -111.90549699999999689 41.41491699999999554, -111.92717199999999877 41.41277600000000092, -111.9381089999999972 41.41579000000000121, -111.95828600000000108 41.4338729999999984, -111.97236499999999637 41.42008999999999475, -111.96775700000000597 41.40993900000000139, -111.96750199999999609 41.39513600000000082, -111.97575899999999649 41.38415799999999933, -111.97446499999999503 41.37663200000000074, -111.96342199999999423 41.36512099999999492, -112.00315799999999911 41.34946000000000055, -112.00873500000000149 41.3437279999999987, -112.02030100000000346 41.34422500000000156, -112.02867200000000025 41.33651199999999903, -112.23806500000000597 41.33655199999999752, -112.49351500000000215 41.07688799999999674, -112.79935899999999549 40.99993899999999769, -114.0421451331390017 40.99989652456839906, -114.04255299999999806 41.21092300000000108)))</t>
+  </si>
+  <si>
+    <t>Box Elder</t>
+  </si>
+  <si>
+    <t>46-49003</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((-110.90434700000000134 40.70149899999999832, -110.89776999999999418 40.71335799999999949, -110.88560000000001082 40.71529299999999552, -110.89445499999999356 40.72356699999999563, -110.89198000000000377 40.72712299999999885, -110.87525899999999979 40.72832299999999606, -110.86141800000000046 40.72154599999999647, -110.84747699999999782 40.72526699999999522, -110.82340600000000563 40.71047599999999989, -110.80671200000000454 40.71157099999999929, -110.7937430000000063 40.71901700000000091, -110.78321699999999339 40.73096299999999559, -110.77461499999999717 40.73135899999999765, -110.76521999999999935 40.7370340000000013, -110.76634900000000528 40.74138699999999602, -110.75073299999999676 40.74770600000000087, -110.72183900000000278 40.74547899999999601, -110.71318499999999574 40.75288400000000166, -110.69052800000000047 40.74151599999999718, -110.65674300000000585 40.7402709999999999, -110.64651100000000383 40.75344199999999972, -110.62573700000000088 40.7694709999999958, -110.60702200000000062 40.75726499999999675, -110.58317599999999459 40.76271699999999498, -110.57664300000000424 40.75730599999999981, -110.56848899999999958 40.75699499999999631, -110.55267499999999359 40.7645209999999949, -110.54703100000000404 40.773733, -110.53351599999999166 40.77108099999999524, -110.5239389999999986 40.76152799999999843, -110.49780799999999203 40.76864700000000141, -110.48724699999999643 40.78016299999999461, -110.47261600000000215 40.771844999999999, -110.46178299999999695 40.77582199999999801, -110.457421999999994 40.78306699999999552, -110.43278200000000311 40.77827800000000025, -110.42455800000000465 40.79194799999999788, -110.4111910000000023 40.78436999999999557, -110.3959689999999938 40.78869799999999657, -110.37436700000000656 40.78808300000000031, -110.35244400000000553 40.80296099999999626, -110.3489450000000005 40.80868199999999746, -110.351302000000004 40.81548599999999993, -110.34273500000000467 40.82335599999999687, -110.32032100000000696 40.82050999999999874, -110.30142299999999977 40.82638800000000145, -110.29304700000000139 40.833399, -110.28587500000000432 40.82813099999999906, -110.26156600000000196 40.8348049999999958, -110.23820499999999356 40.82818999999999932, -110.22938700000000267 40.83080700000000007, -110.22578400000000443 40.82646299999999684, -110.21416899999999828 40.8273889999999966, -110.2026610000000062 40.82180199999999815, -110.18780900000000145 40.82613899999999774, -110.17589999999999861 40.81769899999999751, -110.1587949999999978 40.82101600000000019, -110.13950099999999566 40.8109929999999963, -110.12651400000000024 40.81493499999999841, -110.10285899999999515 40.80791699999999622, -110.06440999999999519 40.81421399999999977, -110.05135699999999588 40.81255000000000166, -110.0429239999999993 40.82060099999999636, -110.02330499999999347 40.82004799999999989, -110.01334400000000358 40.8137439999999998, -109.99366700000000208 40.81520000000000437, -109.9878620000000069 40.80761799999999795, -109.97640200000000732 40.80968599999999924, -109.97681400000000451 39.80622999999999934, -110.51819799999999816 39.80671900000000107, -110.51819500000000573 39.81164100000000161, -110.85778000000000532 39.81328500000000048, -110.85764700000000005 39.89970699999999937, -110.89165500000000009 39.89965399999999818, -110.89178900000000283 40.08240099999999728, -110.89627000000000123 40.08238399999999757, -110.89659199999999828 40.43118299999999721, -110.90292800000000284 40.43121099999999757, -110.90197399999999561 40.67816200000000038, -110.89376799999999434 40.67974799999999647, -110.90434700000000134 40.70149899999999832)))</t>
+  </si>
+  <si>
+    <t>Duchesne</t>
+  </si>
+  <si>
+    <t>46-49013</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((-111.30701100000000281 38.67233099999999979, -111.29913799999999924 38.67232899999999773, -111.29843200000000536 38.75180399999999992, -111.3009050000000002 39.46723699999999724, -111.24774800000000141 39.46719900000000081, -111.24739099999999326 39.70434999999999803, -111.23739600000000394 39.70314099999999513, -111.23006399999999871 39.69951400000000064, -111.22921200000000397 39.69330699999999723, -111.22215500000000077 39.69250499999999704, -111.22163999999999362 39.67532899999999785, -111.20131100000000401 39.65712099999999651, -111.20198200000000099 39.64555000000000007, -111.19269300000000555 39.64132199999999528, -111.18623900000000049 39.61949500000000057, -111.17608799999999292 39.61432999999999538, -111.17049199999999587 39.6033869999999979, -111.15705699999999467 39.59601299999999924, -111.14823499999999967 39.6003029999999967, -111.14876300000000242 39.60624699999999621, -111.14075499999999863 39.60834599999999739, -111.13774399999999787 39.61521700000000124, -111.13224800000000414 39.61387599999999765, -111.12029900000000282 39.57244000000000028, -111.11355199999999854 39.56877499999999515, -111.11875200000000063 39.56274700000000166, -111.1144390000000044 39.55623200000000139, -111.11633499999999231 39.5518819999999991, -111.10649200000000292 39.54652199999999596, -111.10743800000000192 39.53806399999999854, -111.09820799999999963 39.53601799999999855, -111.08553000000000566 39.52184599999999648, -111.08489000000000146 39.50794700000000148, -111.08069299999999657 39.49613899999999944, -111.07468900000000644 39.49114099999999894, -111.07535099999999773 39.47925999999999647, -111.08167500000000416 39.47356500000000068, -111.08133300000000077 39.46745500000000106, -110.02411800000000142 39.46926899999999705, -110.02353100000000552 39.46070100000000025, -110.01555799999999863 39.45533199999999852, -110.02297799999999484 39.44629700000000128, -110.02073799999999437 39.42850299999999919, -110.02343399999999463 39.42309399999999897, -110.01220700000000363 39.4185809999999961, -110.01013299999999617 39.40981599999999929, -110.01974500000000035 39.3954609999999974, -110.01911400000000185 39.3789159999999967, -110.02569400000000144 39.37640799999999786, -110.01982300000000237 39.36257899999999665, -110.0238820000000004 39.35804499999999706, -110.02216599999999858 39.35201800000000105, -110.03407400000000393 39.34896799999999928, -110.03502399999999284 39.34070200000000028, -110.04786099999999749 39.32588799999999907, -110.05570000000000164 39.33075499999999636, -110.05916999999999462 39.3289660000000012, -110.0556710000000038 39.31920099999999962, -110.06193199999999877 39.31008299999999878, -110.05294499999999402 39.30763799999999719, -110.0492449999999991 39.30150799999999833, -110.07046300000000372 39.29133499999999657, -110.07748999999999739 39.27718899999999991, -110.07429399999999475 39.27114199999999755, -110.06088400000000149 39.26444099999999793, -110.06357199999999352 39.24996600000000058, -110.05388899999999808 39.22924799999999834, -110.06243999999999517 39.22323799999999494, -110.07029199999999491 39.22848899999999617, -110.07783399999999574 39.22618999999999545, -110.07323300000000188 39.20131099999999691, -110.07883499999999799 39.19353299999999507, -110.0908019999999965 39.19321499999999503, -110.10501999999999612 39.18148800000000165, -110.09878399999999488 39.16771500000000117, -110.11226100000000372 39.16050099999999645, -110.11614799999999548 39.15256399999999815, -110.09941100000000347 39.13627599999999518, -110.11245700000000625 39.12943399999999627, -110.11479599999999834 39.12086899999999901, -110.10933199999999488 39.11297700000000077, -110.11807299999999543 39.10201699999999647, -110.11771500000000401 39.09643399999999502, -110.14229600000000175 39.08756999999999948, -110.14048999999999978 39.08110699999999582, -110.14612200000000541 39.07598099999999874, -110.14010600000000295 39.07096200000000152, -110.13986900000000446 39.05764999999999532, -110.1497410000000059 39.03996099999999814, -110.15692199999999445 39.03464100000000059, -110.13983100000000093 39.02352700000000141, -110.15332800000000191 39.01670399999999717, -110.15026500000000453 39.01068699999999723, -110.13796600000000581 39.00538499999999686, -110.14284700000000328 39.00095100000000059, -110.15025199999999472 39.00214899999999574, -110.15017799999999681 38.99723699999999837, -110.13394300000000214 38.99437799999999754, -110.13389899999999955 39.00173600000000107, -110.09632000000000573 39.00167599999999624, -110.09633599999999376 38.98625699999999483, -110.05980700000000638 38.98624799999999624, -110.05981099999999628 38.99354399999999998, -110.04117600000000721 38.99351599999999962, -110.04118400000000122 38.97897499999999837, -110.02255900000000111 38.97897100000000137, -110.02258700000000147 38.96445099999999684, -110.0039769999999919 38.96444599999999525, -110.00398400000000265 38.94991100000000017, -110.04119799999999429 38.94993199999999689, -110.04119900000000598 38.95719199999999915, -110.05051000000000272 38.95718799999999504, -110.05050500000000113 38.96445200000000142, -110.06913400000000536 38.96444799999999731, -110.06911399999999901 38.97898299999999949, -110.10568800000000067 38.97979600000000033, -110.10569999999999879 38.9833849999999984, -110.15035299999999552 38.9797930000000008, -110.14929200000000264 38.97189600000000098, -110.1378389999999996 38.96019299999999674, -110.14987700000000359 38.95510799999999563, -110.15264200000000017 38.94969599999999588, -110.1415619999999933 38.94515200000000021, -110.13468000000000302 38.92796699999999532, -110.14045099999999877 38.92432199999999654, -110.17446900000000198 38.92605700000000013, -110.1792520000000053 38.90724799999999561, -110.16510099999999284 38.8989869999999982, -110.15984299999999507 38.89115599999999517, -110.16252900000000636 38.86392199999999519, -110.1578010000000063 38.86193899999999957, -110.14272699999999361 38.86937299999999595, -110.1381149999999991 38.86786099999999777, -110.13594399999999496 38.86074399999999684, -110.14600400000000491 38.84299399999999736, -110.14394799999999464 38.839027999999999, -110.12075000000000102 38.83151399999999853, -110.12372799999999984 38.82051799999999986, -110.11368600000000129 38.81881500000000074, -110.10612600000000327 38.81065399999999954, -110.1064970000000045 38.79941900000000032, -110.11860099999999818 38.79570400000000063, -110.12129799999999591 38.79113100000000003, -110.10739800000000344 38.7773249999999976, -110.09054399999999418 38.77063299999999657, -110.08193900000000554 38.75666599999999562, -110.08386099999999885 38.75195199999999573, -110.1008199999999988 38.74819199999999597, -110.11341600000000085 38.72993699999999961, -110.10626700000000255 38.71610400000000141, -110.12306300000000192 38.7081099999999978, -110.11793600000000026 38.70557699999999812, -110.10225300000000459 38.71343799999999646, -110.08753500000000258 38.71299700000000144, -110.08670299999999997 38.70576799999999906, -110.10043400000000702 38.69265899999999903, -110.08691799999999716 38.67907799999999696, -110.09482599999999763 38.66676199999999852, -110.08871600000000512 38.66503199999999651, -110.07859000000000549 38.67191599999999596, -110.07051900000000444 38.6721769999999978, -110.06856899999999655 38.6673979999999986, -110.07419799999999555 38.65937900000000127, -110.06839300000000037 38.65643899999999888, -110.05725800000000447 38.66154999999999831, -110.05948100000000522 38.64985799999999472, -110.05616000000000554 38.64618499999999557, -110.0491439999999983 38.64774399999999588, -110.04507999999999868 38.65946399999999983, -110.03620700000000454 38.65459699999999543, -110.04945399999999722 38.63342600000000004, -110.04285600000000045 38.61669599999999747, -110.06547100000000228 38.6190379999999962, -110.0688300000000055 38.61306899999999587, -110.05594999999999573 38.60495299999999474, -110.02595200000000375 38.60896400000000028, -110.02065999999999235 38.61146199999999595, -110.01478600000000085 38.62383700000000175, -109.99882399999999905 38.61568199999999962, -109.99614699999999345 38.5980559999999997, -109.99913399999999797 38.59006899999999973, -110.01650999999999669 38.5885589999999965, -110.03306299999999851 38.60435599999999567, -110.05789699999999698 38.58373999999999882, -110.05768299999999726 38.57884899999999817, -110.04428400000000465 38.57736899999999736, -110.03697599999999568 38.57143899999999803, -110.02216799999999353 38.57601499999999817, -110.01489100000000576 38.56136499999999501, -109.99666500000000724 38.56864199999999698, -109.98804499999999962 38.56394199999999728, -110.00542599999999993 38.54381499999999505, -109.99484800000000462 38.52422299999999922, -110.00068000000000268 38.52178599999999875, -110.01243499999999642 38.52512699999999768, -110.01842700000000264 38.51288600000000173, -110.03721199999999669 38.51864499999999936, -110.04558900000000676 38.51461199999999963, -110.04387699999999484 38.50697699999999912, -110.0254019999999997 38.49998099999999823, -111.30570099999999911 38.49999799999999794, -111.30701100000000281 38.67233099999999979)))</t>
+  </si>
+  <si>
+    <t>46-49015</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((-110.17897499999999411 38.90919699999999892, -110.17446900000000198 38.92605700000000013, -110.14045099999999877 38.92432199999999654, -110.13468000000000302 38.92796699999999532, -110.1415619999999933 38.94515200000000021, -110.15264200000000017 38.94969599999999588, -110.14987700000000359 38.95510799999999563, -110.1378389999999996 38.96019299999999674, -110.14929200000000264 38.97189600000000098, -110.15035299999999552 38.9797930000000008, -110.10569999999999879 38.9833849999999984, -110.10568800000000067 38.97979600000000033, -110.06911399999999901 38.97898299999999949, -110.06913400000000536 38.96444799999999731, -110.05050500000000113 38.96445200000000142, -110.05051000000000272 38.95718799999999504, -110.04119900000000598 38.95719199999999915, -110.04119799999999429 38.94993199999999689, -110.00398400000000265 38.94991100000000017, -110.0039769999999919 38.96444599999999525, -110.02258700000000147 38.96445099999999684, -110.02255900000000111 38.97897100000000137, -110.04118400000000122 38.97897499999999837, -110.04117600000000721 38.99351599999999962, -110.05981099999999628 38.99354399999999998, -110.05980700000000638 38.98624799999999624, -110.09633599999999376 38.98625699999999483, -110.09632000000000573 39.00167599999999624, -110.13389899999999955 39.00173600000000107, -110.13394300000000214 38.99437799999999754, -110.15017799999999681 38.99723699999999837, -110.15025199999999472 39.00214899999999574, -110.14284700000000328 39.00095100000000059, -110.13796600000000581 39.00538499999999686, -110.15026500000000453 39.01068699999999723, -110.15332800000000191 39.01670399999999717, -110.13983100000000093 39.02352700000000141, -110.15692199999999445 39.03464100000000059, -110.1497410000000059 39.03996099999999814, -110.13986900000000446 39.05764999999999532, -110.14010600000000295 39.07096200000000152, -110.14612200000000541 39.07598099999999874, -110.14048999999999978 39.08110699999999582, -110.14229600000000175 39.08756999999999948, -110.11771500000000401 39.09643399999999502, -110.11807299999999543 39.10201699999999647, -110.10933199999999488 39.11297700000000077, -110.11479599999999834 39.12086899999999901, -110.11245700000000625 39.12943399999999627, -110.09941100000000347 39.13627599999999518, -110.11614799999999548 39.15256399999999815, -110.11226100000000372 39.16050099999999645, -110.09878399999999488 39.16771500000000117, -110.10501999999999612 39.18148800000000165, -110.0908019999999965 39.19321499999999503, -110.07883499999999799 39.19353299999999507, -110.07323300000000188 39.20131099999999691, -110.07783399999999574 39.22618999999999545, -110.07029199999999491 39.22848899999999617, -110.06243999999999517 39.22323799999999494, -110.05388899999999808 39.22924799999999834, -110.06357199999999352 39.24996600000000058, -110.06088400000000149 39.26444099999999793, -110.07429399999999475 39.27114199999999755, -110.07748999999999739 39.27718899999999991, -110.07046300000000372 39.29133499999999657, -110.0492449999999991 39.30150799999999833, -110.05294499999999402 39.30763799999999719, -110.06193199999999877 39.31008299999999878, -110.0556710000000038 39.31920099999999962, -110.05916999999999462 39.3289660000000012, -110.05570000000000164 39.33075499999999636, -110.04786099999999749 39.32588799999999907, -110.03502399999999284 39.34070200000000028, -110.03407400000000393 39.34896799999999928, -110.02216599999999858 39.35201800000000105, -110.0238820000000004 39.35804499999999706, -110.01982300000000237 39.36257899999999665, -110.02569400000000144 39.37640799999999786, -110.01911400000000185 39.3789159999999967, -110.01974500000000035 39.3954609999999974, -110.01013299999999617 39.40981599999999929, -110.01220700000000363 39.4185809999999961, -110.02343399999999463 39.42309399999999897, -110.02073799999999437 39.42850299999999919, -110.02297799999999484 39.44629700000000128, -110.01555799999999863 39.45533199999999852, -110.02353100000000552 39.46070100000000025, -110.02411800000000142 39.46926899999999705, -109.95334900000000289 39.46927000000000163, -109.95334900000000289 39.46180100000000124, -109.10697199999999896 39.46197899999999947, -109.10429700000000253 39.4693719999999999, -109.09582600000000241 39.4715929999999986, -109.09592999999999563 39.47905099999999834, -109.08756800000000453 39.49233299999999502, -109.07675299999999652 39.48919099999999816, -109.07297599999999704 39.49983599999999484, -109.06827599999999734 39.49554599999999738, -109.06296299999999633 39.49961599999999606, -109.05136294195901314 39.49770327601060416, -109.05243600000000015 38.99998499999999524, -109.05954099999999585 38.71988799999999742, -109.05996200594900358 38.49998903101420211, -110.0254019999999997 38.49998099999999823, -110.04081999999999653 38.5052170000000018, -110.04608899999999494 38.51185900000000117, -110.04003900000000726 38.51801799999999787, -110.01842700000000264 38.51288600000000173, -110.01243499999999642 38.52512699999999768, -110.00068000000000268 38.52178599999999875, -109.99484800000000462 38.52422299999999922, -110.00542599999999993 38.54381499999999505, -109.98804499999999962 38.56394199999999728, -109.99666500000000724 38.56864199999999698, -110.01489100000000576 38.56136499999999501, -110.02216799999999353 38.57601499999999817, -110.03697599999999568 38.57143899999999803, -110.04428400000000465 38.57736899999999736, -110.05768299999999726 38.57884899999999817, -110.05789699999999698 38.58373999999999882, -110.03306299999999851 38.60435599999999567, -110.01650999999999669 38.5885589999999965, -109.99913399999999797 38.59006899999999973, -109.99614699999999345 38.5980559999999997, -109.99882399999999905 38.61568199999999962, -110.01478600000000085 38.62383700000000175, -110.02065999999999235 38.61146199999999595, -110.02595200000000375 38.60896400000000028, -110.05594999999999573 38.60495299999999474, -110.0688300000000055 38.61306899999999587, -110.06547100000000228 38.6190379999999962, -110.04285600000000045 38.61669599999999747, -110.04945399999999722 38.63342600000000004, -110.03620700000000454 38.65459699999999543, -110.04507999999999868 38.65946399999999983, -110.0491439999999983 38.64774399999999588, -110.05616000000000554 38.64618499999999557, -110.05948100000000522 38.64985799999999472, -110.05725800000000447 38.66154999999999831, -110.06839300000000037 38.65643899999999888, -110.07419799999999555 38.65937900000000127, -110.06856899999999655 38.6673979999999986, -110.07051900000000444 38.6721769999999978, -110.07859000000000549 38.67191599999999596, -110.08871600000000512 38.66503199999999651, -110.09482599999999763 38.66676199999999852, -110.08691799999999716 38.67907799999999696, -110.10043400000000702 38.69265899999999903, -110.08670299999999997 38.70576799999999906, -110.08753500000000258 38.71299700000000144, -110.10225300000000459 38.71343799999999646, -110.11793600000000026 38.70557699999999812, -110.12306300000000192 38.7081099999999978, -110.10626700000000255 38.71610400000000141, -110.11341600000000085 38.72993699999999961, -110.1008199999999988 38.74819199999999597, -110.08386099999999885 38.75195199999999573, -110.08193900000000554 38.75666599999999562, -110.09054399999999418 38.77063299999999657, -110.10739800000000344 38.7773249999999976, -110.12129799999999591 38.79113100000000003, -110.11860099999999818 38.79570400000000063, -110.1064970000000045 38.79941900000000032, -110.10612600000000327 38.81065399999999954, -110.11368600000000129 38.81881500000000074, -110.12372799999999984 38.82051799999999986, -110.12075000000000102 38.83151399999999853, -110.14394799999999464 38.839027999999999, -110.14600400000000491 38.84299399999999736, -110.13594399999999496 38.86074399999999684, -110.1381149999999991 38.86786099999999777, -110.14272699999999361 38.86937299999999595, -110.1578010000000063 38.86193899999999957, -110.16252900000000636 38.86392199999999519, -110.15984299999999507 38.89115599999999517, -110.17897499999999411 38.90919699999999892)))</t>
+  </si>
+  <si>
+    <t>Grand</t>
+  </si>
+  <si>
+    <t>46-49019</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((-112.90099299999999971 37.50002099999999672, -112.90116199999999935 37.54348600000000147, -112.36118700000000104 37.54311799999999977, -112.3613330000000019 37.53642500000000126, -112.16491800000000012 37.53590399999999505, -111.84080900000000725 37.53578900000000118, -111.84081799999999873 37.53970899999999489, -110.6463940000000008 37.54106300000000118, -110.661327 37.52442800000000034, -110.6677970000000073 37.49719100000000083, -110.63889600000000257 37.48908999999999736, -110.64089699999999539 37.48519100000000037, -110.66629700000000014 37.47749100000000055, -110.71919800000000578 37.48139099999999502, -110.72599800000000414 37.46999100000000027, -110.72619799999999657 37.45949099999999987, -110.7474990000000048 37.45799099999999981, -110.74599899999999764 37.45269100000000151, -110.72549800000000175 37.43559099999999518, -110.70869799999999827 37.43739099999999809, -110.69919699999999807 37.43069099999999594, -110.70959700000000225 37.4076909999999998, -110.71739800000000287 37.40089100000000144, -110.72629799999999989 37.39989099999999667, -110.74499799999999539 37.40749100000000027, -110.7537980000000033 37.40399099999999777, -110.74059800000000564 37.38509200000000021, -110.72229699999999752 37.37319199999999597, -110.72539700000000096 37.36569199999999569, -110.73589799999999173 37.35739199999999727, -110.73609799999999836 37.34519199999999728, -110.74219800000000191 37.34439199999999914, -110.74839799999999457 37.35139199999999704, -110.7536970000000025 37.35139199999999704, -110.75809800000000394 37.33359199999999589, -110.76919900000000041 37.33159200000000055, -110.77529900000000396 37.3236920000000012, -110.80070000000000618 37.32129199999999969, -110.85470300000000066 37.34779100000000085, -110.86550400000000138 37.35039099999999479, -110.87210400000000732 37.34649100000000033, -110.87370400000000359 37.34029100000000057, -110.86760400000000004 37.32849099999999964, -110.84060200000000407 37.31879199999999486, -110.83720200000000489 37.29929200000000122, -110.84540200000000709 37.29349200000000053, -110.87370400000000359 37.28699199999999792, -110.87350299999999947 37.27719099999999486, -110.86050299999999424 37.26199199999999934, -110.8649029999999982 37.2564920000000015, -110.88695400000000291 37.24999199999999888, -110.87527299999999286 37.229065999999996, -110.89621499999999799 37.21475399999999922, -110.88868100000000538 37.20026199999999506, -110.89900699999999745 37.18689700000000187, -110.89951700000000301 37.17615299999999934, -110.92186800000000346 37.17860599999999494, -110.93343199999999626 37.15060499999999877, -110.94290999999999769 37.14827899999999516, -110.95488799999999685 37.15142199999999661, -110.95066400000000328 37.13496899999999812, -110.9583329999999961 37.12443799999999783, -110.98081100000000276 37.12799700000000058, -110.98466299999999762 37.12499299999999636, -110.9813039999999944 37.1164929999999984, -110.98870399999999847 37.11169299999999538, -111.01369400000000098 37.11568099999999504, -111.04270999999999958 37.10759900000000044, -111.05149000000000115 37.09908599999999979, -111.05767000000000166 37.09939500000000123, -111.06563599999999781 37.10797199999999663, -111.07794300000000476 37.10268800000000056, -111.10197300000000098 37.10285499999999814, -111.12093799999999533 37.10804100000000005, -111.13790699999999845 37.08863999999999805, -111.14960600000000568 37.09023499999999984, -111.1647609999999986 37.10528000000000048, -111.1783489999999972 37.10261299999999807, -111.21666600000000358 37.05756699999999881, -111.22587000000000046 37.05728799999999978, -111.23319499999999493 37.06968399999999519, -111.24087600000000009 37.06707199999999602, -111.24733200000000011 37.04769499999999738, -111.23207600000000639 37.04261999999999944, -111.22993999999999915 37.03856899999999541, -111.24177399999999238 37.02083899999999517, -111.25070700000000556 37.02510799999999591, -111.26776999999999873 37.05358499999999822, -111.2978870000000029 37.0664599999999993, -111.30510599999999499 37.06196200000000118, -111.30292400000000441 37.04673299999999614, -111.28153199999999856 37.04191499999999593, -111.30728999999999473 37.02497299999999569, -111.30499799999999766 37.01337900000000047, -111.31485599999999181 37.01213299999999862, -111.32862699999999734 37.02101799999999798, -111.344333000000006 37.00896600000000092, -111.37148600000000442 37.0015549999999962, -111.40290500000000407 37.00514899999999585, -111.41278398787299864 37.00147768715600449, -112.8991909022780078 37.00031972661560076, -112.90099299999999971 37.50002099999999672)))</t>
+  </si>
+  <si>
+    <t>Kane</t>
+  </si>
+  <si>
+    <t>46-49025</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((-114.04665894185301056 39.98058748939420326, -114.0421451331390017 40.99989652456839906, -112.79935899999999549 40.99993899999999769, -112.49351500000000215 41.07688799999999674, -112.22779500000000041 40.72559400000000096, -112.2076759999999922 40.71572099999999494, -112.2004050000000035 40.70297899999999913, -112.19863999999999749 40.69319300000000084, -112.20436499999999569 40.67864600000000053, -112.20292600000000505 40.6539810000000017, -112.19414999999999338 40.63560700000000026, -112.19767400000000634 40.62546199999999885, -112.17533699999999897 40.60398099999999744, -112.17493600000000242 40.5854009999999974, -112.18361299999999403 40.57303599999999477, -112.18290700000000015 40.56219000000000108, -112.17831200000000536 40.55641500000000121, -112.18278899999999965 40.54097999999999757, -112.1787609999999944 40.52201699999999818, -112.18754099999999596 40.51409799999999706, -112.17584499999999537 40.50014199999999676, -112.1814329999999984 40.49391800000000075, -112.17156699999999603 40.47118199999999888, -112.17286199999999496 40.46706499999999807, -112.19026999999999816 40.46851799999999599, -112.19546499999999867 40.4623149999999967, -112.2122190000000046 40.45928199999999464, -112.21417800000000398 40.4523099999999971, -112.20948500000000081 40.43306799999999868, -112.19463899999999512 40.42110900000000129, -112.20153999999999428 40.38764099999999502, -112.18873399999999663 40.37248699999999957, -112.19372799999999302 40.36789399999999972, -112.1939869999999928 40.35986899999999622, -112.17553300000000149 40.33583699999999794, -112.19627599999999745 40.32583599999999535, -112.1926820000000049 40.32289099999999848, -112.19860500000000059 40.3069149999999965, -112.19208000000000425 40.30410000000000537, -112.18665899999999169 40.28651999999999589, -112.19219599999999559 40.26450000000000529, -112.18384299999999598 40.25813199999999625, -112.18391099999999483 40.24996300000000105, -112.17949899999999275 40.24944399999999689, -112.1768030000000067 40.22789099999999962, -112.1705390000000051 40.22556699999999807, -112.16869800000000623 40.21930700000000058, -112.15384799999999643 40.21821699999999566, -112.14948599999999601 40.21217399999999742, -112.15858099999999808 40.20662899999999951, -112.16039899999999818 40.19884899999999561, -112.14856100000000083 40.19535499999999928, -112.14683800000000247 40.1896549999999948, -112.15337300000000198 40.18215800000000115, -112.14429799999999204 40.17318300000000164, -112.15589900000000512 40.17016799999999677, -112.15917699999999968 40.16297300000000092, -112.17334300000000269 40.15540299999999974, -112.16776899999999273 40.14666599999999619, -112.17610100000000273 40.13080599999999976, -112.16361399999999549 40.12318899999999644, -112.16428600000000415 40.11888700000000085, -112.15096499999999935 40.10555899999999951, -112.15717899999999929 40.09796000000000049, -112.15800400000000536 40.08897899999999481, -112.17262099999999236 40.08457099999999684, -112.17596100000000092 40.07771599999999523, -112.17193500000000483 40.06878799999999785, -112.18019900000000177 40.06704200000000071, -112.18359399999999937 40.05965499999999935, -112.17198100000000238 40.03948400000000163, -112.17707899999999199 40.03058899999999909, -112.17980000000000018 40.011655999999995, -112.1921169999999961 40.00400599999999685, -112.20014700000000119 40.00404899999999486, -112.20199900000000071 39.99978699999999776, -112.2238619999999969 39.98898899999999657, -112.22741399999999601 39.97793599999999969, -112.23512099999999236 39.97056500000000057, -112.23631299999999555 39.96057899999999563, -112.26988199999999551 39.93894699999999887, -112.28128200000000447 39.94144699999999659, -112.30368300000000659 39.93694699999999642, -112.30908300000000111 39.94834699999999827, -112.32368300000000261 39.94434700000000049, -112.33229599999999948 39.95278899999999567, -112.33978299999999706 39.94414700000000096, -112.33538300000000731 39.92324699999999638, -112.34318299999999624 39.91024699999999825, -112.34198800000000062 39.90445799999999821, -114.04713361329200438 39.90609768574429239, -114.04665894185301056 39.98058748939420326)))</t>
+  </si>
+  <si>
+    <t>Tooele</t>
+  </si>
+  <si>
+    <t>46-49045</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((-111.87463099999999372 41.17345399999999955, -111.86882799999999349 41.1810649999999967, -111.87295100000000048 41.18777399999999744, -111.85820800000000474 41.19759599999999722, -111.8175679999999943 41.20470900000000114, -111.80622099999999364 41.21579599999999743, -111.78970599999999536 41.21863199999999949, -111.77448099999999442 41.21814499999999981, -111.76366600000000062 41.21044499999999999, -111.76492899999999509 41.20802899999999624, -111.74908200000000136 41.21454099999999698, -111.7455190000000016 41.20376299999999503, -111.72812100000000157 41.19725599999999588, -111.7165509999999955 41.18625199999999609, -111.68476499999999874 41.18060599999999738, -111.66660600000000159 41.18758700000000061, -111.65687199999999279 41.1861419999999967, -111.64036400000000526 41.19894699999999688, -111.62429099999999949 41.20037299999999902, -111.62287299999999846 41.20575499999999636, -111.61065700000000334 41.21195699999999817, -111.60686300000000415 41.22311799999999948, -111.60925100000000043 41.22922200000000004, -111.59130700000000047 41.24080999999999619, -111.55973099999999931 41.24024000000000001, -111.53525899999999638 41.23618099999999487, -111.52612299999999834 41.22875200000000007, -111.50605899999999338 41.23092700000000121, -111.49718199999999513 41.22690499999999503, -111.49114199999999641 41.2378439999999955, -111.49460700000000202 41.24088899999999569, -111.47731899999999428 41.24528499999999553, -111.47818100000000641 41.25048799999999716, -111.4644349999999946 41.25811099999999954, -111.46645999999999788 41.26247899999999902, -111.45814400000000433 41.26787399999999906, -111.45807399999999632 41.27328599999999881, -111.44512100000000032 41.27805699999999689, -111.44601000000000113 41.28527100000000161, -111.43907000000000096 41.29475499999999499, -111.44941000000000031 41.31570699999999619, -111.4375129999999956 41.32336600000000004, -111.43797599999999193 41.33793500000000165, -111.42626900000000489 41.34318100000000129, -111.42072799999999688 41.36130800000000107, -111.40497399999999573 41.36219200000000029, -111.40407000000000437 41.36875699999999512, -111.39612999999999943 41.37331400000000059, -111.38226099999999974 41.37353999999999843, -111.36702800000000479 41.36164099999999877, -111.34827300000000605 41.36234100000000069, -111.33963599999999872 41.35524999999999807, -111.33194399999999291 41.35747200000000134, -111.32711499999999205 41.35324699999999609, -111.32720299999999725 41.34564299999999548, -111.29488600000000531 41.3299689999999984, -111.29348699999999894 41.32054499999999564, -111.29667100000000346 41.31889199999999818, -111.29248099999999511 41.30977399999999733, -111.28446200000000488 41.30944600000000122, -111.28602300000000014 41.30561000000000149, -111.26180300000000045 41.29668099999999953, -111.25945000000000107 41.2907949999999957, -111.27728299999999706 41.27736799999999562, -111.2742460000000051 41.26438999999999879, -111.28090899999999408 41.26140399999999886, -111.27663599999999633 41.25686499999999768, -111.27719199999999944 41.24490899999999982, -111.26943099999999731 41.23726299999999867, -111.28119599999999423 41.23037000000000063, -111.2816919999999925 41.2251629999999949, -111.25411400000000128 41.22905599999999993, -111.25647200000000225 41.21782899999999472, -111.25202099999999916 41.21455699999999922, -111.2336480000000023 41.21827100000000144, -111.22148400000000379 41.21268399999999588, -111.23167599999999311 41.20265099999999592, -111.22566899999999634 41.19126399999999677, -111.23527699999999641 41.18421800000000133, -111.23470500000000527 41.17471400000000159, -111.26097899999999186 41.14631399999999672, -111.2907289999999989 41.14315999999999462, -111.30700500000000375 41.1309309999999968, -111.33275600000000338 41.13797199999999776, -111.34636000000000422 41.12867099999999709, -111.36691500000000588 41.12994299999999726, -111.36755499999999586 41.11963099999999827, -111.37543399999999849 41.11216499999999741, -111.38163799999999526 41.0965969999999956, -111.38065299999999525 41.08699299999999965, -111.41292500000000132 41.07395799999999753, -111.42405899999999974 41.08005800000000107, -111.4465059999999994 41.0821329999999989, -111.4743220000000008 41.06429199999999469, -111.49054399999999987 41.0610849999999985, -111.4946340000000049 41.06413299999999822, -111.50750999999999635 41.06323400000000134, -111.52364199999999528 41.05623099999999681, -111.55507000000000062 41.03220199999999807, -111.55296599999999785 41.02971099999999893, -111.55742499999999495 41.02421400000000062, -111.55444400000000371 41.0166279999999972, -111.56873000000000218 41.00288400000000166, -111.56663199999999847 41.00048400000000015, -111.59256999999999493 40.99330099999999533, -111.58803199999999833 40.96586299999999881, -111.5832240000000013 40.9611629999999991, -111.56245099999999582 40.96017599999999703, -111.55172600000000216 40.95407000000000153, -111.53426500000000487 40.95815199999999834, -111.52489500000000078 40.95384200000000163, -111.52875399999999217 40.91895600000000144, -111.51664399999999944 40.91770700000000005, -111.510579000000007 40.91209500000000077, -111.509767999999994 40.89778099999999483, -111.48615900000000067 40.87312399999999712, -111.4797930000000008 40.8598700000000008, -111.4812909999999988 40.85437399999999997, -111.48813300000000481 40.85440499999999986, -111.49193200000000559 40.8500969999999981, -111.50573199999999474 40.82538100000000014, -111.51692199999999389 40.8193860000000015, -111.51616599999999835 40.81278599999999557, -111.51083800000000679 40.81038399999999911, -111.51942499999999825 40.79168899999999809, -111.53122199999999964 40.78432000000000102, -111.55483399999999961 40.78003299999999598, -111.55928600000000017 40.7846929999999972, -111.5814629999999994 40.78926899999999733, -111.59421700000000044 40.80500099999999719, -111.61103400000000363 40.81105699999999814, -111.64105200000000195 40.798924999999997, -111.64247899999999447 40.80574199999999507, -111.63904599999999334 40.80928600000000017, -111.64199399999999684 40.81813599999999553, -111.65673400000000015 40.83049599999999657, -111.66569099999999537 40.83065799999999967, -111.66050900000000468 40.84558299999999775, -111.66979899999999759 40.85352799999999718, -111.69591099999999528 40.86178400000000011, -111.71236100000000135 40.85167999999999466, -111.73874399999999696 40.86099799999999505, -111.74699300000000335 40.87117699999999587, -111.76829499999999484 40.87253299999999712, -111.76176699999999187 40.88737299999999664, -111.78169599999999662 40.89604099999999676, -111.77602400000000671 40.90013700000000085, -111.7815920000000034 40.91136900000000054, -111.79347199999999418 40.91586099999999959, -111.79081499999999494 40.9277930000000012, -111.81529799999999852 40.95717899999999645, -111.79473299999999369 40.96093399999999463, -111.78253300000000081 40.95679799999999915, -111.77561799999999437 40.96136099999999658, -111.80612600000000612 41.00168499999999483, -111.81997799999999188 41.00645199999999591, -111.82569900000000018 41.01849899999999849, -111.8383879999999948 41.02348399999999629, -111.83939800000000275 41.03137199999999751, -111.8336879999999951 41.03701199999999716, -111.83944300000000283 41.04064899999999483, -111.84442699999999604 41.05886199999999775, -111.85179600000000733 41.06665100000000024, -111.84835999999999956 41.07573899999999867, -111.85512699999999597 41.09271799999999786, -111.85176199999999369 41.097687999999998, -111.85650400000000104 41.10288200000000103, -111.85611500000000262 41.11191099999999921, -111.84916499999999928 41.11559899999999601, -111.8449370000000016 41.12397899999999851, -111.84900600000000281 41.13375800000000027, -111.85702899999999715 41.1368969999999976, -111.85455799999999726 41.15452200000000005, -111.87055300000000102 41.16109799999999552, -111.87659600000000637 41.16974400000000145, -111.87463099999999372 41.17345399999999955)))</t>
+  </si>
+  <si>
+    <t>46-49029</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((-112.26021599999999978 40.76909299999999803, -112.14827099999999405 40.84613299999999469, -112.0065659999999923 40.92184599999999506, -111.95867200000000707 40.92182199999999881, -111.95926599999999951 40.89632699999999943, -111.96614700000000653 40.89165299999999803, -111.97106899999999996 40.87664499999999634, -111.96289199999999653 40.87000400000000155, -111.96587599999999441 40.85462599999999611, -111.95889800000000491 40.84924499999999625, -111.9630030000000005 40.84816999999999609, -111.95587199999999939 40.84911199999999809, -111.94428700000000276 40.83415399999999806, -111.94586300000000278 40.8217909999999975, -111.87089500000000442 40.82170199999999483, -111.8440389999999951 40.83223499999999717, -111.8221279999999922 40.83423499999999962, -111.81261600000000556 40.84008999999999645, -111.80438700000000551 40.83835099999999585, -111.78922500000000184 40.84555399999999992, -111.77853100000000097 40.84457700000000102, -111.7510379999999941 40.85401399999999938, -111.74599899999999764 40.86037100000000066, -111.71236100000000135 40.85167999999999466, -111.69591099999999528 40.86178400000000011, -111.66399599999999737 40.85019399999999479, -111.66050900000000468 40.84558299999999775, -111.66569099999999537 40.83065799999999967, -111.65673400000000015 40.83049599999999657, -111.65175800000000095 40.82403999999999655, -111.64565000000000339 40.82406100000000038, -111.63904599999999334 40.80928600000000017, -111.64247899999999447 40.80574199999999507, -111.64105200000000195 40.798924999999997, -111.64648400000000095 40.79757000000000033, -111.64874299999999607 40.7922450000000012, -111.64304099999999664 40.78594299999999606, -111.64912900000000207 40.77344300000000032, -111.63992799999999761 40.77053000000000083, -111.63520599999999661 40.76240500000000111, -111.62133400000000449 40.75821899999999687, -111.62348299999999313 40.75347000000000008, -111.61757400000000473 40.74591600000000113, -111.62418399999999963 40.74160399999999527, -111.62346900000000005 40.73173899999999747, -111.61333999999999378 40.72793899999999923, -111.61463799999999935 40.71938399999999803, -111.59272599999999898 40.69912000000000063, -111.60110699999999895 40.68728300000000075, -111.60441099999999892 40.66652299999999798, -111.59387200000000462 40.65165599999999557, -111.57824200000000303 40.64408600000000149, -111.57605100000000675 40.63277799999999473, -111.5689700000000073 40.62940199999999891, -111.56741999999999848 40.62328099999999864, -111.55750499999999192 40.6193230000000014, -111.55902500000000543 40.6142019999999988, -111.5532659999999936 40.60931300000000022, -111.56401400000000024 40.58491699999999724, -111.59850400000000548 40.57785799999999909, -111.60581200000000024 40.56440699999999566, -111.6380839999999921 40.56775299999999618, -111.65025099999999725 40.55113399999999757, -111.66187399999999741 40.549673999999996, -111.66409899999999311 40.54121899999999812, -111.67846199999999612 40.5317099999999968, -111.69811300000000642 40.53572799999999887, -111.71314100000000735 40.53269499999999681, -111.72085400000000277 40.52519399999999905, -111.73510600000000181 40.5326909999999998, -111.74376999999999782 40.52254099999999681, -111.76236799999999505 40.52923799999999943, -111.7878379999999936 40.51376299999999731, -111.7916709999999938 40.50520699999999863, -111.78962599999999838 40.49777199999999766, -111.82940899999999829 40.48469800000000163, -111.83476699999999937 40.48181100000000043, -111.83640099999999507 40.47488500000000045, -111.84638800000000458 40.47653199999999885, -111.85761999999999716 40.46942999999999557, -111.86575000000000557 40.47042199999999923, -111.87316699999999514 40.47704499999999683, -111.89237900000000536 40.46408499999999719, -111.90088099999999827 40.46345099999999917, -111.92965699999999174 40.43471900000000119, -111.96004100000000392 40.41839299999999469, -111.96795899999999335 40.41973199999999622, -111.98213599999999701 40.41421700000000072, -111.99245299999999759 40.42036299999999471, -111.99257299999999304 40.42401799999999668, -112.00656899999999894 40.42670499999999834, -112.00662400000000218 40.43521499999999946, -112.02133899999999755 40.43879299999999688, -112.02453400000000272 40.44509199999999538, -112.02057200000000137 40.4473780000000005, -112.03150800000000231 40.45060099999999892, -112.03340599999999938 40.46281499999999909, -112.03816999999999382 40.46462299999999601, -112.06678899999999999 40.44639000000000095, -112.09355100000000505 40.44782999999999618, -112.11190000000000566 40.43895099999999587, -112.11478099999999358 40.45069600000000065, -112.13879500000000178 40.46846999999999639, -112.15364200000000494 40.46835699999999747, -112.16016600000000381 40.46106499999999784, -112.17286199999999496 40.46706499999999807, -112.1814329999999984 40.49391800000000075, -112.17584499999999537 40.50014199999999676, -112.18754099999999596 40.51409799999999706, -112.1787609999999944 40.52201699999999818, -112.18278899999999965 40.54097999999999757, -112.17831200000000536 40.55641500000000121, -112.18290700000000015 40.56219000000000108, -112.18361299999999403 40.57303599999999477, -112.17493600000000242 40.5854009999999974, -112.17533699999999897 40.60398099999999744, -112.19767400000000634 40.62546199999999885, -112.19414999999999338 40.63560700000000026, -112.20292600000000505 40.6539810000000017, -112.20436499999999569 40.67864600000000053, -112.19877700000000686 40.69751499999999567, -112.2076759999999922 40.71572099999999494, -112.22779500000000041 40.72559400000000096, -112.26021599999999978 40.76909299999999803)))</t>
+  </si>
+  <si>
+    <t>Salt Lake</t>
+  </si>
+  <si>
+    <t>46-49035</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((-111.64797899999999231 40.7762999999999991, -111.64304099999999664 40.78594299999999606, -111.64874299999999607 40.7922450000000012, -111.64648400000000095 40.79757000000000033, -111.61322799999999233 40.81113500000000016, -111.59421700000000044 40.80500099999999719, -111.5814629999999994 40.78926899999999733, -111.55928600000000017 40.7846929999999972, -111.55783800000000383 40.78068999999999988, -111.52746500000000651 40.78575199999999512, -111.51942499999999825 40.79168899999999809, -111.51160699999999792 40.80790199999999857, -111.51692199999999389 40.8193860000000015, -111.51005800000000079 40.82106900000000138, -111.50006000000000483 40.83202199999999493, -111.48813300000000481 40.85440499999999986, -111.48040399999999295 40.85523599999999789, -111.48395299999999963 40.86999399999999838, -111.509767999999994 40.89778099999999483, -111.50845599999999536 40.90942199999999929, -111.51664399999999944 40.91770700000000005, -111.52875399999999217 40.91895600000000144, -111.52489500000000078 40.95384200000000163, -111.53426500000000487 40.95815199999999834, -111.54924599999999657 40.95402699999999641, -111.56245099999999582 40.96017599999999703, -111.5778269999999992 40.95849899999999622, -111.58803199999999833 40.96586299999999881, -111.59256999999999493 40.99330099999999533, -111.56663199999999847 41.00048400000000015, -111.56873000000000218 41.00288400000000166, -111.55444400000000371 41.0166279999999972, -111.55742499999999495 41.02421400000000062, -111.55296599999999785 41.02971099999999893, -111.55507000000000062 41.03220199999999807, -111.54536899999999378 41.03739499999999651, -111.541049000000001 41.04527900000000074, -111.50750999999999635 41.06323400000000134, -111.4946340000000049 41.06413299999999822, -111.49054399999999987 41.0610849999999985, -111.47208499999999276 41.0650580000000005, -111.4465059999999994 41.0821329999999989, -111.42405899999999974 41.08005800000000107, -111.41292500000000132 41.07395799999999753, -111.38065299999999525 41.08699299999999965, -111.38163799999999526 41.0965969999999956, -111.37543399999999849 41.11216499999999741, -111.36755499999999586 41.11963099999999827, -111.36691500000000588 41.12994299999999726, -111.34636000000000422 41.12867099999999709, -111.33275600000000338 41.13797199999999776, -111.30700500000000375 41.1309309999999968, -111.2907289999999989 41.14315999999999462, -111.2328239999999937 41.14288099999999559, -111.20618000000000336 41.16226699999999994, -111.18793200000000354 41.16965099999999467, -111.17565299999999695 41.17025100000000037, -111.14094400000000462 41.18711499999999859, -111.14175699999999836 41.19044499999999687, -111.12945100000000309 41.19762699999999711, -111.13323400000000163 41.2068219999999954, -111.11026300000000333 41.21465800000000002, -111.10133500000000595 41.20768999999999949, -111.07561099999999499 41.24329300000000131, -111.06161199999999667 41.25107699999999511, -111.04655106042400803 41.25162685431100584, -111.04672300000000007 40.99795900000000159, -110.50071800000000621 40.99474599999999924, -110.00071595432901006 40.99735263640130256, -110.00071099999999547 40.8136779999999959, -110.01334400000000358 40.8137439999999998, -110.02565799999999285 40.8205820000000017, -110.0429239999999993 40.82060099999999636, -110.05135699999999588 40.81255000000000166, -110.06440999999999519 40.81421399999999977, -110.10285899999999515 40.80791699999999622, -110.12651400000000024 40.81493499999999841, -110.13950099999999566 40.8109929999999963, -110.1587949999999978 40.82101600000000019, -110.17589999999999861 40.81769899999999751, -110.18780900000000145 40.82613899999999774, -110.2026610000000062 40.82180199999999815, -110.21416899999999828 40.8273889999999966, -110.22578400000000443 40.82646299999999684, -110.22938700000000267 40.83080700000000007, -110.23820499999999356 40.82818999999999932, -110.26156600000000196 40.8348049999999958, -110.28587500000000432 40.82813099999999906, -110.29304700000000139 40.833399, -110.30142299999999977 40.82638800000000145, -110.32032100000000696 40.82050999999999874, -110.34273500000000467 40.82335599999999687, -110.351302000000004 40.81548599999999993, -110.3489450000000005 40.80868199999999746, -110.35516900000000362 40.80009400000000142, -110.37896200000000135 40.78717999999999932, -110.3959689999999938 40.78869799999999657, -110.4111910000000023 40.78436999999999557, -110.42455800000000465 40.79194799999999788, -110.43278200000000311 40.77827800000000025, -110.457421999999994 40.78306699999999552, -110.46178299999999695 40.77582199999999801, -110.47261600000000215 40.771844999999999, -110.48724699999999643 40.78016299999999461, -110.49780799999999203 40.76864700000000141, -110.5239389999999986 40.76152799999999843, -110.53351599999999166 40.77108099999999524, -110.54703100000000404 40.773733, -110.55267499999999359 40.7645209999999949, -110.56848899999999958 40.75699499999999631, -110.57664300000000424 40.75730599999999981, -110.58317599999999459 40.76271699999999498, -110.60702200000000062 40.75726499999999675, -110.62573700000000088 40.7694709999999958, -110.64651100000000383 40.75344199999999972, -110.65674300000000585 40.7402709999999999, -110.69052800000000047 40.74151599999999718, -110.71318499999999574 40.75288400000000166, -110.72183900000000278 40.74547899999999601, -110.75073299999999676 40.74770600000000087, -110.76634900000000528 40.74138699999999602, -110.76521999999999935 40.7370340000000013, -110.77461499999999717 40.73135899999999765, -110.78321699999999339 40.73096299999999559, -110.7937430000000063 40.71901700000000091, -110.80671200000000454 40.71157099999999929, -110.82340600000000563 40.71047599999999989, -110.84747699999999782 40.72526699999999522, -110.86141800000000046 40.72154599999999647, -110.87525899999999979 40.72832299999999606, -110.89198000000000377 40.72712299999999885, -110.89445499999999356 40.72356699999999563, -110.88560000000001082 40.71529299999999552, -110.89776999999999418 40.71335799999999949, -110.90419699999999636 40.70641099999999568, -110.90345899999999801 40.69758300000000162, -110.89376799999999434 40.67974799999999647, -110.93352500000000305 40.68033599999999694, -110.94443099999999447 40.67260399999999976, -110.94882300000000441 40.661330999999997, -110.94498799999999505 40.6464769999999973, -110.9606990000000053 40.62420600000000093, -110.96255999999999631 40.60493199999999803, -110.97576100000000565 40.59314299999999776, -111.01049799999999834 40.59207099999999713, -111.02236399999999605 40.5792549999999963, -111.03116900000000555 40.57596199999999698, -111.05533900000000358 40.58170199999999994, -111.0791059999999959 40.59455099999999561, -111.12086999999999648 40.59045700000000068, -111.13331300000000113 40.57498400000000061, -111.1370589999999936 40.55839399999999983, -111.15135999999999683 40.54835200000000128, -111.21441400000000499 40.57458199999999948, -111.2527199999999965 40.58184299999999922, -111.28554199999999241 40.59702099999999803, -111.29393400000000725 40.60810299999999984, -111.30326999999999771 40.60590399999999534, -111.3267189999999971 40.62312000000000012, -111.35002099999999814 40.62501100000000065, -111.36308700000000727 40.63080799999999471, -111.36862299999999948 40.62894399999999706, -111.37548099999999351 40.63311600000000112, -111.37638599999999656 40.64261299999999721, -111.39019799999999805 40.66064300000000031, -111.38870500000000163 40.67043599999999515, -111.39361300000000199 40.69035999999999831, -111.39931300000000647 40.69044399999999939, -111.41219200000000455 40.68115099999999984, -111.43663599999999292 40.68597599999999659, -111.43619099999999378 40.6741090000000014, -111.43036200000000235 40.66513099999999525, -111.45081299999999658 40.65347599999999773, -111.46040999999999599 40.65233999999999526, -111.46379500000000462 40.644956999999998, -111.4736910000000023 40.64309499999999531, -111.47418500000000563 40.63239199999999585, -111.48688400000000343 40.62084399999999818, -111.48262499999999875 40.60903799999999819, -111.48926500000000317 40.59943799999999925, -111.50049400000000333 40.60609199999999674, -111.5279469999999975 40.61196199999999834, -111.5532659999999936 40.60931300000000022, -111.55902500000000543 40.6142019999999988, -111.55750499999999192 40.6193230000000014, -111.56741999999999848 40.62328099999999864, -111.5689700000000073 40.62940199999999891, -111.57605100000000675 40.63277799999999473, -111.57824200000000303 40.64408600000000149, -111.59387200000000462 40.65165599999999557, -111.60441099999999892 40.66652299999999798, -111.60110699999999895 40.68728300000000075, -111.59272599999999898 40.69912000000000063, -111.59396100000000729 40.70277799999999502, -111.61463799999999935 40.71938399999999803, -111.61333999999999378 40.72793899999999923, -111.62346900000000005 40.73173899999999747, -111.62418399999999963 40.74160399999999527, -111.61757400000000473 40.74591600000000113, -111.62348299999999313 40.75347000000000008, -111.62133400000000449 40.75821899999999687, -111.6374100000000027 40.76389700000000005, -111.63736500000000262 40.76818999999999704, -111.64782599999999491 40.77239099999999894, -111.64797899999999231 40.7762999999999991)))</t>
+  </si>
+  <si>
+    <t>Summit</t>
+  </si>
+  <si>
+    <t>46-49043</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((-110.04760899999999424 39.53438399999999575, -110.02944899999999961 39.54073199999999844, -110.02843699999999671 39.55336099999999533, -110.0370889999999946 39.56012899999999632, -110.0379520000000042 39.56666699999999537, -110.03092300000000137 39.57779699999999679, -110.01872699999999838 39.58539799999999786, -110.0269090000000034 39.59264199999999789, -110.02897799999999506 39.60065099999999916, -110.01366099999999904 39.61506299999999925, -110.01130299999999806 39.62496199999999646, -109.9975379999999916 39.62603699999999662, -110.01170600000000377 39.63781399999999877, -110.01023399999999697 39.64682899999999677, -109.99598799999999699 39.64662899999999723, -109.98430199999999957 39.66412799999999805, -109.98643300000000522 39.68269699999999744, -110.00393099999999436 39.68269000000000091, -110.00453199999999754 39.68747499999999917, -109.99426800000000526 39.69330999999999676, -109.99374099999999999 39.70277999999999707, -109.9748079999999959 39.70498899999999765, -109.97052899999999909 39.70986099999999652, -109.98414200000000562 39.72626599999999542, -109.99189300000000458 39.72975599999999474, -109.99158800000000724 39.7392369999999957, -109.96676899999999932 39.7427369999999982, -109.96055799999999181 39.73530099999999976, -109.96063100000000645 39.72344100000000111, -109.94980699999999274 39.71968400000000088, -109.94820400000000404 39.72305199999999559, -109.95411400000000413 39.73387400000000014, -109.94816299999999387 39.7392019999999988, -109.94507600000000025 39.7499520000000004, -109.93037099999999384 39.74814399999999637, -109.921323000000001 39.77260799999999819, -109.92349699999999757 39.78403199999999629, -109.92913899999999217 39.79075199999999768, -109.92746400000000051 39.79846699999999515, -109.92187400000000252 39.79954000000000036, -109.91921999999999571 39.78619399999999473, -109.89316900000000032 39.78861200000000053, -109.87758599999999376 39.78317399999999537, -109.87389899999999443 39.78613800000000111, -109.87691200000000435 39.79257700000000142, -109.89325900000000047 39.8003309999999999, -109.88308000000000675 39.8062359999999984, -109.97681400000000451 39.80622999999999934, -109.97640200000000732 40.80968599999999924, -109.97004900000000305 40.81071199999999521, -109.96291800000000194 40.80340100000000092, -109.94142200000000287 40.79501399999999478, -109.93220099999999206 40.7965859999999978, -109.92413799999999924 40.79001399999999933, -109.91866999999999166 40.79088499999999584, -109.91391400000000544 40.78244699999999767, -109.89682200000000023 40.78198400000000134, -109.8933799999999934 40.77291900000000169, -109.88306799999999441 40.77487999999999602, -109.87020699999999351 40.7638290000000012, -109.83413299999999424 40.76824200000000076, -109.8318790000000007 40.77573100000000039, -109.81623500000000604 40.77937299999999965, -109.76467800000000352 40.78253300000000081, -109.75249900000000025 40.80285099999999687, -109.731544999999997 40.79442600000000141, -109.71995699999999374 40.8018509999999992, -109.70055600000000595 40.80344499999999641, -109.67677499999999213 40.79486500000000149, -109.66312399999999627 40.80068399999999684, -109.65281199999999728 40.79972999999999672, -109.6501739999999927 40.80546199999999857, -109.63580600000000231 40.81019500000000022, -109.63212400000000457 40.81566999999999723, -109.62060599999999511 40.81246999999999758, -109.61343300000000056 40.81804100000000091, -109.59828199999999754 40.81583899999999687, -109.58060299999999643 40.82534499999999866, -109.57114199999999471 40.81865899999999669, -109.57185300000000439 40.81341499999999911, -109.52926800000000185 40.82760100000000136, -109.51336100000000329 40.81063599999999525, -109.51145800000000463 40.79452799999999968, -109.51898300000000575 40.78227700000000056, -109.5147049999999922 40.77127399999999824, -109.51645200000000102 40.75470599999999877, -109.4842129999999969 40.74046599999999785, -109.47422799999999654 40.74388400000000132, -109.4697840000000042 40.75515299999999996, -109.43653700000000129 40.75769799999999776, -109.44114999999999327 40.76532299999999509, -109.43436300000000472 40.77708499999999958, -109.41495299999999702 40.78681900000000127, -109.39446499999999673 40.79103200000000129, -109.39449100000000215 40.8581659999999971, -109.20324999999999704 40.85840100000000064, -109.20140100000000416 40.78587499999999721, -109.16342500000000371 40.78595500000000129, -109.16106299999999862 40.68381699999999768, -109.123470999999995 40.6841269999999966, -109.12347900000000323 40.66238500000000045, -109.04837297424100484 40.66260885896900135, -109.05136294195901314 39.49770327601060416, -109.06296299999999633 39.49961599999999606, -109.06827599999999734 39.49554599999999738, -109.07297599999999704 39.49983599999999484, -109.07675299999999652 39.48919099999999816, -109.08756800000000453 39.49233299999999502, -109.09592999999999563 39.47905099999999834, -109.09582600000000241 39.4715929999999986, -109.10429700000000253 39.4693719999999999, -109.10697199999999896 39.46197899999999947, -109.95334900000000289 39.46180100000000124, -109.95334900000000289 39.46927000000000163, -110.02396299999999485 39.46926799999999957, -110.02121200000000556 39.47221400000000102, -110.02459199999999839 39.47701800000000105, -110.0156690000000026 39.48518500000000131, -110.01459300000000496 39.4916069999999948, -110.02228200000000413 39.499964999999996, -110.02642900000000736 39.52326099999999798, -110.03957900000000336 39.52492000000000161, -110.04760899999999424 39.53438399999999575)))</t>
+  </si>
+  <si>
+    <t>Uintah</t>
+  </si>
+  <si>
+    <t>46-49047</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((-112.49351500000000215 41.07688799999999674, -112.23806500000000597 41.33655199999999752, -112.02828499999999678 41.3366359999999986, -112.02326600000000667 41.34310399999999674, -112.00873500000000149 41.3437279999999987, -112.00315799999999911 41.34946000000000055, -111.96342199999999423 41.36512099999999492, -111.97446499999999503 41.37663200000000074, -111.97575899999999649 41.38415799999999933, -111.96750199999999609 41.39513600000000082, -111.96775700000000597 41.40993900000000139, -111.97236499999999637 41.42008999999999475, -111.95828600000000108 41.4338729999999984, -111.9381089999999972 41.41579000000000121, -111.92717199999999877 41.41277600000000092, -111.90549699999999689 41.41491699999999554, -111.90107299999999668 41.41948199999999503, -111.89301199999999881 41.41809500000000099, -111.8854429999999951 41.42637399999999559, -111.87577400000000694 41.42357399999999501, -111.87224100000000249 41.42134799999999473, -111.88012799999999913 41.41449499999999517, -111.86850699999999392 41.39849699999999899, -111.86370700000000511 41.39956499999999551, -111.83695000000000164 41.38782899999999643, -111.82784200000000396 41.39260999999999768, -111.81410800000000449 41.38796399999999664, -111.79270200000000557 41.39126499999999709, -111.78084499999999935 41.3786139999999989, -111.76058999999999344 41.36881799999999743, -111.72651000000000465 41.37581399999999832, -111.72688700000000495 41.38505099999999715, -111.71203199999999356 41.39502900000000096, -111.7061779999999942 41.41085999999999956, -111.71873600000000692 41.41702899999999943, -111.72147099999999398 41.4273239999999987, -111.71181099999999731 41.4231410000000011, -111.70779000000000281 41.42542499999999706, -111.69648599999999306 41.4170739999999995, -111.67907099999999332 41.42729599999999834, -111.66692799999999863 41.42880199999999746, -111.64751900000000262 41.40545600000000093, -111.63985800000000381 41.41464099999999604, -111.61899300000000324 41.42209299999999672, -111.58472999999999331 41.41811099999999612, -111.57547599999999477 41.4287739999999971, -111.56466100000000097 41.4231189999999998, -111.55477100000000235 41.42408899999999505, -111.55168100000000209 41.41407600000000144, -111.54187400000000707 41.40505900000000139, -111.53184799999999655 41.41452100000000058, -111.52134800000000325 41.41597099999999898, -111.51083900000000426 41.42310000000000514, -111.50640099999999677 41.41787599999999969, -111.50786200000000292 41.41384299999999996, -111.47551199999999483 41.39986700000000042, -111.47761800000000676 41.38434799999999569, -111.46520499999999743 41.38074299999999539, -111.45853800000000433 41.37327899999999659, -111.44816699999999798 41.3728580000000008, -111.44593700000000069 41.36667200000000122, -111.43776800000000549 41.36668900000000093, -111.43405900000000486 41.36224199999999485, -111.424121999999997 41.36478599999999517, -111.42072799999999688 41.36130800000000107, -111.42626900000000489 41.34318100000000129, -111.43797599999999193 41.33793500000000165, -111.4375129999999956 41.32336600000000004, -111.44941000000000031 41.31570699999999619, -111.43907000000000096 41.29475499999999499, -111.44601000000000113 41.28527100000000161, -111.44512100000000032 41.27805699999999689, -111.45807399999999632 41.27328599999999881, -111.45814400000000433 41.26787399999999906, -111.46645999999999788 41.26247899999999902, -111.4644349999999946 41.25811099999999954, -111.47818100000000641 41.25048799999999716, -111.47731899999999428 41.24528499999999553, -111.49460700000000202 41.24088899999999569, -111.49114199999999641 41.2378439999999955, -111.49718199999999513 41.22690499999999503, -111.50605899999999338 41.23092700000000121, -111.52612299999999834 41.22875200000000007, -111.53525899999999638 41.23618099999999487, -111.55973099999999931 41.24024000000000001, -111.59130700000000047 41.24080999999999619, -111.60925100000000043 41.22922200000000004, -111.60686300000000415 41.22311799999999948, -111.61065700000000334 41.21195699999999817, -111.62287299999999846 41.20575499999999636, -111.62429099999999949 41.20037299999999902, -111.64036400000000526 41.19894699999999688, -111.65687199999999279 41.1861419999999967, -111.66660600000000159 41.18758700000000061, -111.68476499999999874 41.18060599999999738, -111.7165509999999955 41.18625199999999609, -111.72812100000000157 41.19725599999999588, -111.7455190000000016 41.20376299999999503, -111.74908200000000136 41.21454099999999698, -111.76492899999999509 41.20802899999999624, -111.76366600000000062 41.21044499999999999, -111.77448099999999442 41.21814499999999981, -111.79981100000000538 41.21717799999999698, -111.81191599999999653 41.21223899999999674, -111.8175679999999943 41.20470900000000114, -111.85820800000000474 41.19759599999999722, -111.87295100000000048 41.18777399999999744, -111.86882799999999349 41.1810649999999967, -111.87659600000000637 41.16974400000000145, -111.87055300000000102 41.16109799999999552, -111.85455799999999726 41.15452200000000005, -111.85624699999999621 41.1390829999999994, -111.86164599999999325 41.14021799999999729, -111.86125499999999988 41.13751099999999639, -111.91075499999999465 41.13457499999999811, -111.92090899999999465 41.13866999999999763, -111.94948899999999981 41.13807299999999856, -111.97100399999999354 41.15264699999999465, -112.18653999999999371 41.15302700000000158, -112.49351500000000215 41.07688799999999674)))</t>
+  </si>
+  <si>
+    <t>Weber</t>
+  </si>
+  <si>
+    <t>46-49057</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((-112.16472371106800665 41.99669656113780292, -111.50778967478200343 41.99951759416349972, -111.50799100000000408 41.98770299999999622, -111.49749599999999816 41.98509099999999705, -111.48434699999999964 41.97535500000000042, -111.48336000000000467 41.96379900000000163, -111.47586300000000392 41.957650000000001, -111.47748300000000654 41.95341499999999968, -111.47323599999999999 41.947496000000001, -111.47679899999999975 41.93623199999999684, -111.47132100000000321 41.92815699999999879, -111.47833099999999718 41.91268699999999825, -111.49128199999999822 41.91068599999999833, -111.50259400000000198 41.9136529999999965, -111.51154499999999814 41.90860599999999891, -111.50039599999999496 41.89826300000000003, -111.50277900000000386 41.88765999999999678, -111.49365799999999638 41.88712799999999703, -111.49218399999999463 41.88391899999999879, -111.49417699999999343 41.87362600000000157, -111.5026979999999952 41.86800699999999864, -111.50930099999999356 41.8687579999999997, -111.50194399999999462 41.86098899999999645, -111.50786399999999787 41.85258899999999471, -111.46072200000000407 41.81698499999999541, -111.46198699999999349 41.81274599999999708, -111.4539400000000029 41.8037479999999988, -111.4509000000000043 41.79281999999999897, -111.45465599999999995 41.77956999999999965, -111.44932799999999418 41.77185899999999918, -111.44351199999999835 41.77170100000000019, -111.44552199999999686 41.7605259999999987, -111.44101600000000474 41.75577299999999781, -111.44528800000000501 41.74475499999999784, -111.44077799999999456 41.74177399999999949, -111.44208600000000331 41.73606699999999847, -111.41792200000000435 41.72172599999999676, -111.41991299999999399 41.69683399999999551, -111.42694399999999177 41.69431300000000107, -111.42413500000000681 41.6920730000000006, -111.42685500000000332 41.67786399999999958, -111.42338499999999613 41.67430499999999682, -111.41546099999999342 41.67611999999999739, -111.41388999999999498 41.6664169999999956, -111.40743899999999655 41.66670099999999621, -111.40157600000000571 41.65408099999999791, -111.41661799999999971 41.63925599999999605, -111.41187100000000498 41.62577299999999525, -111.42279200000000117 41.62403099999999512, -111.42985500000000343 41.61839299999999753, -111.42656700000000569 41.61048699999999911, -111.42723300000000108 41.58127700000000004, -111.43309899999999857 41.55362900000000081, -111.44518800000000169 41.54433600000000126, -111.44226799999999855 41.53253199999999623, -111.45867400000000202 41.531805999999996, -111.45635899999999197 41.52092999999999989, -111.46713499999999897 41.50925900000000013, -111.47806099999999674 41.50393100000000146, -111.47480600000000095 41.5003019999999978, -111.47798199999999724 41.49725199999999603, -111.47550800000000493 41.48860000000000525, -111.48141599999999585 41.47691999999999979, -111.49055900000000463 41.47220799999999485, -111.48987099999999373 41.46638300000000044, -111.50075699999999301 41.46444899999999478, -111.50353799999999183 41.45941099999999579, -111.50592899999999474 41.44374599999999731, -111.50076099999999713 41.43762399999999957, -111.51083900000000426 41.42310000000000514, -111.52134800000000325 41.41597099999999898, -111.53184799999999655 41.41452100000000058, -111.54187400000000707 41.40505900000000139, -111.55168100000000209 41.41407600000000144, -111.55477100000000235 41.42408899999999505, -111.56466100000000097 41.4231189999999998, -111.57547599999999477 41.4287739999999971, -111.58472999999999331 41.41811099999999612, -111.61899300000000324 41.42209299999999672, -111.63985800000000381 41.41464099999999604, -111.64751900000000262 41.40545600000000093, -111.66692799999999863 41.42880199999999746, -111.67907099999999332 41.42729599999999834, -111.69648599999999306 41.4170739999999995, -111.70779000000000281 41.42542499999999706, -111.71181099999999731 41.4231410000000011, -111.72147099999999398 41.4273239999999987, -111.71873600000000692 41.41702899999999943, -111.70675299999999197 41.41269099999999526, -111.70651700000000517 41.4048439999999971, -111.71203199999999356 41.39502900000000096, -111.72688700000000495 41.38505099999999715, -111.72651000000000465 41.37581399999999832, -111.74629899999999338 41.36978500000000025, -111.76654499999999359 41.37002299999999622, -111.78910700000000134 41.38452600000000103, -111.79270200000000557 41.39126499999999709, -111.81410800000000449 41.38796399999999664, -111.82784200000000396 41.39260999999999768, -111.83695000000000164 41.38782899999999643, -111.86370700000000511 41.39956499999999551, -111.86850699999999392 41.39849699999999899, -111.88012799999999913 41.41449499999999517, -111.87224100000000249 41.42134799999999473, -111.8854429999999951 41.42637399999999559, -111.88156399999999735 41.4411879999999968, -111.89263699999999346 41.44249699999999592, -111.90050200000000302 41.44835099999999528, -111.90010900000000049 41.45369099999999918, -111.9165880000000044 41.46037499999999909, -111.91288799999999526 41.46978099999999756, -111.87833700000000192 41.47422799999999654, -111.87778199999999629 41.4822810000000004, -111.87331399999999348 41.48574299999999937, -111.87555899999999554 41.48968899999999849, -111.88415600000000438 41.49602300000000099, -111.90516900000000078 41.49684999999999491, -111.90911699999999485 41.50709699999999458, -111.90581699999999898 41.51497299999999768, -111.91190000000000282 41.51851800000000026, -111.91635200000000339 41.53840599999999483, -111.92670300000000339 41.53697199999999867, -111.9405930000000069 41.55247399999999658, -111.95367400000000657 41.55044199999999677, -111.96195500000000322 41.54360099999999534, -111.97255300000000489 41.54356899999999797, -111.97780299999999443 41.53515399999999858, -111.98389600000000144 41.53592099999999476, -111.99660599999999988 41.5575720000000004, -111.99410699999999963 41.56612499999999955, -112.00634800000000268 41.59250399999999814, -112.00367400000000373 41.61251599999999939, -112.00770699999999636 41.62352200000000124, -112.00463799999999992 41.62962399999999974, -112.01551999999999509 41.64180899999999497, -112.01274200000000292 41.64806699999999751, -112.01587399999999661 41.65827499999999617, -112.02751700000000312 41.67175900000000155, -112.03090399999999249 41.68183899999999653, -112.04507200000000466 41.68684999999999974, -112.05186199999999985 41.70016299999999632, -112.05031700000000683 41.70603599999999744, -112.04274200000000405 41.71070799999999679, -112.04397500000000321 41.73525399999999763, -112.03386899999999571 41.74965299999999502, -112.03278000000000247 41.76794299999999538, -112.02637099999999748 41.77641200000000055, -112.01457299999999861 41.78065999999999747, -112.00862599999999247 41.79463700000000159, -112.01818799999999499 41.80456799999999618, -112.02971800000000258 41.80850000000000222, -112.02835500000000479 41.81973099999999732, -112.04615400000000136 41.84203600000000023, -112.0528630000000021 41.86623099999999909, -112.06398199999999576 41.86795199999999539, -112.06369700000000478 41.8750609999999952, -112.08549399999999707 41.90331099999999509, -112.10515399999999886 41.91086299999999909, -112.11486700000000383 41.91946499999999531, -112.12192400000000703 41.92817099999999897, -112.13417900000000316 41.95898100000000142, -112.15087699999999415 41.97056399999999599, -112.15384099999999989 41.98501199999999756, -112.16472371106800665 41.99669656113780292)))</t>
+  </si>
+  <si>
+    <t>Cache</t>
+  </si>
+  <si>
+    <t>46-49005</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((-112.68922100000000341 37.80558999999999514, -112.578550000000007 37.80453999999999581, -112.57839699999999539 37.88214699999999624, -112.58846800000000599 37.88220799999999855, -112.58840200000000209 37.89042299999999841, -112.46817699999999718 37.89046400000000148, -112.46696599999999933 37.97765899999999561, -112.47896500000000231 37.97767699999999991, -112.47867999999999711 38.1474189999999993, -112.47344599999999559 38.14885799999999705, -112.06092900000000157 38.14927999999999741, -112.06092399999999998 38.14556400000000025, -111.95134899999999334 38.14598300000000108, -111.95144899999999666 38.15108299999999986, -111.41415100000000393 38.15006100000000089, -111.41402999999999679 38.15398199999999918, -109.92799499999999568 38.15188399999999547, -109.92719400000000007 38.14796099999999512, -109.93322999999999467 38.13630500000000012, -109.95501299999999389 38.13068399999999514, -109.96364400000000217 38.11432999999999538, -109.97793400000000474 38.11010100000000023, -109.98676000000000386 38.100715000000001, -109.99594500000000608 38.100521999999998, -110.00851199999999608 38.10973099999999647, -110.02666399999999669 38.09681399999999485, -110.04716100000000267 38.07057700000000011, -110.04321400000000608 38.06099100000000135, -110.04556200000000388 38.05030099999999749, -110.06387499999999591 38.04295099999999508, -110.0758560000000017 38.0230850000000018, -110.07274200000000519 38.00684100000000143, -110.07858400000000643 37.99817499999999626, -110.09454099999999244 37.99520599999999604, -110.11341000000000179 38.00829600000000141, -110.13669000000000153 38.00538600000000145, -110.14549300000000187 37.99062099999999731, -110.16215699999999345 37.98099099999999595, -110.16633899999999358 37.96630000000000393, -110.20238200000000006 37.94653600000000182, -110.20533199999999852 37.93128499999999548, -110.19846200000000636 37.91759499999999861, -110.20518500000000017 37.89735100000000045, -110.2106420000000071 37.89309199999999578, -110.26797600000000443 37.89828899999999834, -110.27621499999999344 37.89110000000000156, -110.27762199999999382 37.87118999999999858, -110.28435100000000091 37.86610599999999494, -110.29166800000000137 37.86961600000000061, -110.29493600000000697 37.88595399999999813, -110.30498000000000047 37.89051800000000014, -110.36414600000000519 37.89218499999999779, -110.38808600000000126 37.88790499999999639, -110.40461200000000019 37.87992299999999801, -110.40236000000000161 37.85223799999999983, -110.43124000000000251 37.83680899999999525, -110.43753800000000354 37.80691999999999808, -110.47031200000000695 37.80912199999999501, -110.47653499999999838 37.80084300000000042, -110.4705900000000014 37.78125199999999495, -110.46308399999999494 37.77193599999999662, -110.44151300000000049 37.77345799999999798, -110.43099700000000496 37.77890099999999762, -110.4266190000000023 37.77609999999999957, -110.44648200000000315 37.75856100000000026, -110.44728299999999876 37.73692799999999892, -110.46813000000000216 37.72477800000000059, -110.47006600000000276 37.71269499999999653, -110.48787699999999745 37.70218899999999707, -110.48340400000000727 37.69667400000000157, -110.48412199999999928 37.68168099999999754, -110.49431500000000028 37.66557900000000103, -110.49771099999999535 37.65220499999999504, -110.50159399999999721 37.64999999999999858, -110.5138769999999937 37.65663299999999936, -110.53805099999999584 37.63289699999999982, -110.55517199999999889 37.64233899999999977, -110.56096099999999183 37.64071799999999968, -110.56627699999999948 37.61587799999999504, -110.60101099999999974 37.60160199999999975, -110.59933800000000303 37.58165400000000034, -110.60360699999999667 37.57126399999999933, -110.63421999999999912 37.55575499999999778, -110.6463940000000008 37.54106300000000118, -111.84081799999999873 37.53970899999999489, -111.84080900000000725 37.53578900000000118, -112.16491800000000012 37.53590399999999505, -112.3613330000000019 37.53642500000000126, -112.36118700000000104 37.54311799999999977, -112.68375000000000341 37.54369200000000006, -112.68922100000000341 37.80558999999999514)))</t>
+  </si>
+  <si>
+    <t>Garfield</t>
+  </si>
+  <si>
+    <t>46-49017</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((-111.51154499999999814 41.90860599999999891, -111.50259400000000198 41.9136529999999965, -111.49128199999999822 41.91068599999999833, -111.47833099999999718 41.91268699999999825, -111.47132100000000321 41.92815699999999879, -111.47679899999999975 41.93623199999999684, -111.47323599999999999 41.947496000000001, -111.47748300000000654 41.95341499999999968, -111.47586300000000392 41.957650000000001, -111.48336000000000467 41.96379900000000163, -111.48434699999999964 41.97535500000000042, -111.49749599999999816 41.98509099999999705, -111.50799100000000408 41.98770299999999622, -111.50778967478200343 41.99951759416349972, -111.04668900000000065 42.00156700000000143, -111.04655106042400803 41.25162685431100584, -111.06161199999999667 41.25107699999999511, -111.0740160000000003 41.24482099999999463, -111.10133500000000595 41.20768999999999949, -111.11026300000000333 41.21465800000000002, -111.13323400000000163 41.2068219999999954, -111.12945100000000309 41.19762699999999711, -111.14175699999999836 41.19044499999999687, -111.14094400000000462 41.18711499999999859, -111.17565299999999695 41.17025100000000037, -111.18793200000000354 41.16965099999999467, -111.20618000000000336 41.16226699999999994, -111.2328239999999937 41.14288099999999559, -111.24454699999999718 41.14510500000000093, -111.26265800000000183 41.14106599999999503, -111.26497399999999516 41.14404400000000095, -111.23470500000000527 41.17471400000000159, -111.23527699999999641 41.18421800000000133, -111.22566899999999634 41.19126399999999677, -111.23167599999999311 41.20265099999999592, -111.22177600000000552 41.21511900000000139, -111.2336480000000023 41.21827100000000144, -111.25202099999999916 41.21455699999999922, -111.25647200000000225 41.21782899999999472, -111.25411400000000128 41.22905599999999993, -111.2816919999999925 41.2251629999999949, -111.28119599999999423 41.23037000000000063, -111.26943099999999731 41.23726299999999867, -111.27719199999999944 41.24490899999999982, -111.27663599999999633 41.25686499999999768, -111.28090899999999408 41.26140399999999886, -111.2742460000000051 41.26438999999999879, -111.27728299999999706 41.27736799999999562, -111.25945000000000107 41.2907949999999957, -111.26180300000000045 41.29668099999999953, -111.28602300000000014 41.30561000000000149, -111.28446200000000488 41.30944600000000122, -111.29248099999999511 41.30977399999999733, -111.29667100000000346 41.31889199999999818, -111.29348699999999894 41.32054499999999564, -111.29488600000000531 41.3299689999999984, -111.32720299999999725 41.34564299999999548, -111.32711499999999205 41.35324699999999609, -111.33194399999999291 41.35747200000000134, -111.33963599999999872 41.35524999999999807, -111.34827300000000605 41.36234100000000069, -111.36702800000000479 41.36164099999999877, -111.38226099999999974 41.37353999999999843, -111.39612999999999943 41.37331400000000059, -111.40407000000000437 41.36875699999999512, -111.40497399999999573 41.36219200000000029, -111.42072799999999688 41.36130800000000107, -111.424121999999997 41.36478599999999517, -111.43405900000000486 41.36224199999999485, -111.43776800000000549 41.36668900000000093, -111.44593700000000069 41.36667200000000122, -111.44816699999999798 41.3728580000000008, -111.45853800000000433 41.37327899999999659, -111.46520499999999743 41.38074299999999539, -111.47761800000000676 41.38434799999999569, -111.47551199999999483 41.39986700000000042, -111.49989399999999762 41.40889500000000112, -111.50786200000000292 41.41384299999999996, -111.50640099999999677 41.41787599999999969, -111.51069099999999423 41.42068299999999681, -111.51045799999999986 41.42801800000000156, -111.50076099999999713 41.43762399999999957, -111.50592899999999474 41.44374599999999731, -111.50353799999999183 41.45941099999999579, -111.50075699999999301 41.46444899999999478, -111.48987099999999373 41.46638300000000044, -111.49055900000000463 41.47220799999999485, -111.48141599999999585 41.47691999999999979, -111.47550800000000493 41.48860000000000525, -111.47798199999999724 41.49725199999999603, -111.47480600000000095 41.5003019999999978, -111.47806099999999674 41.50393100000000146, -111.46713499999999897 41.50925900000000013, -111.45635899999999197 41.52092999999999989, -111.45867400000000202 41.531805999999996, -111.44226799999999855 41.53253199999999623, -111.44518800000000169 41.54433600000000126, -111.43309899999999857 41.55362900000000081, -111.42723300000000108 41.58127700000000004, -111.42656700000000569 41.61048699999999911, -111.42985500000000343 41.61839299999999753, -111.42279200000000117 41.62403099999999512, -111.41187100000000498 41.62577299999999525, -111.41661799999999971 41.63925599999999605, -111.40157600000000571 41.65408099999999791, -111.40743899999999655 41.66670099999999621, -111.41388999999999498 41.6664169999999956, -111.41546099999999342 41.67611999999999739, -111.42338499999999613 41.67430499999999682, -111.42685500000000332 41.67786399999999958, -111.42413500000000681 41.6920730000000006, -111.42694399999999177 41.69431300000000107, -111.41991299999999399 41.69683399999999551, -111.41792200000000435 41.72172599999999676, -111.44208600000000331 41.73606699999999847, -111.44077799999999456 41.74177399999999949, -111.44528800000000501 41.74475499999999784, -111.44101600000000474 41.75577299999999781, -111.44552199999999686 41.7605259999999987, -111.44351199999999835 41.77170100000000019, -111.44932799999999418 41.77185899999999918, -111.45465599999999995 41.77956999999999965, -111.4509000000000043 41.79281999999999897, -111.4539400000000029 41.8037479999999988, -111.46198699999999349 41.81274599999999708, -111.46072200000000407 41.81698499999999541, -111.50786399999999787 41.85258899999999471, -111.50194399999999462 41.86098899999999645, -111.50930099999999356 41.8687579999999997, -111.5026979999999952 41.86800699999999864, -111.49417699999999343 41.87362600000000157, -111.49218399999999463 41.88391899999999879, -111.49365799999999638 41.88712799999999703, -111.50277900000000386 41.88765999999999678, -111.50039599999999496 41.89826300000000003, -111.51154499999999814 41.90860599999999891)))</t>
+  </si>
+  <si>
+    <t>Rich</t>
+  </si>
+  <si>
+    <t>46-49033</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((-114.04778299999999547 39.79415999999999798, -114.04713361329200438 39.90609768574429239, -112.34198800000000062 39.90445799999999821, -112.34318299999999624 39.91024699999999825, -112.33538300000000731 39.92324699999999638, -112.33978299999999706 39.94414700000000096, -112.33229599999999948 39.95278899999999567, -112.32368300000000261 39.94434700000000049, -112.30908300000000111 39.94834699999999827, -112.30368300000000659 39.93694699999999642, -112.28128200000000447 39.94144699999999659, -112.26988199999999551 39.93894699999999887, -112.23631299999999555 39.96057899999999563, -112.23512099999999236 39.97056500000000057, -112.22741399999999601 39.97793599999999969, -112.2238619999999969 39.98898899999999657, -112.20199900000000071 39.99978699999999776, -112.20014700000000119 40.00404899999999486, -112.1921169999999961 40.00400599999999685, -112.17980000000000018 40.011655999999995, -112.160026000000002 40.00675799999999782, -112.13275500000000306 39.97752499999999998, -112.11013900000000376 39.97383500000000112, -112.10242399999999918 39.95888800000000174, -112.09413499999999431 39.9544739999999976, -112.10252800000000661 39.94825999999999766, -112.10625899999999433 39.93930499999999739, -112.10250000000000625 39.93484499999999571, -112.10358999999999696 39.92876700000000056, -112.09302599999999472 39.93004200000000026, -112.0852480000000071 39.92549400000000048, -112.08125599999999622 39.91314699999999505, -112.06255199999999661 39.90467999999999904, -112.06110599999999522 39.89814099999999542, -112.05351100000000031 39.89339700000000022, -112.05955600000000061 39.88716999999999757, -112.05914699999999584 39.88037999999999528, -112.08122000000000185 39.86508099999999644, -112.08061399999999708 39.85331699999999699, -112.07408900000000074 39.84750100000000117, -112.07521500000000003 39.83969299999999691, -112.06541500000000156 39.83003899999999931, -112.07270900000000324 39.81214200000000147, -112.07787999999999329 39.80849399999999605, -112.07998100000000363 39.80195700000000159, -112.07675600000000316 39.80012599999999878, -112.08726500000000215 39.79062599999999605, -112.08984300000000189 39.78192800000000062, -112.06832699999999647 39.77736399999999861, -112.06095000000000539 39.78215300000000099, -112.05503500000000372 39.77712499999999807, -112.04718400000000145 39.77684899999999857, -112.04156100000000151 39.7834269999999961, -112.03033499999999378 39.78121699999999805, -112.00446900000000028 39.79559100000000171, -112.00329200000000185 39.79988199999999665, -111.99039399999999489 39.80531500000000023, -111.98917699999999797 39.81169699999999523, -111.96939100000000167 39.80724199999999513, -111.96268200000000093 39.81607100000000088, -111.96404300000000376 39.8273669999999953, -111.95716899999999328 39.83683500000000066, -111.95041499999999246 39.83436799999999778, -111.94827899999999943 39.84899000000000058, -111.92808399999999835 39.86487100000000083, -111.92661599999999567 39.87267200000000145, -111.92168200000000411 39.87448200000000043, -111.90946399999999983 39.89457099999999912, -111.9028030000000058 39.89850599999999758, -111.89113199999999892 39.89835300000000018, -111.88155100000000175 39.90740399999999966, -111.86619799999999714 39.90574999999999761, -111.85849400000000742 39.91036599999999623, -111.858429000000001 39.91537299999999533, -111.83362599999999532 39.92394499999999624, -111.83271100000000331 39.93669099999999617, -111.82528999999999542 39.94769600000000054, -111.78865999999999303 39.92588200000000143, -111.78625599999999451 39.92136199999999491, -111.78909699999999816 39.91532799999999526, -111.78084599999999682 39.90082400000000007, -111.76865800000000206 39.89832399999999524, -111.75788900000000581 39.89041299999999524, -111.76104200000000333 39.88386099999999601, -111.75735000000000241 39.87595199999999807, -111.73813400000000229 39.86424499999999682, -111.73458200000000318 39.85647099999999909, -111.73759599999999637 39.85131799999999913, -111.74645800000000406 39.85012100000000146, -111.7487339999999989 39.83320499999999953, -111.76632499999999482 39.81081700000000012, -111.64194399999999519 39.81286899999999918, -111.6420569999999941 39.79831399999999775, -111.62212300000000198 39.79848299999999739, -111.62251399999999535 39.78381600000000162, -111.58485799999999699 39.78423499999999535, -111.58475400000000377 39.74014100000000127, -111.64251899999999296 39.73969299999999549, -111.64261899999999628 39.72516199999999742, -111.6613490000000013 39.72505799999999709, -111.6613619999999969 39.7176550000000006, -111.68035899999999572 39.71746499999999713, -111.68026899999999557 39.71019599999999627, -111.68959599999999455 39.71036000000000143, -111.68948100000000068 39.69523099999999971, -111.71748200000000395 39.69455999999999563, -111.71322399999999675 39.46029399999999754, -111.74773600000000329 39.46007699999999829, -111.74704400000000248 39.38275000000000148, -111.92238899999999546 39.38159100000000024, -111.92169799999999213 39.36686199999999758, -111.95877299999999366 39.36613299999999782, -111.95810600000000079 39.33684600000000131, -112.01581199999999683 39.33686300000000102, -112.01600299999999777 39.31456099999999765, -112.05342100000000016 39.31448299999999563, -112.07221799999999234 39.31492300000000029, -112.07210800000000006 39.32969500000000096, -112.18892200000000514 39.32939199999999857, -112.18890700000000038 39.37308900000000023, -112.19359599999999944 39.3730899999999977, -112.19327699999999481 39.48983399999999477, -112.20262599999999509 39.48985799999999813, -112.20263299999999163 39.50432299999999941, -112.20730000000000359 39.50433400000000006, -112.20728499999999883 39.51156599999999486, -112.21196100000000229 39.51157899999999756, -112.21197300000000041 39.52604199999999679, -112.19324199999999792 39.52602299999999502, -112.19329199999999958 39.54045099999999735, -112.20266599999999357 39.54043399999999764, -112.20735299999999768 39.54769599999999485, -112.21202900000000113 39.54773000000000138, -112.21204500000000337 39.55398699999999934, -113.81574299999999766 39.5526440000000008, -113.81576599999999644 39.54408999999999708, -114.04772798183900306 39.54274080232679722, -114.04778299999999547 39.79415999999999798)))</t>
+  </si>
+  <si>
+    <t>Juab</t>
+  </si>
+  <si>
+    <t>46-49023</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((-112.21322700000000339 40.45510799999999563, -112.2122190000000046 40.45928199999999464, -112.19546499999999867 40.4623149999999967, -112.19026999999999816 40.46851799999999599, -112.17286199999999496 40.46706499999999807, -112.16016600000000381 40.46106499999999784, -112.15364200000000494 40.46835699999999747, -112.1436779999999942 40.47035199999999833, -112.11478099999999358 40.45069600000000065, -112.11190000000000566 40.43895099999999587, -112.09355100000000505 40.44782999999999618, -112.06678899999999999 40.44639000000000095, -112.03816999999999382 40.46462299999999601, -112.03340599999999938 40.46281499999999909, -112.03150800000000231 40.45060099999999892, -112.02057200000000137 40.4473780000000005, -112.02453400000000272 40.44509199999999538, -112.02133899999999755 40.43879299999999688, -112.00662400000000218 40.43521499999999946, -112.00656899999999894 40.42670499999999834, -111.99257299999999304 40.42401799999999668, -111.99245299999999759 40.42036299999999471, -111.98213599999999701 40.41421700000000072, -111.96795899999999335 40.41973199999999622, -111.96004100000000392 40.41839299999999469, -111.92965699999999174 40.43471900000000119, -111.90088099999999827 40.46345099999999917, -111.89237900000000536 40.46408499999999719, -111.87316699999999514 40.47704499999999683, -111.86575000000000557 40.47042199999999923, -111.85761999999999716 40.46942999999999557, -111.84638800000000458 40.47653199999999885, -111.83640099999999507 40.47488500000000045, -111.83476699999999937 40.48181100000000043, -111.82940899999999829 40.48469800000000163, -111.78962599999999838 40.49777199999999766, -111.7916709999999938 40.50520699999999863, -111.7878379999999936 40.51376299999999731, -111.76236799999999505 40.52923799999999943, -111.74376999999999782 40.52254099999999681, -111.73510600000000181 40.5326909999999998, -111.72085400000000277 40.52519399999999905, -111.71314100000000735 40.53269499999999681, -111.69811300000000642 40.53572799999999887, -111.67846199999999612 40.5317099999999968, -111.66409899999999311 40.54121899999999812, -111.66187399999999741 40.549673999999996, -111.65025099999999725 40.55113399999999757, -111.6380839999999921 40.56775299999999618, -111.60581200000000024 40.56440699999999566, -111.60126599999999542 40.57625099999999918, -111.59394199999999842 40.57706599999999497, -111.56772499999999582 40.54721099999999723, -111.57260899999999992 40.53774500000000103, -111.56976600000000133 40.52683999999999997, -111.57542999999999722 40.51640700000000095, -111.57544300000000703 40.50318800000000152, -111.57912600000000225 40.50035599999999647, -111.57482899999999404 40.48712400000000144, -111.5948669999999936 40.46770799999999468, -111.60948399999999481 40.46632499999999766, -111.62043699999999546 40.45501799999999548, -111.62096800000000485 40.44965299999999786, -111.61173399999999845 40.43146600000000035, -111.5952609999999936 40.43261299999999636, -111.58836900000000014 40.4213009999999997, -111.58380300000000318 40.42021099999999478, -111.5836749999999995 40.41284499999999724, -111.57426800000000355 40.41290699999999703, -111.57420899999999619 40.39137300000000153, -111.56009699999999896 40.38776999999999617, -111.56019499999999312 40.36983699999999686, -111.55528400000000033 40.3699009999999987, -111.55523499999999615 40.36269599999999969, -111.48033699999999158 40.36216900000000152, -111.48053600000000074 40.35495699999999886, -111.47585800000000233 40.35486499999999666, -111.47157799999999384 40.34758399999999767, -111.46228100000000438 40.34748400000000146, -111.4624639999999971 40.34033900000000017, -111.45315300000000036 40.34028399999999692, -111.45329499999999712 40.33426699999999698, -111.43790599999999813 40.32177199999999573, -111.45719300000000374 40.30074099999999504, -111.44344800000000362 40.28988199999999864, -111.43368599999999446 40.2919029999999978, -111.42648199999999292 40.28690599999999478, -111.41267700000000218 40.28955200000000048, -111.41036300000000381 40.29511099999999857, -111.39664500000000658 40.29230400000000145, -111.39212499999999295 40.29620399999999592, -111.38142700000000218 40.29444099999999906, -111.37715599999999938 40.29748699999999673, -111.36075300000000254 40.28872700000000151, -111.33956200000000081 40.28865499999999855, -111.32754400000000317 40.28213499999999669, -111.32174100000000294 40.28730699999999842, -111.30789300000000708 40.28390399999999971, -111.30789699999999698 40.2745000000000033, -111.29420600000000263 40.27074100000000101, -111.29417399999999816 40.26546899999999596, -111.2787620000000004 40.25879299999999716, -111.26478600000000085 40.24232800000000054, -111.26810199999999895 40.23693199999999592, -111.27361700000000155 40.2362150000000014, -111.27337199999999484 40.22186099999999698, -111.26186900000000435 40.21097799999999722, -111.26478099999999927 40.20949499999999688, -111.25640599999999836 40.20072700000000054, -111.25815500000000213 40.19784899999999794, -111.24790199999999629 40.19372699999999554, -111.22522499999999468 40.16636700000000104, -111.23116500000000428 40.14748099999999909, -111.22485600000000261 40.14251199999999642, -111.22141299999999831 40.12502999999999531, -111.2419089999999926 40.09014799999999923, -111.23800699999999608 40.08055099999999982, -111.24069299999999316 40.07350299999999521, -111.23605799999999988 40.06911300000000153, -111.24922700000000475 40.05559499999999673, -111.23823099999999897 40.03873399999999805, -111.22670499999999549 40.03569299999999487, -111.2038299999999964 40.04929800000000029, -111.19770800000000577 40.03117900000000162, -111.19186000000000547 40.03013699999999631, -111.18608000000000402 40.0196550000000002, -111.1715549999999979 40.01058499999999896, -111.16766400000000203 39.99058999999999742, -111.16014400000000251 39.99197399999999902, -111.15219600000000355 39.98505899999999968, -111.14304699999999571 39.98698799999999665, -111.12934599999999818 39.97037399999999963, -111.11927099999999768 39.96815600000000046, -111.1202210000000008 39.95707699999999818, -111.13129599999999186 39.94739599999999768, -111.11842199999999536 39.94348399999999799, -111.08306100000000072 39.94319799999999532, -111.08245499999999595 39.90015499999999804, -110.85764700000000005 39.89970699999999937, -110.85778000000000532 39.81328500000000048, -111.76632499999999482 39.81081700000000012, -111.7487339999999989 39.83320499999999953, -111.74645800000000406 39.85012100000000146, -111.73759599999999637 39.85131799999999913, -111.73458200000000318 39.85647099999999909, -111.73813400000000229 39.86424499999999682, -111.75735000000000241 39.87595199999999807, -111.76104200000000333 39.88386099999999601, -111.75788900000000581 39.89041299999999524, -111.76865800000000206 39.89832399999999524, -111.78084599999999682 39.90082400000000007, -111.78909699999999816 39.91532799999999526, -111.78625599999999451 39.92136199999999491, -111.78865999999999303 39.92588200000000143, -111.82528999999999542 39.94769600000000054, -111.83271100000000331 39.93669099999999617, -111.83362599999999532 39.92394499999999624, -111.858429000000001 39.91537299999999533, -111.85849400000000742 39.91036599999999623, -111.86619799999999714 39.90574999999999761, -111.88155100000000175 39.90740399999999966, -111.89113199999999892 39.89835300000000018, -111.9028030000000058 39.89850599999999758, -111.90946399999999983 39.89457099999999912, -111.92168200000000411 39.87448200000000043, -111.92661599999999567 39.87267200000000145, -111.92808399999999835 39.86487100000000083, -111.94827899999999943 39.84899000000000058, -111.95041499999999246 39.83436799999999778, -111.95716899999999328 39.83683500000000066, -111.96404300000000376 39.8273669999999953, -111.96268200000000093 39.81607100000000088, -111.96939100000000167 39.80724199999999513, -111.98917699999999797 39.81169699999999523, -111.99039399999999489 39.80531500000000023, -112.00329200000000185 39.79988199999999665, -112.00446900000000028 39.79559100000000171, -112.03033499999999378 39.78121699999999805, -112.04156100000000151 39.7834269999999961, -112.04718400000000145 39.77684899999999857, -112.05503500000000372 39.77712499999999807, -112.06095000000000539 39.78215300000000099, -112.06832699999999647 39.77736399999999861, -112.08984300000000189 39.78192800000000062, -112.08726500000000215 39.79062599999999605, -112.07675600000000316 39.80012599999999878, -112.07998100000000363 39.80195700000000159, -112.07787999999999329 39.80849399999999605, -112.07270900000000324 39.81214200000000147, -112.06541500000000156 39.83003899999999931, -112.07521500000000003 39.83969299999999691, -112.07408900000000074 39.84750100000000117, -112.08061399999999708 39.85331699999999699, -112.08122000000000185 39.86508099999999644, -112.05914699999999584 39.88037999999999528, -112.05955600000000061 39.88716999999999757, -112.05351100000000031 39.89339700000000022, -112.06110599999999522 39.89814099999999542, -112.06255199999999661 39.90467999999999904, -112.08125599999999622 39.91314699999999505, -112.0852480000000071 39.92549400000000048, -112.09302599999999472 39.93004200000000026, -112.10358999999999696 39.92876700000000056, -112.10250000000000625 39.93484499999999571, -112.10625899999999433 39.93930499999999739, -112.10252800000000661 39.94825999999999766, -112.09413499999999431 39.9544739999999976, -112.10242399999999918 39.95888800000000174, -112.11013900000000376 39.97383500000000112, -112.13275500000000306 39.97752499999999998, -112.160026000000002 40.00675799999999782, -112.17980000000000018 40.011655999999995, -112.17707899999999199 40.03058899999999909, -112.17198100000000238 40.03948400000000163, -112.18359399999999937 40.05965499999999935, -112.18019900000000177 40.06704200000000071, -112.17193500000000483 40.06878799999999785, -112.17454800000000148 40.08183400000000063, -112.15800400000000536 40.08897899999999481, -112.15089199999999892 40.10729800000000012, -112.16085900000000208 40.11432099999999679, -112.16361399999999549 40.12318899999999644, -112.17610100000000273 40.13080599999999976, -112.16776899999999273 40.14666599999999619, -112.17399299999999585 40.15428800000000109, -112.15917699999999968 40.16297300000000092, -112.15589900000000512 40.17016799999999677, -112.14429799999999204 40.17318300000000164, -112.15337300000000198 40.18215800000000115, -112.14683800000000247 40.1896549999999948, -112.14856100000000083 40.19535499999999928, -112.16039899999999818 40.19884899999999561, -112.15858099999999808 40.20662899999999951, -112.14948599999999601 40.21217399999999742, -112.15384799999999643 40.21821699999999566, -112.16869800000000623 40.21930700000000058, -112.1705390000000051 40.22556699999999807, -112.1768030000000067 40.22789099999999962, -112.17949899999999275 40.24944399999999689, -112.18391099999999483 40.24996300000000105, -112.18384299999999598 40.25813199999999625, -112.19219599999999559 40.26450000000000529, -112.18665899999999169 40.28651999999999589, -112.19208000000000425 40.30410000000000537, -112.19860500000000059 40.3069149999999965, -112.1926820000000049 40.32289099999999848, -112.19627599999999745 40.32583599999999535, -112.17553300000000149 40.33583699999999794, -112.1939869999999928 40.35986899999999622, -112.19372799999999302 40.36789399999999972, -112.18873399999999663 40.37248699999999957, -112.20153999999999428 40.38764099999999502, -112.19463899999999512 40.42110900000000129, -112.20948500000000081 40.43306799999999868, -112.21322700000000339 40.45510799999999563)))</t>
+  </si>
+  <si>
+    <t>46-49049</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((-111.24749599999999816 39.81302799999999564, -110.51819500000000573 39.81164100000000161, -110.51819799999999816 39.80671900000000107, -109.88308000000000675 39.8062359999999984, -109.89325900000000047 39.8003309999999999, -109.87691200000000435 39.79257700000000142, -109.87389899999999443 39.78613800000000111, -109.87758599999999376 39.78317399999999537, -109.89316900000000032 39.78861200000000053, -109.91921999999999571 39.78619399999999473, -109.92187400000000252 39.79954000000000036, -109.92746400000000051 39.79846699999999515, -109.92913899999999217 39.79075199999999768, -109.92349699999999757 39.78403199999999629, -109.921323000000001 39.77260799999999819, -109.93037099999999384 39.74814399999999637, -109.94507600000000025 39.7499520000000004, -109.94816299999999387 39.7392019999999988, -109.95411400000000413 39.73387400000000014, -109.94820400000000404 39.72305199999999559, -109.94980699999999274 39.71968400000000088, -109.96063100000000645 39.72344100000000111, -109.96055799999999181 39.73530099999999976, -109.96676899999999932 39.7427369999999982, -109.98683099999999513 39.74100299999999919, -109.9933719999999937 39.73576599999999814, -109.99189300000000458 39.72975599999999474, -109.98414200000000562 39.72626599999999542, -109.97052899999999909 39.70986099999999652, -109.9748079999999959 39.70498899999999765, -109.99374099999999999 39.70277999999999707, -109.99426800000000526 39.69330999999999676, -110.00453199999999754 39.68747499999999917, -110.00393099999999436 39.68269000000000091, -109.98643300000000522 39.68269699999999744, -109.98430199999999957 39.66412799999999805, -109.99598799999999699 39.64662899999999723, -110.01023399999999697 39.64682899999999677, -110.01170600000000377 39.63781399999999877, -109.9975379999999916 39.62603699999999662, -110.01130299999999806 39.62496199999999646, -110.01366099999999904 39.61506299999999925, -110.02897799999999506 39.60065099999999916, -110.0269090000000034 39.59264199999999789, -110.01872699999999838 39.58539799999999786, -110.03092300000000137 39.57779699999999679, -110.0379520000000042 39.56666699999999537, -110.0370889999999946 39.56012899999999632, -110.02843699999999671 39.55336099999999533, -110.02944899999999961 39.54073199999999844, -110.04823000000000377 39.53314999999999912, -110.03957900000000336 39.52492000000000161, -110.02642900000000736 39.52326099999999798, -110.02228200000000413 39.499964999999996, -110.01459300000000496 39.4916069999999948, -110.0156690000000026 39.48518500000000131, -110.02459199999999839 39.47701800000000105, -110.02121200000000556 39.47221400000000102, -110.02396299999999485 39.46926799999999957, -111.08133300000000077 39.46745500000000106, -111.08167500000000416 39.47356500000000068, -111.07535099999999773 39.47925999999999647, -111.07468900000000644 39.49114099999999894, -111.08069299999999657 39.49613899999999944, -111.08489000000000146 39.50794700000000148, -111.08553000000000566 39.52184599999999648, -111.09820799999999963 39.53601799999999855, -111.10743800000000192 39.53806399999999854, -111.10649200000000292 39.54652199999999596, -111.11633499999999231 39.5518819999999991, -111.1144390000000044 39.55623200000000139, -111.11875200000000063 39.56274700000000166, -111.11355199999999854 39.56877499999999515, -111.12029900000000282 39.57244000000000028, -111.13224800000000414 39.61387599999999765, -111.13774399999999787 39.61521700000000124, -111.14075499999999863 39.60834599999999739, -111.14876300000000242 39.60624699999999621, -111.14823499999999967 39.6003029999999967, -111.15705699999999467 39.59601299999999924, -111.17049199999999587 39.6033869999999979, -111.17608799999999292 39.61432999999999538, -111.18623900000000049 39.61949500000000057, -111.19269300000000555 39.64132199999999528, -111.20198200000000099 39.64555000000000007, -111.20131100000000401 39.65712099999999651, -111.22163999999999362 39.67532899999999785, -111.22215500000000077 39.69250499999999704, -111.22921200000000397 39.69330699999999723, -111.23006399999999871 39.69951400000000064, -111.23739600000000394 39.70314099999999513, -111.24739099999999326 39.70434999999999803, -111.24749599999999816 39.81302799999999564)))</t>
+  </si>
+  <si>
+    <t>Carbon</t>
+  </si>
+  <si>
+    <t>46-49007</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((-110.00071595432901006 40.99735263640130256, -109.05007600000000423 41.00065899999999885, -109.04837297424100484 40.66260885896900135, -109.12347900000000323 40.66238500000000045, -109.123470999999995 40.6841269999999966, -109.16106299999999862 40.68381699999999768, -109.16342500000000371 40.78595500000000129, -109.20140100000000416 40.78587499999999721, -109.20324999999999704 40.85840100000000064, -109.39449100000000215 40.8581659999999971, -109.39446499999999673 40.79103200000000129, -109.41495299999999702 40.78681900000000127, -109.43436300000000472 40.77708499999999958, -109.44114999999999327 40.76532299999999509, -109.43653700000000129 40.75769799999999776, -109.4697840000000042 40.75515299999999996, -109.47422799999999654 40.74388400000000132, -109.4842129999999969 40.74046599999999785, -109.51645200000000102 40.75470599999999877, -109.5147049999999922 40.77127399999999824, -109.51898300000000575 40.78227700000000056, -109.51145800000000463 40.79452799999999968, -109.51336100000000329 40.81063599999999525, -109.52926800000000185 40.82760100000000136, -109.57185300000000439 40.81341499999999911, -109.57114199999999471 40.81865899999999669, -109.58060299999999643 40.82534499999999866, -109.59828199999999754 40.81583899999999687, -109.61343300000000056 40.81804100000000091, -109.62060599999999511 40.81246999999999758, -109.63212400000000457 40.81566999999999723, -109.63580600000000231 40.81019500000000022, -109.6501739999999927 40.80546199999999857, -109.65281199999999728 40.79972999999999672, -109.66312399999999627 40.80068399999999684, -109.67677499999999213 40.79486500000000149, -109.70055600000000595 40.80344499999999641, -109.71995699999999374 40.8018509999999992, -109.731544999999997 40.79442600000000141, -109.75249900000000025 40.80285099999999687, -109.76467800000000352 40.78253300000000081, -109.81623500000000604 40.77937299999999965, -109.8318790000000007 40.77573100000000039, -109.83413299999999424 40.76824200000000076, -109.87020699999999351 40.7638290000000012, -109.88306799999999441 40.77487999999999602, -109.8933799999999934 40.77291900000000169, -109.89682200000000023 40.78198400000000134, -109.91391400000000544 40.78244699999999767, -109.91866999999999166 40.79088499999999584, -109.92413799999999924 40.79001399999999933, -109.93220099999999206 40.7965859999999978, -109.95013600000000054 40.7980930000000015, -109.97004900000000305 40.81071199999999521, -109.9878620000000069 40.80761799999999795, -109.99366700000000208 40.81520000000000437, -110.00071099999999547 40.8136779999999959, -110.00071595432901006 40.99735263640130256)))</t>
+  </si>
+  <si>
+    <t>Daggett</t>
+  </si>
+  <si>
+    <t>46-49009</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((-114.05230583428699731 37.63631644109739938, -114.04847300000000132 37.80986099999999794, -114.04990337565800473 38.14876302667059349, -112.47867999999999711 38.1474189999999993, -112.47896500000000231 37.97767699999999991, -112.46696599999999933 37.97765899999999561, -112.46817699999999718 37.89046400000000148, -112.58840200000000209 37.89042299999999841, -112.58846800000000599 37.88220799999999855, -112.57839699999999539 37.88214699999999624, -112.578550000000007 37.80453999999999581, -112.68922100000000341 37.80558999999999514, -112.68375000000000341 37.54369200000000006, -112.90116199999999935 37.54348600000000147, -112.90099299999999971 37.50002099999999672, -113.03708799999999712 37.49974799999999675, -113.03704799999999864 37.47447400000000073, -113.14608400000000188 37.47429799999999744, -113.14610999999999308 37.4810279999999949, -113.25348999999999933 37.4821669999999969, -113.25333999999999435 37.52898299999999665, -113.47402900000000159 37.52908499999999492, -113.47448500000000138 37.6182889999999972, -113.58777299999999855 37.61822300000000041, -113.5877969999999948 37.60461099999999846, -114.05247199661400259 37.60477664271940057, -114.05230583428699731 37.63631644109739938)))</t>
+  </si>
+  <si>
+    <t>Iron</t>
+  </si>
+  <si>
+    <t>46-49021</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((-111.62072499999999309 40.45132199999999756, -111.60948399999999481 40.46632499999999766, -111.5948669999999936 40.46770799999999468, -111.57482899999999404 40.48712400000000144, -111.57912600000000225 40.50035599999999647, -111.57544300000000703 40.50318800000000152, -111.57542999999999722 40.51640700000000095, -111.56976600000000133 40.52683999999999997, -111.57260899999999992 40.53774500000000103, -111.56772499999999582 40.54721099999999723, -111.59394199999999842 40.57706599999999497, -111.56401400000000024 40.58491699999999724, -111.55421300000000429 40.60848899999999873, -111.53995999999999356 40.6132080000000002, -111.50049400000000333 40.60609199999999674, -111.48926500000000317 40.59943799999999925, -111.48561100000000579 40.60182799999999759, -111.48262499999999875 40.60903799999999819, -111.48688400000000343 40.62084399999999818, -111.47418500000000563 40.63239199999999585, -111.4736910000000023 40.64309499999999531, -111.46379500000000462 40.644956999999998, -111.46040999999999599 40.65233999999999526, -111.45081299999999658 40.65347599999999773, -111.43036200000000235 40.66513099999999525, -111.43619099999999378 40.6741090000000014, -111.43663599999999292 40.68597599999999659, -111.41219200000000455 40.68115099999999984, -111.39931300000000647 40.69044399999999939, -111.39361300000000199 40.69035999999999831, -111.38870500000000163 40.67043599999999515, -111.39019799999999805 40.66064300000000031, -111.37638599999999656 40.64261299999999721, -111.37548099999999351 40.63311600000000112, -111.36862299999999948 40.62894399999999706, -111.36308700000000727 40.63080799999999471, -111.35002099999999814 40.62501100000000065, -111.3267189999999971 40.62312000000000012, -111.30326999999999771 40.60590399999999534, -111.29393400000000725 40.60810299999999984, -111.28554199999999241 40.59702099999999803, -111.2527199999999965 40.58184299999999922, -111.21441400000000499 40.57458199999999948, -111.15135999999999683 40.54835200000000128, -111.1370589999999936 40.55839399999999983, -111.13331300000000113 40.57498400000000061, -111.12086999999999648 40.59045700000000068, -111.0791059999999959 40.59455099999999561, -111.05533900000000358 40.58170199999999994, -111.03116900000000555 40.57596199999999698, -111.02236399999999605 40.5792549999999963, -111.01049799999999834 40.59207099999999713, -110.97576100000000565 40.59314299999999776, -110.96255999999999631 40.60493199999999803, -110.9606990000000053 40.62420600000000093, -110.94498799999999505 40.6464769999999973, -110.94882300000000441 40.661330999999997, -110.94443099999999447 40.67260399999999976, -110.93352500000000305 40.68033599999999694, -110.90194999999999936 40.68218699999999899, -110.90292800000000284 40.43121099999999757, -110.89659199999999828 40.43118299999999721, -110.89627000000000123 40.08238399999999757, -110.89178900000000283 40.08240099999999728, -110.89164900000000102 39.8991449999999972, -111.08245499999999595 39.90015499999999804, -111.08306100000000072 39.94319799999999532, -111.11842199999999536 39.94348399999999799, -111.13129599999999186 39.94739599999999768, -111.1202210000000008 39.95707699999999818, -111.11927099999999768 39.96815600000000046, -111.12934599999999818 39.97037399999999963, -111.14304699999999571 39.98698799999999665, -111.15219600000000355 39.98505899999999968, -111.16014400000000251 39.99197399999999902, -111.16766400000000203 39.99058999999999742, -111.1715549999999979 40.01058499999999896, -111.18608000000000402 40.0196550000000002, -111.19186000000000547 40.03013699999999631, -111.19770800000000577 40.03117900000000162, -111.2038299999999964 40.04929800000000029, -111.22670499999999549 40.03569299999999487, -111.23823099999999897 40.03873399999999805, -111.24620699999999829 40.04746600000000001, -111.24922700000000475 40.05559499999999673, -111.23605799999999988 40.06911300000000153, -111.24069299999999316 40.07350299999999521, -111.23800699999999608 40.08055099999999982, -111.24236100000000249 40.08589299999999866, -111.24141500000000349 40.09189599999999842, -111.22141299999999831 40.12502999999999531, -111.22485600000000261 40.14251199999999642, -111.23116500000000428 40.14748099999999909, -111.22522499999999468 40.16636700000000104, -111.24790199999999629 40.19372699999999554, -111.25815500000000213 40.19784899999999794, -111.25640599999999836 40.20072700000000054, -111.26478099999999927 40.20949499999999688, -111.26186900000000435 40.21097799999999722, -111.27201700000000528 40.2194329999999951, -111.27361700000000155 40.2362150000000014, -111.26810199999999895 40.23693199999999592, -111.26478600000000085 40.24232800000000054, -111.2787620000000004 40.25879299999999716, -111.29417399999999816 40.26546899999999596, -111.29759900000000528 40.27296299999999718, -111.30789699999999698 40.2745000000000033, -111.30707800000000418 40.28264899999999926, -111.31483000000000061 40.28756599999999821, -111.32754400000000317 40.28213499999999669, -111.33956200000000081 40.28865499999999855, -111.36075300000000254 40.28872700000000151, -111.37715599999999938 40.29748699999999673, -111.38142700000000218 40.29444099999999906, -111.39212499999999295 40.29620399999999592, -111.39664500000000658 40.29230400000000145, -111.41036300000000381 40.29511099999999857, -111.41267700000000218 40.28955200000000048, -111.42648199999999292 40.28690599999999478, -111.43368599999999446 40.2919029999999978, -111.44344800000000362 40.28988199999999864, -111.45163300000000106 40.29316800000000143, -111.45719300000000374 40.30074099999999504, -111.43790599999999813 40.32177199999999573, -111.45329499999999712 40.33426699999999698, -111.45315300000000036 40.34028399999999692, -111.4624639999999971 40.34033900000000017, -111.46228100000000438 40.34748400000000146, -111.47157799999999384 40.34758399999999767, -111.47585800000000233 40.35486499999999666, -111.48053600000000074 40.35495699999999886, -111.48033699999999158 40.36216900000000152, -111.55523499999999615 40.36269599999999969, -111.55528400000000033 40.3699009999999987, -111.56019499999999312 40.36983699999999686, -111.56009699999999896 40.38776999999999617, -111.57420899999999619 40.39137300000000153, -111.57426800000000355 40.41290699999999703, -111.5836749999999995 40.41284499999999724, -111.58380300000000318 40.42021099999999478, -111.58836900000000014 40.4213009999999997, -111.5952609999999936 40.43261299999999636, -111.61173399999999845 40.43146600000000035, -111.61732899999999802 40.43768800000000141, -111.61582199999999432 40.44414599999999638, -111.62072499999999309 40.45132199999999756)))</t>
+  </si>
+  <si>
+    <t>Wasatch</t>
+  </si>
+  <si>
+    <t>46-49051</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((-111.8487609999999961 38.42493299999999579, -111.83756700000000706 38.42850099999999713, -111.823568999999992 38.45721799999999746, -111.75630200000000514 38.51014699999999635, -111.30566500000000474 38.51016899999999765, -111.30570099999999911 38.49999799999999794, -110.0254019999999997 38.49998099999999823, -110.00194000000000472 38.48101599999999678, -110.00437999999999761 38.46848200000000162, -110.01157399999999598 38.45878299999999683, -110.01104999999999734 38.44907399999999598, -110.02057100000000389 38.44705099999999476, -110.03449499999999261 38.45991300000000024, -110.04234499999999741 38.45718399999999804, -110.04435999999999751 38.45101400000000069, -110.04106699999999819 38.4467250000000007, -110.0269569999999959 38.44736999999999938, -110.00298100000000545 38.41448199999999957, -110.03310500000000616 38.39080200000000076, -110.03197299999999359 38.38495699999999999, -110.00983899999999949 38.37736199999999798, -110.01505600000000129 38.366537000000001, -110.01105300000000398 38.36442399999999964, -109.98425600000000202 38.38843599999999867, -109.97596899999999209 38.38830399999999798, -109.97299100000000749 38.37590900000000005, -109.98623399999999606 38.35942000000000007, -109.98290500000000236 38.35149299999999783, -109.96399399999999957 38.33973599999999493, -109.95462999999999454 38.34491599999999778, -109.9524459999999948 38.35434000000000054, -109.94124700000000416 38.35357199999999978, -109.94724499999999523 38.33923899999999918, -109.964224999999999 38.33261699999999905, -109.96367800000000159 38.32061199999999701, -109.94678600000000301 38.3096479999999957, -109.95047700000000646 38.29450699999999586, -109.94789600000000007 38.28906599999999827, -109.93197299999999927 38.28425299999999964, -109.92790899999999965 38.27928899999999857, -109.93596999999999753 38.26567999999999614, -109.93377800000000377 38.26165900000000164, -109.92639900000000353 38.26001300000000072, -109.90889099999999701 38.27125699999999853, -109.90438500000000488 38.2670180000000002, -109.90220600000000672 38.25595699999999511, -109.91843099999999822 38.24283099999999536, -109.912304000000006 38.23859799999999609, -109.89933399999999608 38.24260199999999799, -109.88899700000000337 38.22866799999999898, -109.91121599999999603 38.228158999999998, -109.92022500000000207 38.22189300000000145, -109.91220199999999352 38.21250599999999764, -109.89890800000000581 38.20683999999999969, -109.88801200000000335 38.20748299999999631, -109.90335000000000321 38.19293199999999899, -109.90289500000000089 38.18861899999999565, -109.88512400000000468 38.18849399999999861, -109.88845100000000343 38.18219200000000058, -109.90244300000000521 38.17894899999999581, -109.931122000000002 38.1580499999999958, -109.92799499999999568 38.15188399999999547, -111.41402999999999679 38.15398199999999918, -111.41415100000000393 38.15006100000000089, -111.84321500000000071 38.15127999999999986, -111.8487609999999961 38.42493299999999579)))</t>
+  </si>
+  <si>
+    <t>Wayne</t>
+  </si>
+  <si>
+    <t>46-49055</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((-114.04988334784700044 38.67736500000000177, -114.04772798183900306 39.54274080232679722, -113.81576599999999644 39.54408999999999708, -113.81574299999999766 39.5526440000000008, -112.21204500000000337 39.55398699999999934, -112.21202900000000113 39.54773000000000138, -112.20735299999999768 39.54769599999999485, -112.20266599999999357 39.54043399999999764, -112.19329199999999958 39.54045099999999735, -112.19324199999999792 39.52602299999999502, -112.21197300000000041 39.52604199999999679, -112.21196100000000229 39.51157899999999756, -112.20728499999999883 39.51156599999999486, -112.20730000000000359 39.50433400000000006, -112.20263299999999163 39.50432299999999941, -112.20262599999999509 39.48985799999999813, -112.19327699999999481 39.48983399999999477, -112.19359599999999944 39.3730899999999977, -112.18890700000000038 39.37308900000000023, -112.18892200000000514 39.32939199999999857, -112.07210800000000006 39.32969500000000096, -112.07221799999999234 39.31492300000000029, -112.01600299999999777 39.31456099999999765, -112.01401699999999551 39.02428199999999947, -112.01903400000000488 39.02420699999999698, -112.0189060000000012 38.99590200000000095, -112.05638700000000085 38.99568000000000012, -112.05640200000000561 38.98836800000000125, -112.06566100000000574 38.98843000000000103, -112.06516200000000083 38.95930200000000099, -112.13386199999999349 38.95930200000000099, -112.13403099999999313 38.93545299999999543, -112.15192799999999806 38.93547300000000178, -112.15076000000000533 38.90650899999999979, -112.16935100000000602 38.90613199999999949, -112.17155400000000043 38.87861600000000095, -112.18846999999999525 38.87944699999999898, -112.18854100000000074 38.86478699999999975, -112.22446100000000513 38.86480299999999488, -112.22463700000000131 38.83751399999999876, -112.22843799999999703 38.8375079999999997, -112.22838099999999883 38.76398700000000019, -112.21911799999999459 38.76398700000000019, -112.21835599999999999 38.72736099999999482, -112.23663999999999419 38.72710399999999709, -112.24146999999999252 38.71252399999999483, -112.25535899999999856 38.71230599999999811, -112.25543799999999806 38.70504700000000042, -112.28234999999999388 38.70152699999999868, -112.28225999999999374 38.68687399999999599, -112.30993999999999744 38.68340999999999497, -112.30995300000000725 38.67629000000000161, -112.35663700000000631 38.67673999999999523, -112.35653899999999794 38.68385500000000121, -112.36596400000000529 38.68421800000000133, -112.44751700000000483 38.68126999999999782, -112.4476669999999956 38.67392299999999494, -112.46600100000000566 38.67391699999999588, -112.46615599999999802 38.65926699999999983, -112.47534100000000024 38.65925699999999665, -112.47518499999999619 38.64467499999999944, -112.48444399999999632 38.64464699999999908, -112.48478799999999467 38.60063199999999739, -112.50307399999999802 38.60056799999999555, -112.50314799999999593 38.57137699999999825, -114.05015385887999457 38.57297445830089799, -114.04988334784700044 38.67736500000000177)))</t>
+  </si>
+  <si>
+    <t>Millard</t>
+  </si>
+  <si>
+    <t>46-49027</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((-112.01581199999999683 39.33686300000000102, -111.95810600000000079 39.33684600000000131, -111.95877299999999366 39.36613299999999782, -111.92169799999999213 39.36686199999999758, -111.92238899999999546 39.38159100000000024, -111.74704400000000248 39.38275000000000148, -111.74773600000000329 39.46007699999999829, -111.71322399999999675 39.46029399999999754, -111.71748200000000395 39.69455999999999563, -111.68948100000000068 39.69523099999999971, -111.68959599999999455 39.71036000000000143, -111.68026899999999557 39.71019599999999627, -111.68035899999999572 39.71746499999999713, -111.6613619999999969 39.7176550000000006, -111.6613490000000013 39.72505799999999709, -111.64261899999999628 39.72516199999999742, -111.64251899999999296 39.73969299999999549, -111.58475400000000377 39.74014100000000127, -111.58485799999999699 39.78423499999999535, -111.62251399999999535 39.78381600000000162, -111.62212300000000198 39.79848299999999739, -111.6420569999999941 39.79831399999999775, -111.64194399999999519 39.81286899999999918, -111.24749599999999816 39.81302799999999564, -111.24774800000000141 39.46719900000000081, -111.3009050000000002 39.46723699999999724, -111.29936000000000718 39.03226399999999785, -111.85340200000000266 39.03336799999999585, -111.85322499999999479 39.0406459999999953, -111.84686100000000408 39.04193599999999975, -111.84988599999999792 39.04557700000000153, -112.0140829999999994 39.04551800000000128, -112.01581199999999683 39.33686300000000102)))</t>
+  </si>
+  <si>
+    <t>Sanpete</t>
+  </si>
+  <si>
+    <t>46-49039</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((-114.05296199999999374 37.59278299999999717, -114.05247199661400259 37.60477664271940057, -113.5877969999999948 37.60461099999999846, -113.58777299999999855 37.61822300000000041, -113.47448500000000138 37.6182889999999972, -113.47402900000000159 37.52908499999999492, -113.25333999999999435 37.52898299999999665, -113.25348999999999933 37.4821669999999969, -113.14610999999999308 37.4810279999999949, -113.14608400000000188 37.47429799999999744, -113.03704799999999864 37.47447400000000073, -113.03708799999999712 37.49974799999999675, -112.90099299999999971 37.50002099999999672, -112.8991909022780078 37.00031972661560076, -114.05060000000000286 37.00039599999999496, -114.05296199999999374 37.59278299999999717)))</t>
+  </si>
+  <si>
+    <t>Washington</t>
+  </si>
+  <si>
+    <t>46-49053</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((-111.41278398787299864 37.00147768715600449, -111.40290500000000407 37.00514899999999585, -111.36749700000000018 37.00212099999999538, -111.344333000000006 37.00896600000000092, -111.32862699999999734 37.02101799999999798, -111.31485599999999181 37.01213299999999862, -111.30627599999999688 37.01236699999999757, -111.30374100000000226 37.01781799999999834, -111.30728999999999473 37.02497299999999569, -111.28153199999999856 37.04191499999999593, -111.30206200000000649 37.04559499999999872, -111.3058330000000069 37.05650699999999631, -111.30169700000000432 37.06641199999999969, -111.26776999999999873 37.05358499999999822, -111.25070700000000556 37.02510799999999591, -111.24177399999999238 37.02083899999999517, -111.22993999999999915 37.03856899999999541, -111.23207600000000639 37.04261999999999944, -111.24733200000000011 37.04769499999999738, -111.24087600000000009 37.06707199999999602, -111.23319499999999493 37.06968399999999519, -111.22587000000000046 37.05728799999999978, -111.21666600000000358 37.05756699999999881, -111.1783489999999972 37.10261299999999807, -111.16684800000000166 37.10596799999999718, -111.14960600000000568 37.09023499999999984, -111.13790699999999845 37.08863999999999805, -111.12093799999999533 37.10804100000000005, -111.10197300000000098 37.10285499999999814, -111.07794300000000476 37.10268800000000056, -111.06563599999999781 37.10797199999999663, -111.05767000000000166 37.09939500000000123, -111.05149000000000115 37.09908599999999979, -111.04270999999999958 37.10759900000000044, -111.01369400000000098 37.11568099999999504, -110.98870399999999847 37.11169299999999538, -110.9813039999999944 37.1164929999999984, -110.98466299999999762 37.12499299999999636, -110.98081100000000276 37.12799700000000058, -110.9583329999999961 37.12443799999999783, -110.95066400000000328 37.13496899999999812, -110.95488799999999685 37.15142199999999661, -110.94290999999999769 37.14827899999999516, -110.93343199999999626 37.15060499999999877, -110.92186800000000346 37.17860599999999494, -110.89951700000000301 37.17615299999999934, -110.89900699999999745 37.18689700000000187, -110.88868100000000538 37.20026199999999506, -110.89621499999999799 37.21475399999999922, -110.87527299999999286 37.229065999999996, -110.88695400000000291 37.24999199999999888, -110.8649029999999982 37.2564920000000015, -110.86050299999999424 37.26199199999999934, -110.87350299999999947 37.27719099999999486, -110.87370400000000359 37.28699199999999792, -110.84540200000000709 37.29349200000000053, -110.83720200000000489 37.29929200000000122, -110.84060200000000407 37.31879199999999486, -110.86760400000000004 37.32849099999999964, -110.87370400000000359 37.34029100000000057, -110.87210400000000732 37.34649100000000033, -110.86550400000000138 37.35039099999999479, -110.85470300000000066 37.34779100000000085, -110.80070000000000618 37.32129199999999969, -110.77529900000000396 37.3236920000000012, -110.76919900000000041 37.33159200000000055, -110.75809800000000394 37.33359199999999589, -110.7536970000000025 37.35139199999999704, -110.74839799999999457 37.35139199999999704, -110.74219800000000191 37.34439199999999914, -110.73609799999999836 37.34519199999999728, -110.73589799999999173 37.35739199999999727, -110.72539700000000096 37.36569199999999569, -110.72229699999999752 37.37319199999999597, -110.74059800000000564 37.38509200000000021, -110.7537980000000033 37.40399099999999777, -110.74499799999999539 37.40749100000000027, -110.72629799999999989 37.39989099999999667, -110.71739800000000287 37.40089100000000144, -110.70959700000000225 37.4076909999999998, -110.69919699999999807 37.43069099999999594, -110.70869799999999827 37.43739099999999809, -110.72549800000000175 37.43559099999999518, -110.74599899999999764 37.45269100000000151, -110.7474990000000048 37.45799099999999981, -110.72619799999999657 37.45949099999999987, -110.72599800000000414 37.46999100000000027, -110.71919800000000578 37.48139099999999502, -110.66629700000000014 37.47749100000000055, -110.64089699999999539 37.48519100000000037, -110.63889600000000257 37.48908999999999736, -110.64289600000000746 37.49209099999999495, -110.66729700000000491 37.49569100000000077, -110.66268200000000377 37.52112799999999737, -110.6362749999999977 37.554198999999997, -110.60360699999999667 37.57126399999999933, -110.59933800000000303 37.58165400000000034, -110.60101099999999974 37.60160199999999975, -110.56627699999999948 37.61587799999999504, -110.56307999999999936 37.63781199999999671, -110.5587369999999936 37.64200699999999955, -110.53805099999999584 37.63289699999999982, -110.5138769999999937 37.65663299999999936, -110.50159399999999721 37.64999999999999858, -110.49771099999999535 37.65220499999999504, -110.49431500000000028 37.66557900000000103, -110.48412199999999928 37.68168099999999754, -110.48340400000000727 37.69667400000000157, -110.48787699999999745 37.70218899999999707, -110.47006600000000276 37.71269499999999653, -110.46813000000000216 37.72477800000000059, -110.44728299999999876 37.73692799999999892, -110.44648200000000315 37.75856100000000026, -110.4266190000000023 37.77609999999999957, -110.43099700000000496 37.77890099999999762, -110.44151300000000049 37.77345799999999798, -110.46308399999999494 37.77193599999999662, -110.4705900000000014 37.78125199999999495, -110.47653499999999838 37.80084300000000042, -110.47031200000000695 37.80912199999999501, -110.43753800000000354 37.80691999999999808, -110.43124000000000251 37.83680899999999525, -110.40236000000000161 37.85223799999999983, -110.40461200000000019 37.87992299999999801, -110.38808600000000126 37.88790499999999639, -110.36414600000000519 37.89218499999999779, -110.30498000000000047 37.89051800000000014, -110.29493600000000697 37.88595399999999813, -110.29166800000000137 37.86961600000000061, -110.28435100000000091 37.86610599999999494, -110.27762199999999382 37.87118999999999858, -110.27621499999999344 37.89110000000000156, -110.26797600000000443 37.89828899999999834, -110.2106420000000071 37.89309199999999578, -110.20518500000000017 37.89735100000000045, -110.19846200000000636 37.91759499999999861, -110.20533199999999852 37.93128499999999548, -110.20238200000000006 37.94653600000000182, -110.16633899999999358 37.96630000000000393, -110.16215699999999345 37.98099099999999595, -110.14549300000000187 37.99062099999999731, -110.13669000000000153 38.00538600000000145, -110.11341000000000179 38.00829600000000141, -110.09454099999999244 37.99520599999999604, -110.07858400000000643 37.99817499999999626, -110.07274200000000519 38.00684100000000143, -110.0758560000000017 38.0230850000000018, -110.06387499999999591 38.04295099999999508, -110.04556200000000388 38.05030099999999749, -110.04321400000000608 38.06099100000000135, -110.04716100000000267 38.07057700000000011, -110.02666399999999669 38.09681399999999485, -110.01132799999999179 38.10927900000000079, -110.00375800000000481 38.10876700000000028, -109.9925049999999942 38.09994899999999518, -109.98504099999999539 38.10177999999999798, -109.97793400000000474 38.11010100000000023, -109.96481699999999648 38.11347099999999699, -109.95676600000000178 38.1294460000000015, -109.92937499999999318 38.13992100000000107, -109.92719400000000007 38.14796099999999512, -109.931122000000002 38.1580499999999958, -109.90244300000000521 38.17894899999999581, -109.88640100000000643 38.1843019999999953, -109.88726599999999678 38.19021399999999744, -109.90390800000000127 38.19019600000000025, -109.88801200000000335 38.20748299999999631, -109.89890800000000581 38.20683999999999969, -109.91220199999999352 38.21250599999999764, -109.92022500000000207 38.22189300000000145, -109.91121599999999603 38.228158999999998, -109.88899700000000337 38.22866799999999898, -109.89933399999999608 38.24260199999999799, -109.912304000000006 38.23859799999999609, -109.91843099999999822 38.24283099999999536, -109.90220600000000672 38.25595699999999511, -109.90438500000000488 38.2670180000000002, -109.90889099999999701 38.27125699999999853, -109.92639900000000353 38.26001300000000072, -109.93377800000000377 38.26165900000000164, -109.93596999999999753 38.26567999999999614, -109.92790899999999965 38.27928899999999857, -109.93197299999999927 38.28425299999999964, -109.94789600000000007 38.28906599999999827, -109.95047700000000646 38.29450699999999586, -109.94678600000000301 38.3096479999999957, -109.96367800000000159 38.32061199999999701, -109.964224999999999 38.33261699999999905, -109.94724499999999523 38.33923899999999918, -109.94124700000000416 38.35357199999999978, -109.9524459999999948 38.35434000000000054, -109.95462999999999454 38.34491599999999778, -109.96399399999999957 38.33973599999999493, -109.98290500000000236 38.35149299999999783, -109.98623399999999606 38.35942000000000007, -109.97299100000000749 38.37590900000000005, -109.97596899999999209 38.38830399999999798, -109.98425600000000202 38.38843599999999867, -110.01105300000000398 38.36442399999999964, -110.01505600000000129 38.366537000000001, -110.00983899999999949 38.37736199999999798, -110.03197299999999359 38.38495699999999999, -110.03310500000000616 38.39080200000000076, -110.00298100000000545 38.41448199999999957, -110.0269569999999959 38.44736999999999938, -110.04106699999999819 38.4467250000000007, -110.04435999999999751 38.45101400000000069, -110.04234499999999741 38.45718399999999804, -110.03449499999999261 38.45991300000000024, -110.02057100000000389 38.44705099999999476, -110.01104999999999734 38.44907399999999598, -110.01157399999999598 38.45878299999999683, -110.00437999999999761 38.46848200000000162, -110.00194000000000472 38.48101599999999678, -110.0254019999999997 38.49998099999999823, -109.05996200594900358 38.49998903101420211, -109.06006200000000206 38.27548900000000032, -109.04176200000000563 38.16469000000000023, -109.04522299999999291 36.99908399999999631, -110.47019000000000233 36.99799699999999802, -110.50068999999999164 37.00425999999999505, -111.41278398787299864 37.00147768715600449)))</t>
+  </si>
+  <si>
+    <t>San Juan</t>
+  </si>
+  <si>
+    <t>46-49037</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((-112.52253899999999476 38.52134399999999914, -112.51580300000000534 38.53061699999999945, -112.51842100000000357 38.56770199999999704, -112.51539400000000057 38.57284500000000094, -112.50314799999999593 38.57137699999999825, -112.50307399999999802 38.60056799999999555, -112.48478799999999467 38.60063199999999739, -112.48444399999999632 38.64464699999999908, -112.47518499999999619 38.64467499999999944, -112.47534100000000024 38.65925699999999665, -112.46615599999999802 38.65926699999999983, -112.46600100000000566 38.67391699999999588, -112.4476669999999956 38.67392299999999494, -112.44751700000000483 38.68126999999999782, -112.36596400000000529 38.68421800000000133, -112.35653899999999794 38.68385500000000121, -112.35663700000000631 38.67673999999999523, -112.30995300000000725 38.67629000000000161, -112.30993999999999744 38.68340999999999497, -112.28225999999999374 38.68687399999999599, -112.28234999999999388 38.70152699999999868, -112.25543799999999806 38.70504700000000042, -112.25535899999999856 38.71230599999999811, -112.24146999999999252 38.71252399999999483, -112.23663999999999419 38.72710399999999709, -112.21835599999999999 38.72736099999999482, -112.21911799999999459 38.76398700000000019, -112.22838099999999883 38.76398700000000019, -112.22843799999999703 38.8375079999999997, -112.22463700000000131 38.83751399999999876, -112.22446100000000513 38.86480299999999488, -112.18854100000000074 38.86478699999999975, -112.18846999999999525 38.87944699999999898, -112.17155400000000043 38.87861600000000095, -112.16935100000000602 38.90613199999999949, -112.15076000000000533 38.90650899999999979, -112.15192799999999806 38.93547300000000178, -112.13403099999999313 38.93545299999999543, -112.13386199999999349 38.95930200000000099, -112.06516200000000083 38.95930200000000099, -112.06566100000000574 38.98843000000000103, -112.05640200000000561 38.98836800000000125, -112.05638700000000085 38.99568000000000012, -112.0189060000000012 38.99590200000000095, -112.01903400000000488 39.02420699999999698, -112.01401699999999551 39.02428199999999947, -112.0140829999999994 39.04551800000000128, -111.84988599999999792 39.04557700000000153, -111.84686100000000408 39.04193599999999975, -111.85322499999999479 39.0406459999999953, -111.85340200000000266 39.03336799999999585, -111.29936000000000718 39.03226399999999785, -111.29913799999999924 38.67232899999999773, -111.30701100000000281 38.67233099999999979, -111.30566500000000474 38.51016899999999765, -111.75630200000000514 38.51014699999999635, -111.76639299999999366 38.50224299999999999, -112.06196500000000071 38.50208999999999548, -112.06213200000000541 38.51046999999999798, -112.51849500000000148 38.51041299999999978, -112.52253899999999476 38.52134399999999914)))</t>
+  </si>
+  <si>
+    <t>Sevier</t>
+  </si>
+  <si>
+    <t>46-49041</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((-112.45162100000000294 41.08733399999999847, -112.18653999999999371 41.15302700000000158, -111.97100399999999354 41.15264699999999465, -111.94948899999999981 41.13807299999999856, -111.92090899999999465 41.13866999999999763, -111.91075499999999465 41.13457499999999811, -111.85624699999999621 41.1390829999999994, -111.84900600000000281 41.13375800000000027, -111.84455099999999561 41.12178799999999512, -111.85611500000000262 41.11191099999999921, -111.85650400000000104 41.10288200000000103, -111.85176199999999369 41.097687999999998, -111.85512699999999597 41.09271799999999786, -111.84835999999999956 41.07573899999999867, -111.85179600000000733 41.06665100000000024, -111.84442699999999604 41.05886199999999775, -111.83944300000000283 41.04064899999999483, -111.8336879999999951 41.03701199999999716, -111.83939800000000275 41.03137199999999751, -111.8383879999999948 41.02348399999999629, -111.82569900000000018 41.01849899999999849, -111.81997799999999188 41.00645199999999591, -111.80612600000000612 41.00168499999999483, -111.77504100000000165 40.95931600000000117, -111.78253300000000081 40.95679799999999915, -111.79075600000000179 40.96085300000000018, -111.80769599999999286 40.95741199999999793, -111.81391200000000197 40.9599669999999989, -111.81529799999999852 40.95717899999999645, -111.79081499999999494 40.9277930000000012, -111.79347199999999418 40.91586099999999959, -111.7815920000000034 40.91136900000000054, -111.77602400000000671 40.90013700000000085, -111.78169599999999662 40.89604099999999676, -111.76176699999999187 40.88737299999999664, -111.76829499999999484 40.87253299999999712, -111.74699300000000335 40.87117699999999587, -111.73874399999999696 40.86099799999999505, -111.77853100000000097 40.84457700000000102, -111.78922500000000184 40.84555399999999992, -111.80438700000000551 40.83835099999999585, -111.81261600000000556 40.84008999999999645, -111.8221279999999922 40.83423499999999962, -111.8440389999999951 40.83223499999999717, -111.87089500000000442 40.82170199999999483, -111.94586300000000278 40.8217909999999975, -111.94428700000000276 40.83415399999999806, -111.95587199999999939 40.84911199999999809, -111.9630030000000005 40.84816999999999609, -111.95889800000000491 40.84924499999999625, -111.96587599999999441 40.85462599999999611, -111.96289199999999653 40.87000400000000155, -111.97106899999999996 40.87664499999999634, -111.96614700000000653 40.89165299999999803, -111.95926599999999951 40.89632699999999943, -111.95867200000000707 40.92182199999999881, -112.0065659999999923 40.92184599999999506, -112.14827099999999405 40.84613299999999469, -112.26021599999999978 40.76909299999999803, -112.49351500000000215 41.07688799999999674, -112.45162100000000294 41.08733399999999847)))</t>
+  </si>
+  <si>
+    <t>Davis</t>
+  </si>
+  <si>
+    <t>46-49011</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((-112.51898199999999406 38.48124800000000079, -112.51010700000000497 38.48877499999999685, -112.51882200000000012 38.50002899999999784, -112.51433900000000676 38.50253000000000014, -112.51849500000000148 38.51041299999999978, -112.20525999999999556 38.51217499999999916, -112.06213200000000541 38.51046999999999798, -112.06196500000000071 38.50208999999999548, -111.76639299999999366 38.50224299999999999, -111.823568999999992 38.45721799999999746, -111.83756700000000706 38.42850099999999713, -111.8487609999999961 38.42493299999999579, -111.84321500000000071 38.15127999999999986, -111.95144899999999666 38.15108299999999986, -111.95134899999999334 38.14598300000000108, -112.44421400000000233 38.15000099999999605, -112.43289699999999698 38.15404799999999597, -112.43491000000000213 38.16359399999999624, -112.42245400000000188 38.17082399999999609, -112.42274100000000203 38.18319899999999478, -112.41052700000000186 38.1885690000000011, -112.39505400000000179 38.20598400000000083, -112.36493000000000109 38.21512099999999634, -112.35720499999999333 38.22505100000000056, -112.37115299999999252 38.23451000000000022, -112.38083299999999554 38.25061699999999831, -112.35069799999999418 38.28179799999999489, -112.34708899999999687 38.29100000000000392, -112.34847600000000511 38.30514199999999647, -112.33874099999999885 38.31240000000000379, -112.34082100000000537 38.3255229999999969, -112.33544200000000046 38.33303799999999484, -112.34348500000000115 38.34726699999999511, -112.36263700000000654 38.35681399999999996, -112.37435999999999581 38.37727299999999531, -112.39158899999999619 38.38069199999999626, -112.39807000000000414 38.38654100000000113, -112.40379500000000235 38.39475699999999847, -112.40386300000000119 38.40045299999999884, -112.39765599999999779 38.40487600000000157, -112.40303400000000522 38.41560099999999522, -112.41678699999999935 38.41956899999999564, -112.4209419999999966 38.41121899999999556, -112.4336449999999985 38.40198099999999926, -112.44443300000000363 38.40604799999999841, -112.45301100000000361 38.42923199999999895, -112.47922900000000368 38.44804899999999748, -112.4933809999999994 38.45162499999999994, -112.50114200000000153 38.46536100000000147, -112.50991999999999393 38.46773499999999757, -112.51898199999999406 38.48124800000000079)))</t>
+  </si>
+  <si>
+    <t>46-49031</t>
   </si>
 </sst>
 </file>
@@ -3639,8 +3895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F823377-7D9E-4E85-B9A7-47A78B7D77FD}">
   <dimension ref="A1:D329"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView topLeftCell="A150" workbookViewId="0">
+      <selection activeCell="D179" sqref="D179:D246"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8262,10 +8518,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B565AF2A-F6C0-42A0-8263-1A7BA6114327}">
-  <dimension ref="A1:D241"/>
+  <dimension ref="A1:D121"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:XFD150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8292,3383 +8548,2137 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>391</v>
       </c>
       <c r="B2" t="s">
         <v>14</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>13</v>
-      </c>
+        <v>1066</v>
+      </c>
+      <c r="D2" s="4"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>1069</v>
       </c>
       <c r="B3" t="s">
         <v>14</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>1072</v>
       </c>
       <c r="B4" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" t="s">
-        <v>19</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="B5" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" t="s">
-        <v>22</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>1077</v>
       </c>
       <c r="B6" t="s">
         <v>14</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" t="s">
-        <v>25</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>1080</v>
       </c>
       <c r="B7" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" t="s">
-        <v>28</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>1083</v>
       </c>
       <c r="B8" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" t="s">
-        <v>31</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" t="s">
-        <v>34</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>1088</v>
       </c>
       <c r="B10" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" t="s">
-        <v>37</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>1091</v>
       </c>
       <c r="B11" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" t="s">
-        <v>40</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>1094</v>
       </c>
       <c r="B12" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" t="s">
-        <v>43</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>1097</v>
       </c>
       <c r="B13" t="s">
         <v>14</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D13" t="s">
-        <v>46</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>48</v>
+        <v>1100</v>
       </c>
       <c r="B14" t="s">
         <v>14</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="D14" t="s">
-        <v>49</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>6</v>
+        <v>1103</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D15" t="s">
-        <v>51</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>53</v>
+        <v>1106</v>
       </c>
       <c r="B16" t="s">
         <v>14</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D16" t="s">
-        <v>54</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>1109</v>
       </c>
       <c r="B17" t="s">
         <v>14</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D17" t="s">
-        <v>57</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>59</v>
+        <v>1061</v>
       </c>
       <c r="B18" t="s">
         <v>14</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D18" t="s">
-        <v>60</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>62</v>
+        <v>1114</v>
       </c>
       <c r="B19" t="s">
         <v>14</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D19" t="s">
-        <v>63</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>65</v>
+        <v>1117</v>
       </c>
       <c r="B20" t="s">
         <v>14</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="D20" t="s">
-        <v>66</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>68</v>
+        <v>1120</v>
       </c>
       <c r="B21" t="s">
         <v>14</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D21" t="s">
-        <v>69</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>71</v>
+        <v>1123</v>
       </c>
       <c r="B22" t="s">
         <v>14</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D22" t="s">
-        <v>72</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>74</v>
+        <v>1126</v>
       </c>
       <c r="B23" t="s">
         <v>14</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D23" t="s">
-        <v>75</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>77</v>
+        <v>1129</v>
       </c>
       <c r="B24" t="s">
         <v>14</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="D24" t="s">
-        <v>78</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>80</v>
+        <v>1132</v>
       </c>
       <c r="B25" t="s">
         <v>14</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="D25" t="s">
-        <v>81</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>83</v>
+        <v>1135</v>
       </c>
       <c r="B26" t="s">
         <v>14</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="D26" t="s">
-        <v>84</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>86</v>
+        <v>1138</v>
       </c>
       <c r="B27" t="s">
         <v>14</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="D27" t="s">
-        <v>87</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>89</v>
+        <v>1141</v>
       </c>
       <c r="B28" t="s">
         <v>14</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="D28" t="s">
-        <v>90</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>7</v>
+        <v>1144</v>
       </c>
       <c r="B29" t="s">
         <v>14</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="D29" t="s">
-        <v>92</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>94</v>
+        <v>356</v>
       </c>
       <c r="B30" t="s">
         <v>14</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="D30" t="s">
-        <v>95</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>97</v>
+        <v>454</v>
       </c>
       <c r="B31" t="s">
-        <v>14</v>
+        <v>456</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>96</v>
+        <v>453</v>
       </c>
       <c r="D31" t="s">
-        <v>98</v>
+        <v>455</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>100</v>
+        <v>458</v>
       </c>
       <c r="B32" t="s">
-        <v>14</v>
+        <v>456</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>99</v>
+        <v>457</v>
       </c>
       <c r="D32" t="s">
-        <v>101</v>
+        <v>459</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>103</v>
+        <v>461</v>
       </c>
       <c r="B33" t="s">
-        <v>14</v>
+        <v>456</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>102</v>
+        <v>460</v>
       </c>
       <c r="D33" t="s">
-        <v>104</v>
+        <v>462</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>106</v>
+        <v>464</v>
       </c>
       <c r="B34" t="s">
-        <v>14</v>
+        <v>456</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>105</v>
+        <v>463</v>
       </c>
       <c r="D34" t="s">
-        <v>107</v>
+        <v>465</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>109</v>
+        <v>467</v>
       </c>
       <c r="B35" t="s">
-        <v>14</v>
+        <v>456</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>108</v>
+        <v>466</v>
       </c>
       <c r="D35" t="s">
-        <v>110</v>
+        <v>468</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>112</v>
+        <v>470</v>
       </c>
       <c r="B36" t="s">
-        <v>14</v>
+        <v>456</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>111</v>
+        <v>469</v>
       </c>
       <c r="D36" t="s">
-        <v>113</v>
+        <v>471</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>115</v>
+        <v>473</v>
       </c>
       <c r="B37" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>114</v>
+        <v>472</v>
       </c>
       <c r="D37" t="s">
-        <v>116</v>
+        <v>474</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>118</v>
+        <v>477</v>
       </c>
       <c r="B38" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>117</v>
+        <v>476</v>
       </c>
       <c r="D38" t="s">
-        <v>119</v>
+        <v>478</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>121</v>
+        <v>480</v>
       </c>
       <c r="B39" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>120</v>
+        <v>479</v>
       </c>
       <c r="D39" t="s">
-        <v>122</v>
+        <v>481</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>124</v>
+        <v>483</v>
       </c>
       <c r="B40" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>123</v>
+        <v>482</v>
       </c>
       <c r="D40" t="s">
-        <v>125</v>
+        <v>484</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>127</v>
+        <v>486</v>
       </c>
       <c r="B41" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>126</v>
+        <v>485</v>
       </c>
       <c r="D41" t="s">
-        <v>128</v>
+        <v>487</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>130</v>
+        <v>489</v>
       </c>
       <c r="B42" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>129</v>
+        <v>488</v>
       </c>
       <c r="D42" t="s">
-        <v>131</v>
+        <v>490</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>133</v>
+        <v>492</v>
       </c>
       <c r="B43" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>132</v>
+        <v>491</v>
       </c>
       <c r="D43" t="s">
-        <v>134</v>
+        <v>493</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>136</v>
+        <v>495</v>
       </c>
       <c r="B44" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>135</v>
+        <v>494</v>
       </c>
       <c r="D44" t="s">
-        <v>137</v>
+        <v>496</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>139</v>
+        <v>498</v>
       </c>
       <c r="B45" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>138</v>
+        <v>497</v>
       </c>
       <c r="D45" t="s">
-        <v>140</v>
+        <v>499</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>142</v>
+        <v>501</v>
       </c>
       <c r="B46" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>141</v>
+        <v>500</v>
       </c>
       <c r="D46" t="s">
-        <v>143</v>
+        <v>502</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>145</v>
+        <v>504</v>
       </c>
       <c r="B47" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>144</v>
+        <v>503</v>
       </c>
       <c r="D47" t="s">
-        <v>146</v>
+        <v>505</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>148</v>
+        <v>507</v>
       </c>
       <c r="B48" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>147</v>
+        <v>506</v>
       </c>
       <c r="D48" t="s">
-        <v>149</v>
+        <v>508</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>151</v>
+        <v>510</v>
       </c>
       <c r="B49" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>150</v>
+        <v>509</v>
       </c>
       <c r="D49" t="s">
-        <v>152</v>
+        <v>511</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>154</v>
+        <v>513</v>
       </c>
       <c r="B50" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>153</v>
+        <v>512</v>
       </c>
       <c r="D50" t="s">
-        <v>155</v>
+        <v>514</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>157</v>
+        <v>516</v>
       </c>
       <c r="B51" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>156</v>
+        <v>515</v>
       </c>
       <c r="D51" t="s">
-        <v>158</v>
+        <v>517</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>160</v>
+        <v>519</v>
       </c>
       <c r="B52" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>159</v>
+        <v>518</v>
       </c>
       <c r="D52" t="s">
-        <v>161</v>
+        <v>520</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>163</v>
+        <v>522</v>
       </c>
       <c r="B53" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>162</v>
+        <v>521</v>
       </c>
       <c r="D53" t="s">
-        <v>164</v>
+        <v>523</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>166</v>
+        <v>525</v>
       </c>
       <c r="B54" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>165</v>
+        <v>524</v>
       </c>
       <c r="D54" t="s">
-        <v>167</v>
+        <v>526</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>169</v>
+        <v>528</v>
       </c>
       <c r="B55" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>168</v>
+        <v>527</v>
       </c>
       <c r="D55" t="s">
-        <v>170</v>
+        <v>529</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>172</v>
+        <v>531</v>
       </c>
       <c r="B56" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>171</v>
+        <v>530</v>
       </c>
       <c r="D56" t="s">
-        <v>173</v>
+        <v>532</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>175</v>
+        <v>534</v>
       </c>
       <c r="B57" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>174</v>
+        <v>533</v>
       </c>
       <c r="D57" t="s">
-        <v>176</v>
+        <v>535</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>178</v>
+        <v>537</v>
       </c>
       <c r="B58" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>177</v>
+        <v>536</v>
       </c>
       <c r="D58" t="s">
-        <v>179</v>
+        <v>538</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>181</v>
+        <v>540</v>
       </c>
       <c r="B59" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>180</v>
+        <v>539</v>
       </c>
       <c r="D59" t="s">
-        <v>182</v>
+        <v>541</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>184</v>
+        <v>543</v>
       </c>
       <c r="B60" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>183</v>
+        <v>542</v>
       </c>
       <c r="D60" t="s">
-        <v>185</v>
+        <v>544</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>187</v>
+        <v>546</v>
       </c>
       <c r="B61" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>186</v>
+        <v>545</v>
       </c>
       <c r="D61" t="s">
-        <v>188</v>
+        <v>547</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>190</v>
+        <v>549</v>
       </c>
       <c r="B62" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>189</v>
+        <v>548</v>
       </c>
       <c r="D62" t="s">
-        <v>191</v>
+        <v>550</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>193</v>
+        <v>552</v>
       </c>
       <c r="B63" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>192</v>
+        <v>551</v>
       </c>
       <c r="D63" t="s">
-        <v>194</v>
+        <v>553</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>196</v>
+        <v>555</v>
       </c>
       <c r="B64" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>195</v>
+        <v>554</v>
       </c>
       <c r="D64" t="s">
-        <v>197</v>
+        <v>556</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>199</v>
+        <v>558</v>
       </c>
       <c r="B65" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>198</v>
+        <v>557</v>
       </c>
       <c r="D65" t="s">
-        <v>200</v>
+        <v>559</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>202</v>
+        <v>561</v>
       </c>
       <c r="B66" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>201</v>
+        <v>560</v>
       </c>
       <c r="D66" t="s">
-        <v>203</v>
+        <v>562</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>205</v>
+        <v>564</v>
       </c>
       <c r="B67" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>204</v>
+        <v>563</v>
       </c>
       <c r="D67" t="s">
-        <v>206</v>
+        <v>565</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>208</v>
+        <v>567</v>
       </c>
       <c r="B68" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>207</v>
+        <v>566</v>
       </c>
       <c r="D68" t="s">
-        <v>209</v>
+        <v>568</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>211</v>
+        <v>570</v>
       </c>
       <c r="B69" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>210</v>
+        <v>569</v>
       </c>
       <c r="D69" t="s">
-        <v>212</v>
+        <v>571</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>214</v>
+        <v>573</v>
       </c>
       <c r="B70" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>213</v>
+        <v>572</v>
       </c>
       <c r="D70" t="s">
-        <v>215</v>
+        <v>574</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>217</v>
+        <v>576</v>
       </c>
       <c r="B71" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>216</v>
+        <v>575</v>
       </c>
       <c r="D71" t="s">
-        <v>218</v>
+        <v>577</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>220</v>
+        <v>579</v>
       </c>
       <c r="B72" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>219</v>
+        <v>578</v>
       </c>
       <c r="D72" t="s">
-        <v>221</v>
+        <v>580</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>223</v>
+        <v>582</v>
       </c>
       <c r="B73" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>222</v>
+        <v>581</v>
       </c>
       <c r="D73" t="s">
-        <v>224</v>
+        <v>583</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>226</v>
+        <v>585</v>
       </c>
       <c r="B74" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>225</v>
+        <v>584</v>
       </c>
       <c r="D74" t="s">
-        <v>227</v>
+        <v>586</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>2</v>
+        <v>588</v>
       </c>
       <c r="B75" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>228</v>
+        <v>587</v>
       </c>
       <c r="D75" t="s">
-        <v>229</v>
+        <v>589</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>231</v>
+        <v>591</v>
       </c>
       <c r="B76" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>230</v>
+        <v>590</v>
       </c>
       <c r="D76" t="s">
-        <v>232</v>
+        <v>592</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>234</v>
+        <v>594</v>
       </c>
       <c r="B77" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>233</v>
+        <v>593</v>
       </c>
       <c r="D77" t="s">
-        <v>235</v>
+        <v>595</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>237</v>
+        <v>597</v>
       </c>
       <c r="B78" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>236</v>
+        <v>596</v>
       </c>
       <c r="D78" t="s">
-        <v>238</v>
+        <v>598</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>240</v>
+        <v>600</v>
       </c>
       <c r="B79" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>239</v>
+        <v>599</v>
       </c>
       <c r="D79" t="s">
-        <v>241</v>
+        <v>601</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>243</v>
+        <v>603</v>
       </c>
       <c r="B80" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>242</v>
+        <v>602</v>
       </c>
       <c r="D80" t="s">
-        <v>244</v>
+        <v>604</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>246</v>
+        <v>606</v>
       </c>
       <c r="B81" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>245</v>
+        <v>605</v>
       </c>
       <c r="D81" t="s">
-        <v>247</v>
+        <v>607</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>249</v>
+        <v>609</v>
       </c>
       <c r="B82" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>248</v>
+        <v>608</v>
       </c>
       <c r="D82" t="s">
-        <v>250</v>
+        <v>610</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>252</v>
+        <v>612</v>
       </c>
       <c r="B83" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>251</v>
+        <v>611</v>
       </c>
       <c r="D83" t="s">
-        <v>253</v>
+        <v>613</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>255</v>
+        <v>615</v>
       </c>
       <c r="B84" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>254</v>
+        <v>614</v>
       </c>
       <c r="D84" t="s">
-        <v>256</v>
+        <v>616</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>258</v>
+        <v>618</v>
       </c>
       <c r="B85" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>257</v>
+        <v>617</v>
       </c>
       <c r="D85" t="s">
-        <v>259</v>
+        <v>619</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>261</v>
+        <v>621</v>
       </c>
       <c r="B86" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>260</v>
+        <v>620</v>
       </c>
       <c r="D86" t="s">
-        <v>262</v>
+        <v>622</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>264</v>
+        <v>624</v>
       </c>
       <c r="B87" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>263</v>
+        <v>623</v>
       </c>
       <c r="D87" t="s">
-        <v>265</v>
+        <v>625</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>267</v>
+        <v>627</v>
       </c>
       <c r="B88" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C88" s="6" t="s">
-        <v>266</v>
+        <v>626</v>
       </c>
       <c r="D88" t="s">
-        <v>268</v>
+        <v>628</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>270</v>
+        <v>630</v>
       </c>
       <c r="B89" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>269</v>
+        <v>629</v>
       </c>
       <c r="D89" t="s">
-        <v>271</v>
+        <v>631</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>273</v>
+        <v>633</v>
       </c>
       <c r="B90" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>272</v>
+        <v>632</v>
       </c>
       <c r="D90" t="s">
-        <v>274</v>
+        <v>634</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>276</v>
+        <v>636</v>
       </c>
       <c r="B91" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>275</v>
+        <v>635</v>
       </c>
       <c r="D91" t="s">
-        <v>277</v>
+        <v>637</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>279</v>
+        <v>639</v>
       </c>
       <c r="B92" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>278</v>
+        <v>638</v>
       </c>
       <c r="D92" t="s">
-        <v>280</v>
+        <v>640</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>282</v>
+        <v>642</v>
       </c>
       <c r="B93" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C93" s="6" t="s">
-        <v>281</v>
+        <v>641</v>
       </c>
       <c r="D93" t="s">
-        <v>283</v>
+        <v>643</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>285</v>
+        <v>645</v>
       </c>
       <c r="B94" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C94" s="6" t="s">
-        <v>284</v>
+        <v>644</v>
       </c>
       <c r="D94" t="s">
-        <v>286</v>
+        <v>646</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>288</v>
+        <v>648</v>
       </c>
       <c r="B95" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C95" s="6" t="s">
-        <v>287</v>
+        <v>647</v>
       </c>
       <c r="D95" t="s">
-        <v>289</v>
+        <v>649</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>291</v>
+        <v>651</v>
       </c>
       <c r="B96" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C96" s="6" t="s">
-        <v>290</v>
+        <v>650</v>
       </c>
       <c r="D96" t="s">
-        <v>292</v>
+        <v>652</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>4</v>
+        <v>654</v>
       </c>
       <c r="B97" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C97" s="6" t="s">
-        <v>293</v>
+        <v>653</v>
       </c>
       <c r="D97" t="s">
-        <v>294</v>
+        <v>655</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>296</v>
+        <v>657</v>
       </c>
       <c r="B98" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C98" s="6" t="s">
-        <v>295</v>
+        <v>656</v>
       </c>
       <c r="D98" t="s">
-        <v>297</v>
+        <v>658</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>299</v>
+        <v>660</v>
       </c>
       <c r="B99" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>298</v>
+        <v>659</v>
       </c>
       <c r="D99" t="s">
-        <v>300</v>
+        <v>661</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>302</v>
+        <v>663</v>
       </c>
       <c r="B100" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>301</v>
+        <v>662</v>
       </c>
       <c r="D100" t="s">
-        <v>303</v>
+        <v>664</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>305</v>
+        <v>666</v>
       </c>
       <c r="B101" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C101" s="6" t="s">
-        <v>304</v>
+        <v>665</v>
       </c>
       <c r="D101" t="s">
-        <v>306</v>
+        <v>667</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>308</v>
+        <v>669</v>
       </c>
       <c r="B102" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C102" s="6" t="s">
-        <v>307</v>
+        <v>668</v>
       </c>
       <c r="D102" t="s">
-        <v>309</v>
+        <v>670</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>311</v>
+        <v>672</v>
       </c>
       <c r="B103" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C103" s="6" t="s">
-        <v>310</v>
+        <v>671</v>
       </c>
       <c r="D103" t="s">
-        <v>312</v>
+        <v>673</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>314</v>
+        <v>675</v>
       </c>
       <c r="B104" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C104" s="6" t="s">
-        <v>313</v>
+        <v>674</v>
       </c>
       <c r="D104" t="s">
-        <v>315</v>
+        <v>676</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>317</v>
+        <v>678</v>
       </c>
       <c r="B105" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C105" s="6" t="s">
-        <v>316</v>
+        <v>677</v>
       </c>
       <c r="D105" t="s">
-        <v>318</v>
+        <v>679</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>320</v>
+        <v>681</v>
       </c>
       <c r="B106" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C106" s="6" t="s">
-        <v>319</v>
+        <v>680</v>
       </c>
       <c r="D106" t="s">
-        <v>321</v>
+        <v>682</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>323</v>
+        <v>684</v>
       </c>
       <c r="B107" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C107" s="6" t="s">
-        <v>322</v>
+        <v>683</v>
       </c>
       <c r="D107" t="s">
-        <v>324</v>
+        <v>685</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>326</v>
+        <v>687</v>
       </c>
       <c r="B108" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C108" s="6" t="s">
-        <v>325</v>
+        <v>686</v>
       </c>
       <c r="D108" t="s">
-        <v>327</v>
+        <v>688</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>329</v>
+        <v>690</v>
       </c>
       <c r="B109" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C109" s="6" t="s">
-        <v>328</v>
+        <v>689</v>
       </c>
       <c r="D109" t="s">
-        <v>330</v>
+        <v>691</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>332</v>
+        <v>693</v>
       </c>
       <c r="B110" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C110" s="6" t="s">
-        <v>331</v>
+        <v>692</v>
       </c>
       <c r="D110" t="s">
-        <v>333</v>
+        <v>694</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>335</v>
+        <v>696</v>
       </c>
       <c r="B111" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C111" s="6" t="s">
-        <v>334</v>
+        <v>695</v>
       </c>
       <c r="D111" t="s">
-        <v>336</v>
+        <v>697</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>338</v>
+        <v>699</v>
       </c>
       <c r="B112" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C112" s="6" t="s">
-        <v>337</v>
+        <v>698</v>
       </c>
       <c r="D112" t="s">
-        <v>339</v>
+        <v>700</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>341</v>
+        <v>702</v>
       </c>
       <c r="B113" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C113" s="6" t="s">
-        <v>340</v>
+        <v>701</v>
       </c>
       <c r="D113" t="s">
-        <v>342</v>
+        <v>703</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>344</v>
+        <v>705</v>
       </c>
       <c r="B114" t="s">
-        <v>14</v>
+        <v>475</v>
       </c>
       <c r="C114" s="6" t="s">
-        <v>343</v>
+        <v>704</v>
       </c>
       <c r="D114" t="s">
-        <v>345</v>
+        <v>706</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>347</v>
+        <v>708</v>
       </c>
       <c r="B115" t="s">
-        <v>14</v>
+        <v>710</v>
       </c>
       <c r="C115" s="6" t="s">
-        <v>346</v>
+        <v>707</v>
       </c>
       <c r="D115" t="s">
-        <v>348</v>
+        <v>709</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>350</v>
+        <v>712</v>
       </c>
       <c r="B116" t="s">
-        <v>14</v>
+        <v>710</v>
       </c>
       <c r="C116" s="6" t="s">
-        <v>349</v>
+        <v>711</v>
       </c>
       <c r="D116" t="s">
-        <v>351</v>
+        <v>713</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>353</v>
+        <v>715</v>
       </c>
       <c r="B117" t="s">
-        <v>14</v>
+        <v>710</v>
       </c>
       <c r="C117" s="6" t="s">
-        <v>352</v>
+        <v>714</v>
       </c>
       <c r="D117" t="s">
-        <v>354</v>
+        <v>716</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>356</v>
+        <v>718</v>
       </c>
       <c r="B118" t="s">
-        <v>14</v>
+        <v>710</v>
       </c>
       <c r="C118" s="6" t="s">
-        <v>355</v>
+        <v>717</v>
       </c>
       <c r="D118" t="s">
-        <v>357</v>
+        <v>719</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>359</v>
+        <v>721</v>
       </c>
       <c r="B119" t="s">
-        <v>14</v>
+        <v>710</v>
       </c>
       <c r="C119" s="6" t="s">
-        <v>358</v>
+        <v>720</v>
       </c>
       <c r="D119" t="s">
-        <v>360</v>
+        <v>722</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>3</v>
+        <v>724</v>
       </c>
       <c r="B120" t="s">
-        <v>14</v>
+        <v>710</v>
       </c>
       <c r="C120" s="6" t="s">
-        <v>361</v>
+        <v>723</v>
       </c>
       <c r="D120" t="s">
-        <v>362</v>
+        <v>725</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>364</v>
+        <v>727</v>
       </c>
       <c r="B121" t="s">
-        <v>14</v>
+        <v>710</v>
       </c>
       <c r="C121" s="6" t="s">
-        <v>363</v>
+        <v>726</v>
       </c>
       <c r="D121" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>367</v>
-      </c>
-      <c r="B122" t="s">
-        <v>14</v>
-      </c>
-      <c r="C122" s="6" t="s">
-        <v>366</v>
-      </c>
-      <c r="D122" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>370</v>
-      </c>
-      <c r="B123" t="s">
-        <v>14</v>
-      </c>
-      <c r="C123" s="6" t="s">
-        <v>369</v>
-      </c>
-      <c r="D123" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>373</v>
-      </c>
-      <c r="B124" t="s">
-        <v>14</v>
-      </c>
-      <c r="C124" s="6" t="s">
-        <v>372</v>
-      </c>
-      <c r="D124" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
-        <v>376</v>
-      </c>
-      <c r="B125" t="s">
-        <v>14</v>
-      </c>
-      <c r="C125" s="6" t="s">
-        <v>375</v>
-      </c>
-      <c r="D125" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
-        <v>379</v>
-      </c>
-      <c r="B126" t="s">
-        <v>14</v>
-      </c>
-      <c r="C126" s="6" t="s">
-        <v>378</v>
-      </c>
-      <c r="D126" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
-        <v>382</v>
-      </c>
-      <c r="B127" t="s">
-        <v>14</v>
-      </c>
-      <c r="C127" s="6" t="s">
-        <v>381</v>
-      </c>
-      <c r="D127" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
-        <v>385</v>
-      </c>
-      <c r="B128" t="s">
-        <v>14</v>
-      </c>
-      <c r="C128" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="D128" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
-        <v>388</v>
-      </c>
-      <c r="B129" t="s">
-        <v>14</v>
-      </c>
-      <c r="C129" s="6" t="s">
-        <v>387</v>
-      </c>
-      <c r="D129" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
-        <v>391</v>
-      </c>
-      <c r="B130" t="s">
-        <v>14</v>
-      </c>
-      <c r="C130" s="6" t="s">
-        <v>390</v>
-      </c>
-      <c r="D130" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
-        <v>394</v>
-      </c>
-      <c r="B131" t="s">
-        <v>14</v>
-      </c>
-      <c r="C131" s="6" t="s">
-        <v>393</v>
-      </c>
-      <c r="D131" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
-        <v>397</v>
-      </c>
-      <c r="B132" t="s">
-        <v>14</v>
-      </c>
-      <c r="C132" s="6" t="s">
-        <v>396</v>
-      </c>
-      <c r="D132" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
-        <v>400</v>
-      </c>
-      <c r="B133" t="s">
-        <v>14</v>
-      </c>
-      <c r="C133" s="6" t="s">
-        <v>399</v>
-      </c>
-      <c r="D133" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
-        <v>403</v>
-      </c>
-      <c r="B134" t="s">
-        <v>14</v>
-      </c>
-      <c r="C134" s="6" t="s">
-        <v>402</v>
-      </c>
-      <c r="D134" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
-        <v>406</v>
-      </c>
-      <c r="B135" t="s">
-        <v>14</v>
-      </c>
-      <c r="C135" s="6" t="s">
-        <v>405</v>
-      </c>
-      <c r="D135" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
-        <v>409</v>
-      </c>
-      <c r="B136" t="s">
-        <v>14</v>
-      </c>
-      <c r="C136" s="6" t="s">
-        <v>408</v>
-      </c>
-      <c r="D136" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
-        <v>412</v>
-      </c>
-      <c r="B137" t="s">
-        <v>14</v>
-      </c>
-      <c r="C137" s="6" t="s">
-        <v>411</v>
-      </c>
-      <c r="D137" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
-        <v>415</v>
-      </c>
-      <c r="B138" t="s">
-        <v>14</v>
-      </c>
-      <c r="C138" s="6" t="s">
-        <v>414</v>
-      </c>
-      <c r="D138" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
-        <v>418</v>
-      </c>
-      <c r="B139" t="s">
-        <v>14</v>
-      </c>
-      <c r="C139" s="6" t="s">
-        <v>417</v>
-      </c>
-      <c r="D139" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
-        <v>421</v>
-      </c>
-      <c r="B140" t="s">
-        <v>14</v>
-      </c>
-      <c r="C140" s="6" t="s">
-        <v>420</v>
-      </c>
-      <c r="D140" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
-        <v>424</v>
-      </c>
-      <c r="B141" t="s">
-        <v>14</v>
-      </c>
-      <c r="C141" s="6" t="s">
-        <v>423</v>
-      </c>
-      <c r="D141" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
-        <v>427</v>
-      </c>
-      <c r="B142" t="s">
-        <v>14</v>
-      </c>
-      <c r="C142" s="6" t="s">
-        <v>426</v>
-      </c>
-      <c r="D142" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
-        <v>430</v>
-      </c>
-      <c r="B143" t="s">
-        <v>14</v>
-      </c>
-      <c r="C143" s="6" t="s">
-        <v>429</v>
-      </c>
-      <c r="D143" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
-        <v>433</v>
-      </c>
-      <c r="B144" t="s">
-        <v>14</v>
-      </c>
-      <c r="C144" s="6" t="s">
-        <v>432</v>
-      </c>
-      <c r="D144" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
-        <v>436</v>
-      </c>
-      <c r="B145" t="s">
-        <v>14</v>
-      </c>
-      <c r="C145" s="6" t="s">
-        <v>435</v>
-      </c>
-      <c r="D145" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
-        <v>439</v>
-      </c>
-      <c r="B146" t="s">
-        <v>14</v>
-      </c>
-      <c r="C146" s="6" t="s">
-        <v>438</v>
-      </c>
-      <c r="D146" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
-        <v>442</v>
-      </c>
-      <c r="B147" t="s">
-        <v>14</v>
-      </c>
-      <c r="C147" s="6" t="s">
-        <v>441</v>
-      </c>
-      <c r="D147" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
-        <v>445</v>
-      </c>
-      <c r="B148" t="s">
-        <v>14</v>
-      </c>
-      <c r="C148" s="6" t="s">
-        <v>444</v>
-      </c>
-      <c r="D148" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
-        <v>448</v>
-      </c>
-      <c r="B149" t="s">
-        <v>14</v>
-      </c>
-      <c r="C149" s="6" t="s">
-        <v>447</v>
-      </c>
-      <c r="D149" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
-        <v>451</v>
-      </c>
-      <c r="B150" t="s">
-        <v>14</v>
-      </c>
-      <c r="C150" s="6" t="s">
-        <v>450</v>
-      </c>
-      <c r="D150" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
-        <v>454</v>
-      </c>
-      <c r="B151" t="s">
-        <v>456</v>
-      </c>
-      <c r="C151" s="6" t="s">
-        <v>453</v>
-      </c>
-      <c r="D151" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A152" t="s">
-        <v>458</v>
-      </c>
-      <c r="B152" t="s">
-        <v>456</v>
-      </c>
-      <c r="C152" s="6" t="s">
-        <v>457</v>
-      </c>
-      <c r="D152" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
-        <v>461</v>
-      </c>
-      <c r="B153" t="s">
-        <v>456</v>
-      </c>
-      <c r="C153" s="6" t="s">
-        <v>460</v>
-      </c>
-      <c r="D153" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
-        <v>464</v>
-      </c>
-      <c r="B154" t="s">
-        <v>456</v>
-      </c>
-      <c r="C154" s="6" t="s">
-        <v>463</v>
-      </c>
-      <c r="D154" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
-        <v>467</v>
-      </c>
-      <c r="B155" t="s">
-        <v>456</v>
-      </c>
-      <c r="C155" s="6" t="s">
-        <v>466</v>
-      </c>
-      <c r="D155" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" t="s">
-        <v>470</v>
-      </c>
-      <c r="B156" t="s">
-        <v>456</v>
-      </c>
-      <c r="C156" s="6" t="s">
-        <v>469</v>
-      </c>
-      <c r="D156" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157" t="s">
-        <v>473</v>
-      </c>
-      <c r="B157" t="s">
-        <v>475</v>
-      </c>
-      <c r="C157" s="6" t="s">
-        <v>472</v>
-      </c>
-      <c r="D157" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A158" t="s">
-        <v>477</v>
-      </c>
-      <c r="B158" t="s">
-        <v>475</v>
-      </c>
-      <c r="C158" s="6" t="s">
-        <v>476</v>
-      </c>
-      <c r="D158" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" t="s">
-        <v>480</v>
-      </c>
-      <c r="B159" t="s">
-        <v>475</v>
-      </c>
-      <c r="C159" s="6" t="s">
-        <v>479</v>
-      </c>
-      <c r="D159" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" t="s">
-        <v>483</v>
-      </c>
-      <c r="B160" t="s">
-        <v>475</v>
-      </c>
-      <c r="C160" s="6" t="s">
-        <v>482</v>
-      </c>
-      <c r="D160" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A161" t="s">
-        <v>486</v>
-      </c>
-      <c r="B161" t="s">
-        <v>475</v>
-      </c>
-      <c r="C161" s="6" t="s">
-        <v>485</v>
-      </c>
-      <c r="D161" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
-        <v>489</v>
-      </c>
-      <c r="B162" t="s">
-        <v>475</v>
-      </c>
-      <c r="C162" s="6" t="s">
-        <v>488</v>
-      </c>
-      <c r="D162" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
-        <v>492</v>
-      </c>
-      <c r="B163" t="s">
-        <v>475</v>
-      </c>
-      <c r="C163" s="6" t="s">
-        <v>491</v>
-      </c>
-      <c r="D163" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A164" t="s">
-        <v>495</v>
-      </c>
-      <c r="B164" t="s">
-        <v>475</v>
-      </c>
-      <c r="C164" s="6" t="s">
-        <v>494</v>
-      </c>
-      <c r="D164" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A165" t="s">
-        <v>498</v>
-      </c>
-      <c r="B165" t="s">
-        <v>475</v>
-      </c>
-      <c r="C165" s="6" t="s">
-        <v>497</v>
-      </c>
-      <c r="D165" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A166" t="s">
-        <v>501</v>
-      </c>
-      <c r="B166" t="s">
-        <v>475</v>
-      </c>
-      <c r="C166" s="6" t="s">
-        <v>500</v>
-      </c>
-      <c r="D166" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A167" t="s">
-        <v>504</v>
-      </c>
-      <c r="B167" t="s">
-        <v>475</v>
-      </c>
-      <c r="C167" s="6" t="s">
-        <v>503</v>
-      </c>
-      <c r="D167" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A168" t="s">
-        <v>507</v>
-      </c>
-      <c r="B168" t="s">
-        <v>475</v>
-      </c>
-      <c r="C168" s="6" t="s">
-        <v>506</v>
-      </c>
-      <c r="D168" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A169" t="s">
-        <v>510</v>
-      </c>
-      <c r="B169" t="s">
-        <v>475</v>
-      </c>
-      <c r="C169" s="6" t="s">
-        <v>509</v>
-      </c>
-      <c r="D169" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A170" t="s">
-        <v>513</v>
-      </c>
-      <c r="B170" t="s">
-        <v>475</v>
-      </c>
-      <c r="C170" s="6" t="s">
-        <v>512</v>
-      </c>
-      <c r="D170" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A171" t="s">
-        <v>516</v>
-      </c>
-      <c r="B171" t="s">
-        <v>475</v>
-      </c>
-      <c r="C171" s="6" t="s">
-        <v>515</v>
-      </c>
-      <c r="D171" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A172" t="s">
-        <v>519</v>
-      </c>
-      <c r="B172" t="s">
-        <v>475</v>
-      </c>
-      <c r="C172" s="6" t="s">
-        <v>518</v>
-      </c>
-      <c r="D172" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A173" t="s">
-        <v>522</v>
-      </c>
-      <c r="B173" t="s">
-        <v>475</v>
-      </c>
-      <c r="C173" s="6" t="s">
-        <v>521</v>
-      </c>
-      <c r="D173" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A174" t="s">
-        <v>525</v>
-      </c>
-      <c r="B174" t="s">
-        <v>475</v>
-      </c>
-      <c r="C174" s="6" t="s">
-        <v>524</v>
-      </c>
-      <c r="D174" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A175" t="s">
-        <v>528</v>
-      </c>
-      <c r="B175" t="s">
-        <v>475</v>
-      </c>
-      <c r="C175" s="6" t="s">
-        <v>527</v>
-      </c>
-      <c r="D175" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A176" t="s">
-        <v>531</v>
-      </c>
-      <c r="B176" t="s">
-        <v>475</v>
-      </c>
-      <c r="C176" s="6" t="s">
-        <v>530</v>
-      </c>
-      <c r="D176" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A177" t="s">
-        <v>534</v>
-      </c>
-      <c r="B177" t="s">
-        <v>475</v>
-      </c>
-      <c r="C177" s="6" t="s">
-        <v>533</v>
-      </c>
-      <c r="D177" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A178" t="s">
-        <v>537</v>
-      </c>
-      <c r="B178" t="s">
-        <v>475</v>
-      </c>
-      <c r="C178" s="6" t="s">
-        <v>536</v>
-      </c>
-      <c r="D178" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A179" t="s">
-        <v>540</v>
-      </c>
-      <c r="B179" t="s">
-        <v>475</v>
-      </c>
-      <c r="C179" s="6" t="s">
-        <v>539</v>
-      </c>
-      <c r="D179" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A180" t="s">
-        <v>543</v>
-      </c>
-      <c r="B180" t="s">
-        <v>475</v>
-      </c>
-      <c r="C180" s="6" t="s">
-        <v>542</v>
-      </c>
-      <c r="D180" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A181" t="s">
-        <v>546</v>
-      </c>
-      <c r="B181" t="s">
-        <v>475</v>
-      </c>
-      <c r="C181" s="6" t="s">
-        <v>545</v>
-      </c>
-      <c r="D181" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A182" t="s">
-        <v>549</v>
-      </c>
-      <c r="B182" t="s">
-        <v>475</v>
-      </c>
-      <c r="C182" s="6" t="s">
-        <v>548</v>
-      </c>
-      <c r="D182" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A183" t="s">
-        <v>552</v>
-      </c>
-      <c r="B183" t="s">
-        <v>475</v>
-      </c>
-      <c r="C183" s="6" t="s">
-        <v>551</v>
-      </c>
-      <c r="D183" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A184" t="s">
-        <v>555</v>
-      </c>
-      <c r="B184" t="s">
-        <v>475</v>
-      </c>
-      <c r="C184" s="6" t="s">
-        <v>554</v>
-      </c>
-      <c r="D184" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A185" t="s">
-        <v>558</v>
-      </c>
-      <c r="B185" t="s">
-        <v>475</v>
-      </c>
-      <c r="C185" s="6" t="s">
-        <v>557</v>
-      </c>
-      <c r="D185" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A186" t="s">
-        <v>561</v>
-      </c>
-      <c r="B186" t="s">
-        <v>475</v>
-      </c>
-      <c r="C186" s="6" t="s">
-        <v>560</v>
-      </c>
-      <c r="D186" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A187" t="s">
-        <v>564</v>
-      </c>
-      <c r="B187" t="s">
-        <v>475</v>
-      </c>
-      <c r="C187" s="6" t="s">
-        <v>563</v>
-      </c>
-      <c r="D187" t="s">
-        <v>565</v>
-      </c>
-    </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A188" t="s">
-        <v>567</v>
-      </c>
-      <c r="B188" t="s">
-        <v>475</v>
-      </c>
-      <c r="C188" s="6" t="s">
-        <v>566</v>
-      </c>
-      <c r="D188" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A189" t="s">
-        <v>570</v>
-      </c>
-      <c r="B189" t="s">
-        <v>475</v>
-      </c>
-      <c r="C189" s="6" t="s">
-        <v>569</v>
-      </c>
-      <c r="D189" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A190" t="s">
-        <v>573</v>
-      </c>
-      <c r="B190" t="s">
-        <v>475</v>
-      </c>
-      <c r="C190" s="6" t="s">
-        <v>572</v>
-      </c>
-      <c r="D190" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A191" t="s">
-        <v>576</v>
-      </c>
-      <c r="B191" t="s">
-        <v>475</v>
-      </c>
-      <c r="C191" s="6" t="s">
-        <v>575</v>
-      </c>
-      <c r="D191" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A192" t="s">
-        <v>579</v>
-      </c>
-      <c r="B192" t="s">
-        <v>475</v>
-      </c>
-      <c r="C192" s="6" t="s">
-        <v>578</v>
-      </c>
-      <c r="D192" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A193" t="s">
-        <v>582</v>
-      </c>
-      <c r="B193" t="s">
-        <v>475</v>
-      </c>
-      <c r="C193" s="6" t="s">
-        <v>581</v>
-      </c>
-      <c r="D193" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A194" t="s">
-        <v>585</v>
-      </c>
-      <c r="B194" t="s">
-        <v>475</v>
-      </c>
-      <c r="C194" s="6" t="s">
-        <v>584</v>
-      </c>
-      <c r="D194" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A195" t="s">
-        <v>588</v>
-      </c>
-      <c r="B195" t="s">
-        <v>475</v>
-      </c>
-      <c r="C195" s="6" t="s">
-        <v>587</v>
-      </c>
-      <c r="D195" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A196" t="s">
-        <v>591</v>
-      </c>
-      <c r="B196" t="s">
-        <v>475</v>
-      </c>
-      <c r="C196" s="6" t="s">
-        <v>590</v>
-      </c>
-      <c r="D196" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A197" t="s">
-        <v>594</v>
-      </c>
-      <c r="B197" t="s">
-        <v>475</v>
-      </c>
-      <c r="C197" s="6" t="s">
-        <v>593</v>
-      </c>
-      <c r="D197" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A198" t="s">
-        <v>597</v>
-      </c>
-      <c r="B198" t="s">
-        <v>475</v>
-      </c>
-      <c r="C198" s="6" t="s">
-        <v>596</v>
-      </c>
-      <c r="D198" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A199" t="s">
-        <v>600</v>
-      </c>
-      <c r="B199" t="s">
-        <v>475</v>
-      </c>
-      <c r="C199" s="6" t="s">
-        <v>599</v>
-      </c>
-      <c r="D199" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A200" t="s">
-        <v>603</v>
-      </c>
-      <c r="B200" t="s">
-        <v>475</v>
-      </c>
-      <c r="C200" s="6" t="s">
-        <v>602</v>
-      </c>
-      <c r="D200" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A201" t="s">
-        <v>606</v>
-      </c>
-      <c r="B201" t="s">
-        <v>475</v>
-      </c>
-      <c r="C201" s="6" t="s">
-        <v>605</v>
-      </c>
-      <c r="D201" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A202" t="s">
-        <v>609</v>
-      </c>
-      <c r="B202" t="s">
-        <v>475</v>
-      </c>
-      <c r="C202" s="6" t="s">
-        <v>608</v>
-      </c>
-      <c r="D202" t="s">
-        <v>610</v>
-      </c>
-    </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A203" t="s">
-        <v>612</v>
-      </c>
-      <c r="B203" t="s">
-        <v>475</v>
-      </c>
-      <c r="C203" s="6" t="s">
-        <v>611</v>
-      </c>
-      <c r="D203" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A204" t="s">
-        <v>615</v>
-      </c>
-      <c r="B204" t="s">
-        <v>475</v>
-      </c>
-      <c r="C204" s="6" t="s">
-        <v>614</v>
-      </c>
-      <c r="D204" t="s">
-        <v>616</v>
-      </c>
-    </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A205" t="s">
-        <v>618</v>
-      </c>
-      <c r="B205" t="s">
-        <v>475</v>
-      </c>
-      <c r="C205" s="6" t="s">
-        <v>617</v>
-      </c>
-      <c r="D205" t="s">
-        <v>619</v>
-      </c>
-    </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A206" t="s">
-        <v>621</v>
-      </c>
-      <c r="B206" t="s">
-        <v>475</v>
-      </c>
-      <c r="C206" s="6" t="s">
-        <v>620</v>
-      </c>
-      <c r="D206" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A207" t="s">
-        <v>624</v>
-      </c>
-      <c r="B207" t="s">
-        <v>475</v>
-      </c>
-      <c r="C207" s="6" t="s">
-        <v>623</v>
-      </c>
-      <c r="D207" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A208" t="s">
-        <v>627</v>
-      </c>
-      <c r="B208" t="s">
-        <v>475</v>
-      </c>
-      <c r="C208" s="6" t="s">
-        <v>626</v>
-      </c>
-      <c r="D208" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A209" t="s">
-        <v>630</v>
-      </c>
-      <c r="B209" t="s">
-        <v>475</v>
-      </c>
-      <c r="C209" s="6" t="s">
-        <v>629</v>
-      </c>
-      <c r="D209" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A210" t="s">
-        <v>633</v>
-      </c>
-      <c r="B210" t="s">
-        <v>475</v>
-      </c>
-      <c r="C210" s="6" t="s">
-        <v>632</v>
-      </c>
-      <c r="D210" t="s">
-        <v>634</v>
-      </c>
-    </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A211" t="s">
-        <v>636</v>
-      </c>
-      <c r="B211" t="s">
-        <v>475</v>
-      </c>
-      <c r="C211" s="6" t="s">
-        <v>635</v>
-      </c>
-      <c r="D211" t="s">
-        <v>637</v>
-      </c>
-    </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A212" t="s">
-        <v>639</v>
-      </c>
-      <c r="B212" t="s">
-        <v>475</v>
-      </c>
-      <c r="C212" s="6" t="s">
-        <v>638</v>
-      </c>
-      <c r="D212" t="s">
-        <v>640</v>
-      </c>
-    </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A213" t="s">
-        <v>642</v>
-      </c>
-      <c r="B213" t="s">
-        <v>475</v>
-      </c>
-      <c r="C213" s="6" t="s">
-        <v>641</v>
-      </c>
-      <c r="D213" t="s">
-        <v>643</v>
-      </c>
-    </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A214" t="s">
-        <v>645</v>
-      </c>
-      <c r="B214" t="s">
-        <v>475</v>
-      </c>
-      <c r="C214" s="6" t="s">
-        <v>644</v>
-      </c>
-      <c r="D214" t="s">
-        <v>646</v>
-      </c>
-    </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A215" t="s">
-        <v>648</v>
-      </c>
-      <c r="B215" t="s">
-        <v>475</v>
-      </c>
-      <c r="C215" s="6" t="s">
-        <v>647</v>
-      </c>
-      <c r="D215" t="s">
-        <v>649</v>
-      </c>
-    </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A216" t="s">
-        <v>651</v>
-      </c>
-      <c r="B216" t="s">
-        <v>475</v>
-      </c>
-      <c r="C216" s="6" t="s">
-        <v>650</v>
-      </c>
-      <c r="D216" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A217" t="s">
-        <v>654</v>
-      </c>
-      <c r="B217" t="s">
-        <v>475</v>
-      </c>
-      <c r="C217" s="6" t="s">
-        <v>653</v>
-      </c>
-      <c r="D217" t="s">
-        <v>655</v>
-      </c>
-    </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A218" t="s">
-        <v>657</v>
-      </c>
-      <c r="B218" t="s">
-        <v>475</v>
-      </c>
-      <c r="C218" s="6" t="s">
-        <v>656</v>
-      </c>
-      <c r="D218" t="s">
-        <v>658</v>
-      </c>
-    </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A219" t="s">
-        <v>660</v>
-      </c>
-      <c r="B219" t="s">
-        <v>475</v>
-      </c>
-      <c r="C219" s="6" t="s">
-        <v>659</v>
-      </c>
-      <c r="D219" t="s">
-        <v>661</v>
-      </c>
-    </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A220" t="s">
-        <v>663</v>
-      </c>
-      <c r="B220" t="s">
-        <v>475</v>
-      </c>
-      <c r="C220" s="6" t="s">
-        <v>662</v>
-      </c>
-      <c r="D220" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A221" t="s">
-        <v>666</v>
-      </c>
-      <c r="B221" t="s">
-        <v>475</v>
-      </c>
-      <c r="C221" s="6" t="s">
-        <v>665</v>
-      </c>
-      <c r="D221" t="s">
-        <v>667</v>
-      </c>
-    </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A222" t="s">
-        <v>669</v>
-      </c>
-      <c r="B222" t="s">
-        <v>475</v>
-      </c>
-      <c r="C222" s="6" t="s">
-        <v>668</v>
-      </c>
-      <c r="D222" t="s">
-        <v>670</v>
-      </c>
-    </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A223" t="s">
-        <v>672</v>
-      </c>
-      <c r="B223" t="s">
-        <v>475</v>
-      </c>
-      <c r="C223" s="6" t="s">
-        <v>671</v>
-      </c>
-      <c r="D223" t="s">
-        <v>673</v>
-      </c>
-    </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A224" t="s">
-        <v>675</v>
-      </c>
-      <c r="B224" t="s">
-        <v>475</v>
-      </c>
-      <c r="C224" s="6" t="s">
-        <v>674</v>
-      </c>
-      <c r="D224" t="s">
-        <v>676</v>
-      </c>
-    </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A225" t="s">
-        <v>678</v>
-      </c>
-      <c r="B225" t="s">
-        <v>475</v>
-      </c>
-      <c r="C225" s="6" t="s">
-        <v>677</v>
-      </c>
-      <c r="D225" t="s">
-        <v>679</v>
-      </c>
-    </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A226" t="s">
-        <v>681</v>
-      </c>
-      <c r="B226" t="s">
-        <v>475</v>
-      </c>
-      <c r="C226" s="6" t="s">
-        <v>680</v>
-      </c>
-      <c r="D226" t="s">
-        <v>682</v>
-      </c>
-    </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A227" t="s">
-        <v>684</v>
-      </c>
-      <c r="B227" t="s">
-        <v>475</v>
-      </c>
-      <c r="C227" s="6" t="s">
-        <v>683</v>
-      </c>
-      <c r="D227" t="s">
-        <v>685</v>
-      </c>
-    </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A228" t="s">
-        <v>687</v>
-      </c>
-      <c r="B228" t="s">
-        <v>475</v>
-      </c>
-      <c r="C228" s="6" t="s">
-        <v>686</v>
-      </c>
-      <c r="D228" t="s">
-        <v>688</v>
-      </c>
-    </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A229" t="s">
-        <v>690</v>
-      </c>
-      <c r="B229" t="s">
-        <v>475</v>
-      </c>
-      <c r="C229" s="6" t="s">
-        <v>689</v>
-      </c>
-      <c r="D229" t="s">
-        <v>691</v>
-      </c>
-    </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A230" t="s">
-        <v>693</v>
-      </c>
-      <c r="B230" t="s">
-        <v>475</v>
-      </c>
-      <c r="C230" s="6" t="s">
-        <v>692</v>
-      </c>
-      <c r="D230" t="s">
-        <v>694</v>
-      </c>
-    </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A231" t="s">
-        <v>696</v>
-      </c>
-      <c r="B231" t="s">
-        <v>475</v>
-      </c>
-      <c r="C231" s="6" t="s">
-        <v>695</v>
-      </c>
-      <c r="D231" t="s">
-        <v>697</v>
-      </c>
-    </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A232" t="s">
-        <v>699</v>
-      </c>
-      <c r="B232" t="s">
-        <v>475</v>
-      </c>
-      <c r="C232" s="6" t="s">
-        <v>698</v>
-      </c>
-      <c r="D232" t="s">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A233" t="s">
-        <v>702</v>
-      </c>
-      <c r="B233" t="s">
-        <v>475</v>
-      </c>
-      <c r="C233" s="6" t="s">
-        <v>701</v>
-      </c>
-      <c r="D233" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A234" t="s">
-        <v>705</v>
-      </c>
-      <c r="B234" t="s">
-        <v>475</v>
-      </c>
-      <c r="C234" s="6" t="s">
-        <v>704</v>
-      </c>
-      <c r="D234" t="s">
-        <v>706</v>
-      </c>
-    </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A235" t="s">
-        <v>708</v>
-      </c>
-      <c r="B235" t="s">
-        <v>710</v>
-      </c>
-      <c r="C235" s="6" t="s">
-        <v>707</v>
-      </c>
-      <c r="D235" t="s">
-        <v>709</v>
-      </c>
-    </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A236" t="s">
-        <v>712</v>
-      </c>
-      <c r="B236" t="s">
-        <v>710</v>
-      </c>
-      <c r="C236" s="6" t="s">
-        <v>711</v>
-      </c>
-      <c r="D236" t="s">
-        <v>713</v>
-      </c>
-    </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A237" t="s">
-        <v>715</v>
-      </c>
-      <c r="B237" t="s">
-        <v>710</v>
-      </c>
-      <c r="C237" s="6" t="s">
-        <v>714</v>
-      </c>
-      <c r="D237" t="s">
-        <v>716</v>
-      </c>
-    </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A238" t="s">
-        <v>718</v>
-      </c>
-      <c r="B238" t="s">
-        <v>710</v>
-      </c>
-      <c r="C238" s="6" t="s">
-        <v>717</v>
-      </c>
-      <c r="D238" t="s">
-        <v>719</v>
-      </c>
-    </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A239" t="s">
-        <v>721</v>
-      </c>
-      <c r="B239" t="s">
-        <v>710</v>
-      </c>
-      <c r="C239" s="6" t="s">
-        <v>720</v>
-      </c>
-      <c r="D239" t="s">
-        <v>722</v>
-      </c>
-    </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A240" t="s">
-        <v>724</v>
-      </c>
-      <c r="B240" t="s">
-        <v>710</v>
-      </c>
-      <c r="C240" s="6" t="s">
-        <v>723</v>
-      </c>
-      <c r="D240" t="s">
-        <v>725</v>
-      </c>
-    </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A241" t="s">
-        <v>727</v>
-      </c>
-      <c r="B241" t="s">
-        <v>710</v>
-      </c>
-      <c r="C241" s="6" t="s">
-        <v>726</v>
-      </c>
-      <c r="D241" t="s">
         <v>728</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{C3F428D8-A9C2-4BF8-A9CC-19C2B03DF618}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3E8C717-E709-40B0-9721-8894CB329007}">
+  <dimension ref="A1:E30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1063</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1064</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B2">
+        <v>49001</v>
+      </c>
+      <c r="C2" t="s">
+        <v>391</v>
+      </c>
+      <c r="D2">
+        <v>46</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1068</v>
+      </c>
+      <c r="B3">
+        <v>49003</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1069</v>
+      </c>
+      <c r="D3">
+        <v>46</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1071</v>
+      </c>
+      <c r="B4">
+        <v>49013</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1072</v>
+      </c>
+      <c r="D4">
+        <v>46</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1074</v>
+      </c>
+      <c r="B5">
+        <v>49015</v>
+      </c>
+      <c r="C5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5">
+        <v>46</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B6">
+        <v>49019</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D6">
+        <v>46</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1079</v>
+      </c>
+      <c r="B7">
+        <v>49025</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1080</v>
+      </c>
+      <c r="D7">
+        <v>46</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1082</v>
+      </c>
+      <c r="B8">
+        <v>49045</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1083</v>
+      </c>
+      <c r="D8">
+        <v>46</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1084</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1085</v>
+      </c>
+      <c r="B9">
+        <v>49029</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <v>46</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1086</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1087</v>
+      </c>
+      <c r="B10">
+        <v>49035</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1088</v>
+      </c>
+      <c r="D10">
+        <v>46</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1090</v>
+      </c>
+      <c r="B11">
+        <v>49043</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D11">
+        <v>46</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1092</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1093</v>
+      </c>
+      <c r="B12">
+        <v>49047</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1094</v>
+      </c>
+      <c r="D12">
+        <v>46</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1096</v>
+      </c>
+      <c r="B13">
+        <v>49057</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1097</v>
+      </c>
+      <c r="D13">
+        <v>46</v>
+      </c>
+      <c r="E13" t="s">
+        <v>1098</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1099</v>
+      </c>
+      <c r="B14">
+        <v>49005</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1100</v>
+      </c>
+      <c r="D14">
+        <v>46</v>
+      </c>
+      <c r="E14" t="s">
+        <v>1101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1102</v>
+      </c>
+      <c r="B15">
+        <v>49017</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1103</v>
+      </c>
+      <c r="D15">
+        <v>46</v>
+      </c>
+      <c r="E15" t="s">
+        <v>1104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>1105</v>
+      </c>
+      <c r="B16">
+        <v>49033</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1106</v>
+      </c>
+      <c r="D16">
+        <v>46</v>
+      </c>
+      <c r="E16" t="s">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>1108</v>
+      </c>
+      <c r="B17">
+        <v>49023</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1109</v>
+      </c>
+      <c r="D17">
+        <v>46</v>
+      </c>
+      <c r="E17" t="s">
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>1111</v>
+      </c>
+      <c r="B18">
+        <v>49049</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1061</v>
+      </c>
+      <c r="D18">
+        <v>46</v>
+      </c>
+      <c r="E18" t="s">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>1113</v>
+      </c>
+      <c r="B19">
+        <v>49007</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1114</v>
+      </c>
+      <c r="D19">
+        <v>46</v>
+      </c>
+      <c r="E19" t="s">
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>1116</v>
+      </c>
+      <c r="B20">
+        <v>49009</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1117</v>
+      </c>
+      <c r="D20">
+        <v>46</v>
+      </c>
+      <c r="E20" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>1119</v>
+      </c>
+      <c r="B21">
+        <v>49021</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1120</v>
+      </c>
+      <c r="D21">
+        <v>46</v>
+      </c>
+      <c r="E21" t="s">
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>1122</v>
+      </c>
+      <c r="B22">
+        <v>49051</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1123</v>
+      </c>
+      <c r="D22">
+        <v>46</v>
+      </c>
+      <c r="E22" t="s">
+        <v>1124</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>1125</v>
+      </c>
+      <c r="B23">
+        <v>49055</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1126</v>
+      </c>
+      <c r="D23">
+        <v>46</v>
+      </c>
+      <c r="E23" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>1128</v>
+      </c>
+      <c r="B24">
+        <v>49027</v>
+      </c>
+      <c r="C24" t="s">
+        <v>1129</v>
+      </c>
+      <c r="D24">
+        <v>46</v>
+      </c>
+      <c r="E24" t="s">
+        <v>1130</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>1131</v>
+      </c>
+      <c r="B25">
+        <v>49039</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1132</v>
+      </c>
+      <c r="D25">
+        <v>46</v>
+      </c>
+      <c r="E25" t="s">
+        <v>1133</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>1134</v>
+      </c>
+      <c r="B26">
+        <v>49053</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1135</v>
+      </c>
+      <c r="D26">
+        <v>46</v>
+      </c>
+      <c r="E26" t="s">
+        <v>1136</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>1137</v>
+      </c>
+      <c r="B27">
+        <v>49037</v>
+      </c>
+      <c r="C27" t="s">
+        <v>1138</v>
+      </c>
+      <c r="D27">
+        <v>46</v>
+      </c>
+      <c r="E27" t="s">
+        <v>1139</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>1140</v>
+      </c>
+      <c r="B28">
+        <v>49041</v>
+      </c>
+      <c r="C28" t="s">
+        <v>1141</v>
+      </c>
+      <c r="D28">
+        <v>46</v>
+      </c>
+      <c r="E28" t="s">
+        <v>1142</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>1143</v>
+      </c>
+      <c r="B29">
+        <v>49011</v>
+      </c>
+      <c r="C29" t="s">
+        <v>1144</v>
+      </c>
+      <c r="D29">
+        <v>46</v>
+      </c>
+      <c r="E29" t="s">
+        <v>1145</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>1146</v>
+      </c>
+      <c r="B30">
+        <v>49031</v>
+      </c>
+      <c r="C30" t="s">
+        <v>356</v>
+      </c>
+      <c r="D30">
+        <v>46</v>
+      </c>
+      <c r="E30" t="s">
+        <v>1147</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5B926E0-2923-41A9-80D2-D9F61E4F03DD}">
   <dimension ref="A1:D241"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
-    </sheetView>
+    <sheetView topLeftCell="A130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.42578125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="67.140625" style="6" customWidth="1"/>
     <col min="2" max="5" width="24" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>